<commit_message>
FEAT: moved unset! colums/rows closer to logic! in conversion matrices.
</commit_message>
<xml_diff>
--- a/docs/conversion-matrix.xlsx
+++ b/docs/conversion-matrix.xlsx
@@ -50,7 +50,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L4" authorId="0">
+    <comment ref="M4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -212,7 +212,7 @@
     <author>dk</author>
   </authors>
   <commentList>
-    <comment ref="L4" authorId="0">
+    <comment ref="M4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -447,7 +447,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L4" authorId="0">
+    <comment ref="M4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -584,7 +584,7 @@
     <author>dk</author>
   </authors>
   <commentList>
-    <comment ref="L4" authorId="0">
+    <comment ref="M4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2129,7 +2129,7 @@
     <a:spDef>
       <a:spPr>
         <a:blipFill rotWithShape="1">
-          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
           <a:srcRect/>
           <a:tile tx="0" ty="0" sx="100000" sy="100000" flip="none" algn="tl"/>
         </a:blipFill>
@@ -3026,8 +3026,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:Y23"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q12" sqref="Q12"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3068,16 +3068,16 @@
         <v>31</v>
       </c>
       <c r="J3" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="K3" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="K3" s="20" t="s">
+      <c r="L3" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="L3" s="20" t="s">
+      <c r="M3" s="20" t="s">
         <v>6</v>
-      </c>
-      <c r="M3" s="20" t="s">
-        <v>53</v>
       </c>
       <c r="N3" s="20" t="s">
         <v>7</v>
@@ -3128,13 +3128,13 @@
       <c r="I4" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="J4" s="25"/>
+      <c r="J4" s="23" t="s">
+        <v>121</v>
+      </c>
       <c r="K4" s="25"/>
-      <c r="L4" s="23" t="s">
+      <c r="L4" s="25"/>
+      <c r="M4" s="23" t="s">
         <v>239</v>
-      </c>
-      <c r="M4" s="23" t="s">
-        <v>121</v>
       </c>
       <c r="N4" s="23" t="s">
         <v>178</v>
@@ -3179,12 +3179,12 @@
       <c r="I5" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="J5" s="25"/>
+      <c r="J5" s="23" t="s">
+        <v>121</v>
+      </c>
       <c r="K5" s="25"/>
       <c r="L5" s="25"/>
-      <c r="M5" s="23" t="s">
-        <v>121</v>
-      </c>
+      <c r="M5" s="25"/>
       <c r="N5" s="23" t="s">
         <v>177</v>
       </c>
@@ -3226,12 +3226,12 @@
       <c r="I6" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="J6" s="25"/>
+      <c r="J6" s="23" t="s">
+        <v>121</v>
+      </c>
       <c r="K6" s="25"/>
       <c r="L6" s="25"/>
-      <c r="M6" s="23" t="s">
-        <v>121</v>
-      </c>
+      <c r="M6" s="25"/>
       <c r="N6" s="25"/>
       <c r="O6" s="25"/>
       <c r="P6" s="23" t="s">
@@ -3267,13 +3267,13 @@
       <c r="I7" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="J7" s="25"/>
+      <c r="J7" s="23" t="s">
+        <v>121</v>
+      </c>
       <c r="K7" s="25"/>
-      <c r="L7" s="23" t="s">
+      <c r="L7" s="25"/>
+      <c r="M7" s="23" t="s">
         <v>118</v>
-      </c>
-      <c r="M7" s="23" t="s">
-        <v>121</v>
       </c>
       <c r="N7" s="23" t="s">
         <v>122</v>
@@ -3310,12 +3310,12 @@
       <c r="I8" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="J8" s="25"/>
+      <c r="J8" s="23" t="s">
+        <v>121</v>
+      </c>
       <c r="K8" s="25"/>
       <c r="L8" s="25"/>
-      <c r="M8" s="23" t="s">
-        <v>121</v>
-      </c>
+      <c r="M8" s="25"/>
       <c r="N8" s="23" t="s">
         <v>123</v>
       </c>
@@ -3347,12 +3347,12 @@
       <c r="I9" s="23" t="b">
         <v>0</v>
       </c>
-      <c r="J9" s="25"/>
+      <c r="J9" s="23" t="s">
+        <v>121</v>
+      </c>
       <c r="K9" s="25"/>
       <c r="L9" s="25"/>
-      <c r="M9" s="23" t="s">
-        <v>121</v>
-      </c>
+      <c r="M9" s="25"/>
       <c r="N9" s="25"/>
       <c r="O9" s="25"/>
       <c r="P9" s="25"/>
@@ -3380,12 +3380,12 @@
         <v>116</v>
       </c>
       <c r="I10" s="22"/>
-      <c r="J10" s="25"/>
+      <c r="J10" s="23" t="s">
+        <v>121</v>
+      </c>
       <c r="K10" s="25"/>
       <c r="L10" s="25"/>
-      <c r="M10" s="23" t="s">
-        <v>121</v>
-      </c>
+      <c r="M10" s="25"/>
       <c r="N10" s="25"/>
       <c r="O10" s="23" t="s">
         <v>127</v>
@@ -3406,7 +3406,7 @@
     </row>
     <row r="11" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="19" t="s">
-        <v>12</v>
+        <v>53</v>
       </c>
       <c r="C11" s="25"/>
       <c r="D11" s="25"/>
@@ -3419,24 +3419,20 @@
       <c r="I11" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="J11" s="25"/>
+      <c r="J11" s="22"/>
       <c r="K11" s="25"/>
       <c r="L11" s="25"/>
-      <c r="M11" s="23" t="s">
-        <v>121</v>
-      </c>
+      <c r="M11" s="25"/>
       <c r="N11" s="25"/>
-      <c r="O11" s="23" t="s">
-        <v>111</v>
-      </c>
+      <c r="O11" s="25"/>
       <c r="P11" s="23" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="Q11" s="23" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="R11" s="23" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="S11" s="25"/>
       <c r="T11" s="25"/>
@@ -3445,7 +3441,7 @@
     </row>
     <row r="12" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="19" t="s">
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="C12" s="25"/>
       <c r="D12" s="25"/>
@@ -3458,22 +3454,24 @@
       <c r="I12" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="J12" s="25"/>
-      <c r="K12" s="22"/>
+      <c r="J12" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="K12" s="25"/>
       <c r="L12" s="25"/>
-      <c r="M12" s="23" t="s">
-        <v>121</v>
-      </c>
+      <c r="M12" s="25"/>
       <c r="N12" s="25"/>
-      <c r="O12" s="25"/>
+      <c r="O12" s="23" t="s">
+        <v>111</v>
+      </c>
       <c r="P12" s="23" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="Q12" s="23" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="R12" s="23" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="S12" s="25"/>
       <c r="T12" s="25"/>
@@ -3482,7 +3480,7 @@
     </row>
     <row r="13" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="19" t="s">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="C13" s="25"/>
       <c r="D13" s="25"/>
@@ -3495,24 +3493,22 @@
       <c r="I13" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="J13" s="25"/>
+      <c r="J13" s="23" t="s">
+        <v>121</v>
+      </c>
       <c r="K13" s="25"/>
-      <c r="L13" s="25"/>
-      <c r="M13" s="23" t="s">
-        <v>121</v>
-      </c>
-      <c r="N13" s="23" t="s">
-        <v>111</v>
-      </c>
+      <c r="L13" s="22"/>
+      <c r="M13" s="25"/>
+      <c r="N13" s="25"/>
       <c r="O13" s="25"/>
       <c r="P13" s="23" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="Q13" s="23" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="R13" s="23" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="S13" s="25"/>
       <c r="T13" s="25"/>
@@ -3521,7 +3517,7 @@
     </row>
     <row r="14" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="19" t="s">
-        <v>53</v>
+        <v>6</v>
       </c>
       <c r="C14" s="25"/>
       <c r="D14" s="25"/>
@@ -3534,20 +3530,24 @@
       <c r="I14" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="J14" s="25"/>
+      <c r="J14" s="23" t="s">
+        <v>121</v>
+      </c>
       <c r="K14" s="25"/>
       <c r="L14" s="25"/>
-      <c r="M14" s="22"/>
-      <c r="N14" s="25"/>
+      <c r="M14" s="25"/>
+      <c r="N14" s="23" t="s">
+        <v>111</v>
+      </c>
       <c r="O14" s="25"/>
       <c r="P14" s="23" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="Q14" s="23" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="R14" s="23" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="S14" s="25"/>
       <c r="T14" s="25"/>
@@ -3577,13 +3577,13 @@
       <c r="I15" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="J15" s="25"/>
+      <c r="J15" s="23" t="s">
+        <v>121</v>
+      </c>
       <c r="K15" s="25"/>
-      <c r="L15" s="24" t="s">
+      <c r="L15" s="25"/>
+      <c r="M15" s="24" t="s">
         <v>168</v>
-      </c>
-      <c r="M15" s="23" t="s">
-        <v>121</v>
       </c>
       <c r="N15" s="22" t="s">
         <v>208</v>
@@ -3618,12 +3618,12 @@
       <c r="I16" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="J16" s="25"/>
+      <c r="J16" s="23" t="s">
+        <v>121</v>
+      </c>
       <c r="K16" s="25"/>
       <c r="L16" s="25"/>
-      <c r="M16" s="23" t="s">
-        <v>121</v>
-      </c>
+      <c r="M16" s="25"/>
       <c r="N16" s="25"/>
       <c r="O16" s="22"/>
       <c r="P16" s="23" t="s">
@@ -3665,13 +3665,13 @@
       <c r="I17" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="J17" s="25"/>
+      <c r="J17" s="23" t="s">
+        <v>121</v>
+      </c>
       <c r="K17" s="25"/>
-      <c r="L17" s="23" t="s">
+      <c r="L17" s="25"/>
+      <c r="M17" s="23" t="s">
         <v>119</v>
-      </c>
-      <c r="M17" s="23" t="s">
-        <v>121</v>
       </c>
       <c r="N17" s="23" t="s">
         <v>124</v>
@@ -3710,15 +3710,15 @@
       <c r="I18" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="J18" s="25"/>
-      <c r="K18" s="23" t="s">
+      <c r="J18" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="K18" s="25"/>
+      <c r="L18" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="L18" s="23" t="s">
+      <c r="M18" s="23" t="s">
         <v>120</v>
-      </c>
-      <c r="M18" s="23" t="s">
-        <v>121</v>
       </c>
       <c r="N18" s="23" t="s">
         <v>125</v>
@@ -3755,12 +3755,12 @@
       <c r="I19" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="J19" s="25"/>
+      <c r="J19" s="23" t="s">
+        <v>121</v>
+      </c>
       <c r="K19" s="25"/>
       <c r="L19" s="25"/>
-      <c r="M19" s="23" t="s">
-        <v>121</v>
-      </c>
+      <c r="M19" s="25"/>
       <c r="N19" s="25"/>
       <c r="O19" s="25"/>
       <c r="P19" s="23" t="s">
@@ -3792,12 +3792,12 @@
       <c r="I20" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="J20" s="25"/>
+      <c r="J20" s="23" t="s">
+        <v>121</v>
+      </c>
       <c r="K20" s="25"/>
       <c r="L20" s="25"/>
-      <c r="M20" s="23" t="s">
-        <v>121</v>
-      </c>
+      <c r="M20" s="25"/>
       <c r="N20" s="25"/>
       <c r="O20" s="25"/>
       <c r="P20" s="23" t="s">
@@ -3829,12 +3829,12 @@
       <c r="I21" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="J21" s="25"/>
+      <c r="J21" s="23" t="s">
+        <v>121</v>
+      </c>
       <c r="K21" s="25"/>
       <c r="L21" s="25"/>
-      <c r="M21" s="23" t="s">
-        <v>121</v>
-      </c>
+      <c r="M21" s="25"/>
       <c r="N21" s="25"/>
       <c r="O21" s="25"/>
       <c r="P21" s="23" t="s">
@@ -3866,12 +3866,12 @@
       <c r="I22" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="J22" s="25"/>
+      <c r="J22" s="23" t="s">
+        <v>121</v>
+      </c>
       <c r="K22" s="25"/>
       <c r="L22" s="25"/>
-      <c r="M22" s="23" t="s">
-        <v>121</v>
-      </c>
+      <c r="M22" s="25"/>
       <c r="N22" s="25"/>
       <c r="O22" s="25"/>
       <c r="P22" s="23" t="s">
@@ -3905,12 +3905,12 @@
       <c r="I23" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="J23" s="25"/>
+      <c r="J23" s="23" t="s">
+        <v>121</v>
+      </c>
       <c r="K23" s="25"/>
       <c r="L23" s="25"/>
-      <c r="M23" s="23" t="s">
-        <v>121</v>
-      </c>
+      <c r="M23" s="25"/>
       <c r="N23" s="25"/>
       <c r="O23" s="25"/>
       <c r="P23" s="23" t="s">
@@ -3939,7 +3939,7 @@
   <dimension ref="B3:Y23"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3980,16 +3980,16 @@
         <v>31</v>
       </c>
       <c r="J3" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="K3" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="K3" s="20" t="s">
+      <c r="L3" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="L3" s="20" t="s">
+      <c r="M3" s="20" t="s">
         <v>6</v>
-      </c>
-      <c r="M3" s="20" t="s">
-        <v>53</v>
       </c>
       <c r="N3" s="20" t="s">
         <v>7</v>
@@ -4040,13 +4040,13 @@
       <c r="I4" s="28" t="s">
         <v>204</v>
       </c>
-      <c r="J4" s="25"/>
+      <c r="J4" s="23" t="s">
+        <v>121</v>
+      </c>
       <c r="K4" s="25"/>
-      <c r="L4" s="23" t="s">
+      <c r="L4" s="25"/>
+      <c r="M4" s="23" t="s">
         <v>239</v>
-      </c>
-      <c r="M4" s="23" t="s">
-        <v>121</v>
       </c>
       <c r="N4" s="28" t="s">
         <v>193</v>
@@ -4095,12 +4095,12 @@
       <c r="I5" s="28" t="s">
         <v>205</v>
       </c>
-      <c r="J5" s="25"/>
+      <c r="J5" s="23" t="s">
+        <v>121</v>
+      </c>
       <c r="K5" s="25"/>
       <c r="L5" s="25"/>
-      <c r="M5" s="23" t="s">
-        <v>121</v>
-      </c>
+      <c r="M5" s="25"/>
       <c r="N5" s="28" t="s">
         <v>194</v>
       </c>
@@ -4146,12 +4146,12 @@
       <c r="I6" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="J6" s="25"/>
+      <c r="J6" s="23" t="s">
+        <v>121</v>
+      </c>
       <c r="K6" s="25"/>
       <c r="L6" s="25"/>
-      <c r="M6" s="23" t="s">
-        <v>121</v>
-      </c>
+      <c r="M6" s="25"/>
       <c r="N6" s="25"/>
       <c r="O6" s="25"/>
       <c r="P6" s="23" t="s">
@@ -4187,13 +4187,13 @@
       <c r="I7" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="J7" s="25"/>
+      <c r="J7" s="23" t="s">
+        <v>121</v>
+      </c>
       <c r="K7" s="25"/>
-      <c r="L7" s="23" t="s">
+      <c r="L7" s="25"/>
+      <c r="M7" s="23" t="s">
         <v>118</v>
-      </c>
-      <c r="M7" s="23" t="s">
-        <v>121</v>
       </c>
       <c r="N7" s="23" t="s">
         <v>122</v>
@@ -4226,12 +4226,12 @@
       <c r="I8" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="J8" s="25"/>
+      <c r="J8" s="23" t="s">
+        <v>121</v>
+      </c>
       <c r="K8" s="25"/>
       <c r="L8" s="25"/>
-      <c r="M8" s="23" t="s">
-        <v>121</v>
-      </c>
+      <c r="M8" s="25"/>
       <c r="N8" s="23" t="s">
         <v>123</v>
       </c>
@@ -4259,12 +4259,12 @@
       <c r="I9" s="23" t="b">
         <v>0</v>
       </c>
-      <c r="J9" s="25"/>
+      <c r="J9" s="23" t="s">
+        <v>121</v>
+      </c>
       <c r="K9" s="25"/>
       <c r="L9" s="25"/>
-      <c r="M9" s="23" t="s">
-        <v>121</v>
-      </c>
+      <c r="M9" s="25"/>
       <c r="N9" s="25"/>
       <c r="O9" s="25"/>
       <c r="P9" s="25"/>
@@ -4290,12 +4290,12 @@
         <v>116</v>
       </c>
       <c r="I10" s="22"/>
-      <c r="J10" s="25"/>
+      <c r="J10" s="23" t="s">
+        <v>121</v>
+      </c>
       <c r="K10" s="25"/>
       <c r="L10" s="25"/>
-      <c r="M10" s="23" t="s">
-        <v>121</v>
-      </c>
+      <c r="M10" s="25"/>
       <c r="N10" s="25"/>
       <c r="O10" s="23" t="s">
         <v>127</v>
@@ -4312,7 +4312,7 @@
     </row>
     <row r="11" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="19" t="s">
-        <v>12</v>
+        <v>53</v>
       </c>
       <c r="C11" s="25"/>
       <c r="D11" s="25"/>
@@ -4325,18 +4325,14 @@
       <c r="I11" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="J11" s="25"/>
+      <c r="J11" s="22"/>
       <c r="K11" s="25"/>
       <c r="L11" s="25"/>
-      <c r="M11" s="23" t="s">
-        <v>121</v>
-      </c>
+      <c r="M11" s="25"/>
       <c r="N11" s="25"/>
-      <c r="O11" s="23" t="s">
-        <v>111</v>
-      </c>
+      <c r="O11" s="25"/>
       <c r="P11" s="23" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="Q11" s="28"/>
       <c r="R11" s="28"/>
@@ -4347,7 +4343,7 @@
     </row>
     <row r="12" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="19" t="s">
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="C12" s="25"/>
       <c r="D12" s="25"/>
@@ -4360,16 +4356,18 @@
       <c r="I12" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="J12" s="25"/>
-      <c r="K12" s="22"/>
+      <c r="J12" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="K12" s="25"/>
       <c r="L12" s="25"/>
-      <c r="M12" s="23" t="s">
-        <v>121</v>
-      </c>
+      <c r="M12" s="25"/>
       <c r="N12" s="25"/>
-      <c r="O12" s="25"/>
+      <c r="O12" s="23" t="s">
+        <v>111</v>
+      </c>
       <c r="P12" s="23" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="Q12" s="28"/>
       <c r="R12" s="28"/>
@@ -4380,7 +4378,7 @@
     </row>
     <row r="13" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="19" t="s">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="C13" s="25"/>
       <c r="D13" s="25"/>
@@ -4393,18 +4391,16 @@
       <c r="I13" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="J13" s="25"/>
+      <c r="J13" s="23" t="s">
+        <v>121</v>
+      </c>
       <c r="K13" s="25"/>
-      <c r="L13" s="25"/>
-      <c r="M13" s="23" t="s">
-        <v>121</v>
-      </c>
-      <c r="N13" s="23" t="s">
-        <v>111</v>
-      </c>
+      <c r="L13" s="22"/>
+      <c r="M13" s="25"/>
+      <c r="N13" s="25"/>
       <c r="O13" s="25"/>
       <c r="P13" s="23" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="Q13" s="28"/>
       <c r="R13" s="28"/>
@@ -4415,7 +4411,7 @@
     </row>
     <row r="14" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="19" t="s">
-        <v>53</v>
+        <v>6</v>
       </c>
       <c r="C14" s="25"/>
       <c r="D14" s="25"/>
@@ -4428,14 +4424,18 @@
       <c r="I14" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="J14" s="25"/>
+      <c r="J14" s="23" t="s">
+        <v>121</v>
+      </c>
       <c r="K14" s="25"/>
       <c r="L14" s="25"/>
-      <c r="M14" s="22"/>
-      <c r="N14" s="25"/>
+      <c r="M14" s="25"/>
+      <c r="N14" s="23" t="s">
+        <v>111</v>
+      </c>
       <c r="O14" s="25"/>
       <c r="P14" s="23" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="Q14" s="28"/>
       <c r="R14" s="28"/>
@@ -4467,13 +4467,13 @@
       <c r="I15" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="J15" s="25"/>
+      <c r="J15" s="23" t="s">
+        <v>121</v>
+      </c>
       <c r="K15" s="25"/>
-      <c r="L15" s="24" t="s">
+      <c r="L15" s="25"/>
+      <c r="M15" s="24" t="s">
         <v>168</v>
-      </c>
-      <c r="M15" s="23" t="s">
-        <v>121</v>
       </c>
       <c r="N15" s="22"/>
       <c r="O15" s="25"/>
@@ -4506,12 +4506,12 @@
       <c r="I16" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="J16" s="25"/>
+      <c r="J16" s="23" t="s">
+        <v>121</v>
+      </c>
       <c r="K16" s="25"/>
       <c r="L16" s="25"/>
-      <c r="M16" s="23" t="s">
-        <v>121</v>
-      </c>
+      <c r="M16" s="25"/>
       <c r="N16" s="25"/>
       <c r="O16" s="22"/>
       <c r="P16" s="23" t="s">
@@ -4549,13 +4549,13 @@
       <c r="I17" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="J17" s="25"/>
+      <c r="J17" s="23" t="s">
+        <v>121</v>
+      </c>
       <c r="K17" s="25"/>
-      <c r="L17" s="23" t="s">
+      <c r="L17" s="25"/>
+      <c r="M17" s="23" t="s">
         <v>119</v>
-      </c>
-      <c r="M17" s="23" t="s">
-        <v>121</v>
       </c>
       <c r="N17" s="23" t="s">
         <v>124</v>
@@ -4592,15 +4592,15 @@
       <c r="I18" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="J18" s="25"/>
-      <c r="K18" s="23" t="s">
+      <c r="J18" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="K18" s="25"/>
+      <c r="L18" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="L18" s="23" t="s">
+      <c r="M18" s="23" t="s">
         <v>120</v>
-      </c>
-      <c r="M18" s="23" t="s">
-        <v>121</v>
       </c>
       <c r="N18" s="23" t="s">
         <v>125</v>
@@ -4637,12 +4637,12 @@
       <c r="I19" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="J19" s="25"/>
+      <c r="J19" s="23" t="s">
+        <v>121</v>
+      </c>
       <c r="K19" s="25"/>
       <c r="L19" s="25"/>
-      <c r="M19" s="23" t="s">
-        <v>121</v>
-      </c>
+      <c r="M19" s="25"/>
       <c r="N19" s="25"/>
       <c r="O19" s="25"/>
       <c r="P19" s="23" t="s">
@@ -4672,12 +4672,12 @@
       <c r="I20" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="J20" s="25"/>
+      <c r="J20" s="23" t="s">
+        <v>121</v>
+      </c>
       <c r="K20" s="25"/>
       <c r="L20" s="25"/>
-      <c r="M20" s="23" t="s">
-        <v>121</v>
-      </c>
+      <c r="M20" s="25"/>
       <c r="N20" s="25"/>
       <c r="O20" s="25"/>
       <c r="P20" s="23" t="s">
@@ -4705,12 +4705,12 @@
       <c r="I21" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="J21" s="25"/>
+      <c r="J21" s="23" t="s">
+        <v>121</v>
+      </c>
       <c r="K21" s="25"/>
       <c r="L21" s="25"/>
-      <c r="M21" s="23" t="s">
-        <v>121</v>
-      </c>
+      <c r="M21" s="25"/>
       <c r="N21" s="25"/>
       <c r="O21" s="25"/>
       <c r="P21" s="23" t="s">
@@ -4745,12 +4745,12 @@
       <c r="I22" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="J22" s="25"/>
+      <c r="J22" s="23" t="s">
+        <v>121</v>
+      </c>
       <c r="K22" s="25"/>
       <c r="L22" s="25"/>
-      <c r="M22" s="23" t="s">
-        <v>121</v>
-      </c>
+      <c r="M22" s="25"/>
       <c r="N22" s="25"/>
       <c r="O22" s="25"/>
       <c r="P22" s="23" t="s">
@@ -4789,12 +4789,12 @@
       <c r="I23" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="J23" s="25"/>
+      <c r="J23" s="23" t="s">
+        <v>121</v>
+      </c>
       <c r="K23" s="25"/>
       <c r="L23" s="25"/>
-      <c r="M23" s="23" t="s">
-        <v>121</v>
-      </c>
+      <c r="M23" s="25"/>
       <c r="N23" s="25"/>
       <c r="O23" s="25"/>
       <c r="P23" s="23" t="s">
@@ -4826,7 +4826,7 @@
   <dimension ref="B3:Y23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q12" sqref="Q12"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4867,16 +4867,16 @@
         <v>31</v>
       </c>
       <c r="J3" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="K3" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="K3" s="20" t="s">
+      <c r="L3" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="L3" s="20" t="s">
+      <c r="M3" s="20" t="s">
         <v>6</v>
-      </c>
-      <c r="M3" s="20" t="s">
-        <v>53</v>
       </c>
       <c r="N3" s="20" t="s">
         <v>7</v>
@@ -4927,13 +4927,13 @@
       <c r="I4" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="J4" s="25"/>
+      <c r="J4" s="23" t="s">
+        <v>121</v>
+      </c>
       <c r="K4" s="25"/>
-      <c r="L4" s="23" t="s">
+      <c r="L4" s="25"/>
+      <c r="M4" s="23" t="s">
         <v>239</v>
-      </c>
-      <c r="M4" s="23" t="s">
-        <v>121</v>
       </c>
       <c r="N4" s="23" t="s">
         <v>178</v>
@@ -4978,12 +4978,12 @@
       <c r="I5" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="J5" s="25"/>
+      <c r="J5" s="23" t="s">
+        <v>121</v>
+      </c>
       <c r="K5" s="25"/>
       <c r="L5" s="25"/>
-      <c r="M5" s="23" t="s">
-        <v>121</v>
-      </c>
+      <c r="M5" s="25"/>
       <c r="N5" s="23" t="s">
         <v>225</v>
       </c>
@@ -5025,12 +5025,12 @@
       <c r="I6" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="J6" s="25"/>
+      <c r="J6" s="23" t="s">
+        <v>121</v>
+      </c>
       <c r="K6" s="25"/>
       <c r="L6" s="25"/>
-      <c r="M6" s="23" t="s">
-        <v>121</v>
-      </c>
+      <c r="M6" s="25"/>
       <c r="N6" s="25"/>
       <c r="O6" s="25"/>
       <c r="P6" s="23" t="s">
@@ -5066,13 +5066,13 @@
       <c r="I7" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="J7" s="25"/>
+      <c r="J7" s="23" t="s">
+        <v>121</v>
+      </c>
       <c r="K7" s="25"/>
-      <c r="L7" s="23" t="s">
+      <c r="L7" s="25"/>
+      <c r="M7" s="23" t="s">
         <v>118</v>
-      </c>
-      <c r="M7" s="23" t="s">
-        <v>121</v>
       </c>
       <c r="N7" s="23" t="s">
         <v>122</v>
@@ -5109,12 +5109,12 @@
       <c r="I8" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="J8" s="25"/>
+      <c r="J8" s="23" t="s">
+        <v>121</v>
+      </c>
       <c r="K8" s="25"/>
       <c r="L8" s="25"/>
-      <c r="M8" s="23" t="s">
-        <v>121</v>
-      </c>
+      <c r="M8" s="25"/>
       <c r="N8" s="23" t="s">
         <v>123</v>
       </c>
@@ -5146,12 +5146,12 @@
       <c r="I9" s="23" t="b">
         <v>0</v>
       </c>
-      <c r="J9" s="25"/>
+      <c r="J9" s="23" t="s">
+        <v>121</v>
+      </c>
       <c r="K9" s="25"/>
       <c r="L9" s="25"/>
-      <c r="M9" s="23" t="s">
-        <v>121</v>
-      </c>
+      <c r="M9" s="25"/>
       <c r="N9" s="25"/>
       <c r="O9" s="25"/>
       <c r="P9" s="25"/>
@@ -5179,12 +5179,12 @@
         <v>116</v>
       </c>
       <c r="I10" s="22"/>
-      <c r="J10" s="25"/>
+      <c r="J10" s="23" t="s">
+        <v>121</v>
+      </c>
       <c r="K10" s="25"/>
       <c r="L10" s="25"/>
-      <c r="M10" s="23" t="s">
-        <v>121</v>
-      </c>
+      <c r="M10" s="25"/>
       <c r="N10" s="25"/>
       <c r="O10" s="23" t="s">
         <v>127</v>
@@ -5205,7 +5205,7 @@
     </row>
     <row r="11" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="19" t="s">
-        <v>12</v>
+        <v>53</v>
       </c>
       <c r="C11" s="25"/>
       <c r="D11" s="25"/>
@@ -5218,24 +5218,20 @@
       <c r="I11" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="J11" s="25"/>
+      <c r="J11" s="22"/>
       <c r="K11" s="25"/>
       <c r="L11" s="25"/>
-      <c r="M11" s="23" t="s">
-        <v>121</v>
-      </c>
+      <c r="M11" s="25"/>
       <c r="N11" s="25"/>
-      <c r="O11" s="23" t="s">
-        <v>111</v>
-      </c>
+      <c r="O11" s="25"/>
       <c r="P11" s="23" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="Q11" s="23" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="R11" s="23" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="S11" s="25"/>
       <c r="T11" s="25"/>
@@ -5244,7 +5240,7 @@
     </row>
     <row r="12" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="19" t="s">
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="C12" s="25"/>
       <c r="D12" s="25"/>
@@ -5257,22 +5253,24 @@
       <c r="I12" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="J12" s="25"/>
-      <c r="K12" s="22"/>
+      <c r="J12" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="K12" s="25"/>
       <c r="L12" s="25"/>
-      <c r="M12" s="23" t="s">
-        <v>121</v>
-      </c>
+      <c r="M12" s="25"/>
       <c r="N12" s="25"/>
-      <c r="O12" s="25"/>
+      <c r="O12" s="23" t="s">
+        <v>111</v>
+      </c>
       <c r="P12" s="23" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="Q12" s="23" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="R12" s="23" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="S12" s="25"/>
       <c r="T12" s="25"/>
@@ -5281,7 +5279,7 @@
     </row>
     <row r="13" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="19" t="s">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="C13" s="25"/>
       <c r="D13" s="25"/>
@@ -5294,26 +5292,22 @@
       <c r="I13" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="J13" s="25"/>
+      <c r="J13" s="23" t="s">
+        <v>121</v>
+      </c>
       <c r="K13" s="25"/>
-      <c r="L13" s="22" t="s">
-        <v>208</v>
-      </c>
-      <c r="M13" s="23" t="s">
-        <v>121</v>
-      </c>
-      <c r="N13" s="23" t="s">
-        <v>111</v>
-      </c>
+      <c r="L13" s="22"/>
+      <c r="M13" s="25"/>
+      <c r="N13" s="25"/>
       <c r="O13" s="25"/>
       <c r="P13" s="23" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="Q13" s="23" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="R13" s="23" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="S13" s="25"/>
       <c r="T13" s="25"/>
@@ -5322,7 +5316,7 @@
     </row>
     <row r="14" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="19" t="s">
-        <v>53</v>
+        <v>6</v>
       </c>
       <c r="C14" s="25"/>
       <c r="D14" s="25"/>
@@ -5335,20 +5329,26 @@
       <c r="I14" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="J14" s="25"/>
+      <c r="J14" s="23" t="s">
+        <v>121</v>
+      </c>
       <c r="K14" s="25"/>
       <c r="L14" s="25"/>
-      <c r="M14" s="22"/>
-      <c r="N14" s="25"/>
+      <c r="M14" s="22" t="s">
+        <v>208</v>
+      </c>
+      <c r="N14" s="23" t="s">
+        <v>111</v>
+      </c>
       <c r="O14" s="25"/>
       <c r="P14" s="23" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="Q14" s="23" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="R14" s="23" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="S14" s="25"/>
       <c r="T14" s="25"/>
@@ -5378,13 +5378,13 @@
       <c r="I15" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="J15" s="25"/>
+      <c r="J15" s="23" t="s">
+        <v>121</v>
+      </c>
       <c r="K15" s="25"/>
-      <c r="L15" s="24" t="s">
+      <c r="L15" s="25"/>
+      <c r="M15" s="24" t="s">
         <v>168</v>
-      </c>
-      <c r="M15" s="23" t="s">
-        <v>121</v>
       </c>
       <c r="N15" s="22" t="s">
         <v>208</v>
@@ -5419,12 +5419,12 @@
       <c r="I16" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="J16" s="25"/>
+      <c r="J16" s="23" t="s">
+        <v>121</v>
+      </c>
       <c r="K16" s="25"/>
       <c r="L16" s="25"/>
-      <c r="M16" s="23" t="s">
-        <v>121</v>
-      </c>
+      <c r="M16" s="25"/>
       <c r="N16" s="25"/>
       <c r="O16" s="22"/>
       <c r="P16" s="23" t="s">
@@ -5466,13 +5466,13 @@
       <c r="I17" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="J17" s="25"/>
+      <c r="J17" s="23" t="s">
+        <v>121</v>
+      </c>
       <c r="K17" s="25"/>
-      <c r="L17" s="23" t="s">
+      <c r="L17" s="25"/>
+      <c r="M17" s="23" t="s">
         <v>119</v>
-      </c>
-      <c r="M17" s="23" t="s">
-        <v>121</v>
       </c>
       <c r="N17" s="23" t="s">
         <v>124</v>
@@ -5511,15 +5511,15 @@
       <c r="I18" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="J18" s="25"/>
-      <c r="K18" s="23" t="s">
+      <c r="J18" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="K18" s="25"/>
+      <c r="L18" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="L18" s="23" t="s">
+      <c r="M18" s="23" t="s">
         <v>120</v>
-      </c>
-      <c r="M18" s="23" t="s">
-        <v>121</v>
       </c>
       <c r="N18" s="23" t="s">
         <v>125</v>
@@ -5556,12 +5556,12 @@
       <c r="I19" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="J19" s="25"/>
+      <c r="J19" s="23" t="s">
+        <v>121</v>
+      </c>
       <c r="K19" s="25"/>
       <c r="L19" s="25"/>
-      <c r="M19" s="23" t="s">
-        <v>121</v>
-      </c>
+      <c r="M19" s="25"/>
       <c r="N19" s="25"/>
       <c r="O19" s="25"/>
       <c r="P19" s="23" t="s">
@@ -5593,12 +5593,12 @@
       <c r="I20" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="J20" s="25"/>
+      <c r="J20" s="23" t="s">
+        <v>121</v>
+      </c>
       <c r="K20" s="25"/>
       <c r="L20" s="25"/>
-      <c r="M20" s="23" t="s">
-        <v>121</v>
-      </c>
+      <c r="M20" s="25"/>
       <c r="N20" s="25"/>
       <c r="O20" s="25"/>
       <c r="P20" s="23" t="s">
@@ -5630,12 +5630,12 @@
       <c r="I21" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="J21" s="25"/>
+      <c r="J21" s="23" t="s">
+        <v>121</v>
+      </c>
       <c r="K21" s="25"/>
       <c r="L21" s="25"/>
-      <c r="M21" s="23" t="s">
-        <v>121</v>
-      </c>
+      <c r="M21" s="25"/>
       <c r="N21" s="25"/>
       <c r="O21" s="25"/>
       <c r="P21" s="23" t="s">
@@ -5667,12 +5667,12 @@
       <c r="I22" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="J22" s="25"/>
+      <c r="J22" s="23" t="s">
+        <v>121</v>
+      </c>
       <c r="K22" s="25"/>
       <c r="L22" s="25"/>
-      <c r="M22" s="23" t="s">
-        <v>121</v>
-      </c>
+      <c r="M22" s="25"/>
       <c r="N22" s="25"/>
       <c r="O22" s="25"/>
       <c r="P22" s="23" t="s">
@@ -5706,12 +5706,12 @@
       <c r="I23" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="J23" s="25"/>
+      <c r="J23" s="23" t="s">
+        <v>121</v>
+      </c>
       <c r="K23" s="25"/>
       <c r="L23" s="25"/>
-      <c r="M23" s="23" t="s">
-        <v>121</v>
-      </c>
+      <c r="M23" s="25"/>
       <c r="N23" s="25"/>
       <c r="O23" s="25"/>
       <c r="P23" s="23" t="s">
@@ -5740,7 +5740,7 @@
   <dimension ref="B3:Y23"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5783,16 +5783,16 @@
         <v>31</v>
       </c>
       <c r="J3" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="K3" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="K3" s="20" t="s">
+      <c r="L3" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="L3" s="20" t="s">
+      <c r="M3" s="20" t="s">
         <v>6</v>
-      </c>
-      <c r="M3" s="20" t="s">
-        <v>53</v>
       </c>
       <c r="N3" s="20" t="s">
         <v>7</v>
@@ -5843,13 +5843,13 @@
       <c r="I4" s="28" t="s">
         <v>204</v>
       </c>
-      <c r="J4" s="25"/>
+      <c r="J4" s="23" t="s">
+        <v>121</v>
+      </c>
       <c r="K4" s="25"/>
-      <c r="L4" s="23" t="s">
+      <c r="L4" s="25"/>
+      <c r="M4" s="23" t="s">
         <v>239</v>
-      </c>
-      <c r="M4" s="23" t="s">
-        <v>121</v>
       </c>
       <c r="N4" s="28" t="s">
         <v>193</v>
@@ -5898,12 +5898,12 @@
       <c r="I5" s="28" t="s">
         <v>205</v>
       </c>
-      <c r="J5" s="25"/>
+      <c r="J5" s="23" t="s">
+        <v>121</v>
+      </c>
       <c r="K5" s="25"/>
       <c r="L5" s="25"/>
-      <c r="M5" s="23" t="s">
-        <v>121</v>
-      </c>
+      <c r="M5" s="25"/>
       <c r="N5" s="28" t="s">
         <v>232</v>
       </c>
@@ -5949,12 +5949,12 @@
       <c r="I6" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="J6" s="25"/>
+      <c r="J6" s="23" t="s">
+        <v>121</v>
+      </c>
       <c r="K6" s="25"/>
       <c r="L6" s="25"/>
-      <c r="M6" s="23" t="s">
-        <v>121</v>
-      </c>
+      <c r="M6" s="25"/>
       <c r="N6" s="25"/>
       <c r="O6" s="25"/>
       <c r="P6" s="23" t="s">
@@ -5990,13 +5990,13 @@
       <c r="I7" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="J7" s="25"/>
+      <c r="J7" s="23" t="s">
+        <v>121</v>
+      </c>
       <c r="K7" s="25"/>
-      <c r="L7" s="23" t="s">
+      <c r="L7" s="25"/>
+      <c r="M7" s="23" t="s">
         <v>118</v>
-      </c>
-      <c r="M7" s="23" t="s">
-        <v>121</v>
       </c>
       <c r="N7" s="23" t="s">
         <v>122</v>
@@ -6029,12 +6029,12 @@
       <c r="I8" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="J8" s="25"/>
+      <c r="J8" s="23" t="s">
+        <v>121</v>
+      </c>
       <c r="K8" s="25"/>
       <c r="L8" s="25"/>
-      <c r="M8" s="23" t="s">
-        <v>121</v>
-      </c>
+      <c r="M8" s="25"/>
       <c r="N8" s="23" t="s">
         <v>123</v>
       </c>
@@ -6062,12 +6062,12 @@
       <c r="I9" s="23" t="b">
         <v>0</v>
       </c>
-      <c r="J9" s="25"/>
+      <c r="J9" s="23" t="s">
+        <v>121</v>
+      </c>
       <c r="K9" s="25"/>
       <c r="L9" s="25"/>
-      <c r="M9" s="23" t="s">
-        <v>121</v>
-      </c>
+      <c r="M9" s="25"/>
       <c r="N9" s="25"/>
       <c r="O9" s="25"/>
       <c r="P9" s="25"/>
@@ -6093,12 +6093,12 @@
         <v>116</v>
       </c>
       <c r="I10" s="22"/>
-      <c r="J10" s="25"/>
+      <c r="J10" s="23" t="s">
+        <v>121</v>
+      </c>
       <c r="K10" s="25"/>
       <c r="L10" s="25"/>
-      <c r="M10" s="23" t="s">
-        <v>121</v>
-      </c>
+      <c r="M10" s="25"/>
       <c r="N10" s="25"/>
       <c r="O10" s="23" t="s">
         <v>127</v>
@@ -6115,7 +6115,7 @@
     </row>
     <row r="11" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="19" t="s">
-        <v>12</v>
+        <v>53</v>
       </c>
       <c r="C11" s="25"/>
       <c r="D11" s="25"/>
@@ -6128,18 +6128,14 @@
       <c r="I11" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="J11" s="25"/>
+      <c r="J11" s="22"/>
       <c r="K11" s="25"/>
       <c r="L11" s="25"/>
-      <c r="M11" s="23" t="s">
-        <v>121</v>
-      </c>
+      <c r="M11" s="25"/>
       <c r="N11" s="25"/>
-      <c r="O11" s="23" t="s">
-        <v>111</v>
-      </c>
+      <c r="O11" s="25"/>
       <c r="P11" s="23" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="Q11" s="28"/>
       <c r="R11" s="28"/>
@@ -6150,7 +6146,7 @@
     </row>
     <row r="12" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="19" t="s">
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="C12" s="25"/>
       <c r="D12" s="25"/>
@@ -6163,16 +6159,18 @@
       <c r="I12" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="J12" s="25"/>
-      <c r="K12" s="22"/>
+      <c r="J12" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="K12" s="25"/>
       <c r="L12" s="25"/>
-      <c r="M12" s="23" t="s">
-        <v>121</v>
-      </c>
+      <c r="M12" s="25"/>
       <c r="N12" s="25"/>
-      <c r="O12" s="25"/>
+      <c r="O12" s="23" t="s">
+        <v>111</v>
+      </c>
       <c r="P12" s="23" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="Q12" s="28"/>
       <c r="R12" s="28"/>
@@ -6183,7 +6181,7 @@
     </row>
     <row r="13" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="19" t="s">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="C13" s="25"/>
       <c r="D13" s="25"/>
@@ -6196,20 +6194,16 @@
       <c r="I13" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="J13" s="25"/>
+      <c r="J13" s="23" t="s">
+        <v>121</v>
+      </c>
       <c r="K13" s="25"/>
-      <c r="L13" s="22" t="s">
-        <v>208</v>
-      </c>
-      <c r="M13" s="23" t="s">
-        <v>121</v>
-      </c>
-      <c r="N13" s="23" t="s">
-        <v>111</v>
-      </c>
+      <c r="L13" s="22"/>
+      <c r="M13" s="25"/>
+      <c r="N13" s="25"/>
       <c r="O13" s="25"/>
       <c r="P13" s="23" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="Q13" s="28"/>
       <c r="R13" s="28"/>
@@ -6220,7 +6214,7 @@
     </row>
     <row r="14" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="19" t="s">
-        <v>53</v>
+        <v>6</v>
       </c>
       <c r="C14" s="25"/>
       <c r="D14" s="25"/>
@@ -6233,14 +6227,20 @@
       <c r="I14" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="J14" s="25"/>
+      <c r="J14" s="23" t="s">
+        <v>121</v>
+      </c>
       <c r="K14" s="25"/>
       <c r="L14" s="25"/>
-      <c r="M14" s="22"/>
-      <c r="N14" s="25"/>
+      <c r="M14" s="22" t="s">
+        <v>208</v>
+      </c>
+      <c r="N14" s="23" t="s">
+        <v>111</v>
+      </c>
       <c r="O14" s="25"/>
       <c r="P14" s="23" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="Q14" s="28"/>
       <c r="R14" s="28"/>
@@ -6272,13 +6272,13 @@
       <c r="I15" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="J15" s="25"/>
+      <c r="J15" s="23" t="s">
+        <v>121</v>
+      </c>
       <c r="K15" s="25"/>
-      <c r="L15" s="24" t="s">
+      <c r="L15" s="25"/>
+      <c r="M15" s="24" t="s">
         <v>168</v>
-      </c>
-      <c r="M15" s="23" t="s">
-        <v>121</v>
       </c>
       <c r="N15" s="22" t="s">
         <v>208</v>
@@ -6313,12 +6313,12 @@
       <c r="I16" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="J16" s="25"/>
+      <c r="J16" s="23" t="s">
+        <v>121</v>
+      </c>
       <c r="K16" s="25"/>
       <c r="L16" s="25"/>
-      <c r="M16" s="23" t="s">
-        <v>121</v>
-      </c>
+      <c r="M16" s="25"/>
       <c r="N16" s="25"/>
       <c r="O16" s="22"/>
       <c r="P16" s="23" t="s">
@@ -6356,13 +6356,13 @@
       <c r="I17" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="J17" s="25"/>
+      <c r="J17" s="23" t="s">
+        <v>121</v>
+      </c>
       <c r="K17" s="25"/>
-      <c r="L17" s="23" t="s">
+      <c r="L17" s="25"/>
+      <c r="M17" s="23" t="s">
         <v>119</v>
-      </c>
-      <c r="M17" s="23" t="s">
-        <v>121</v>
       </c>
       <c r="N17" s="23" t="s">
         <v>124</v>
@@ -6401,15 +6401,15 @@
       <c r="I18" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="J18" s="25"/>
-      <c r="K18" s="23" t="s">
+      <c r="J18" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="K18" s="25"/>
+      <c r="L18" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="L18" s="23" t="s">
+      <c r="M18" s="23" t="s">
         <v>120</v>
-      </c>
-      <c r="M18" s="23" t="s">
-        <v>121</v>
       </c>
       <c r="N18" s="23" t="s">
         <v>125</v>
@@ -6448,12 +6448,12 @@
       <c r="I19" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="J19" s="25"/>
+      <c r="J19" s="23" t="s">
+        <v>121</v>
+      </c>
       <c r="K19" s="25"/>
       <c r="L19" s="25"/>
-      <c r="M19" s="23" t="s">
-        <v>121</v>
-      </c>
+      <c r="M19" s="25"/>
       <c r="N19" s="25"/>
       <c r="O19" s="25"/>
       <c r="P19" s="23" t="s">
@@ -6485,12 +6485,12 @@
       <c r="I20" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="J20" s="25"/>
+      <c r="J20" s="23" t="s">
+        <v>121</v>
+      </c>
       <c r="K20" s="25"/>
       <c r="L20" s="25"/>
-      <c r="M20" s="23" t="s">
-        <v>121</v>
-      </c>
+      <c r="M20" s="25"/>
       <c r="N20" s="25"/>
       <c r="O20" s="25"/>
       <c r="P20" s="23" t="s">
@@ -6518,12 +6518,12 @@
       <c r="I21" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="J21" s="25"/>
+      <c r="J21" s="23" t="s">
+        <v>121</v>
+      </c>
       <c r="K21" s="25"/>
       <c r="L21" s="25"/>
-      <c r="M21" s="23" t="s">
-        <v>121</v>
-      </c>
+      <c r="M21" s="25"/>
       <c r="N21" s="25"/>
       <c r="O21" s="25"/>
       <c r="P21" s="23" t="s">
@@ -6556,12 +6556,12 @@
       <c r="I22" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="J22" s="25"/>
+      <c r="J22" s="23" t="s">
+        <v>121</v>
+      </c>
       <c r="K22" s="25"/>
       <c r="L22" s="25"/>
-      <c r="M22" s="23" t="s">
-        <v>121</v>
-      </c>
+      <c r="M22" s="25"/>
       <c r="N22" s="25"/>
       <c r="O22" s="25"/>
       <c r="P22" s="23" t="s">
@@ -6598,12 +6598,12 @@
       <c r="I23" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="J23" s="25"/>
+      <c r="J23" s="23" t="s">
+        <v>121</v>
+      </c>
       <c r="K23" s="25"/>
       <c r="L23" s="25"/>
-      <c r="M23" s="23" t="s">
-        <v>121</v>
-      </c>
+      <c r="M23" s="25"/>
       <c r="N23" s="25"/>
       <c r="O23" s="25"/>
       <c r="P23" s="23" t="s">

</xml_diff>

<commit_message>
FEAT: adds image! and pair! to conversion matrices.
</commit_message>
<xml_diff>
--- a/docs/conversion-matrix.xlsx
+++ b/docs/conversion-matrix.xlsx
@@ -23,6 +23,54 @@
     <author>dk</author>
   </authors>
   <commentList>
+    <comment ref="O3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>dk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+In R3, includes issue!</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>dk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+In R2, includes issue!</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="I4" authorId="0">
       <text>
         <r>
@@ -212,6 +260,54 @@
     <author>dk</author>
   </authors>
   <commentList>
+    <comment ref="O3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>dk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+In R2, includes issue!</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>dk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+In R2, includes issue!</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="L4" authorId="0">
       <text>
         <r>
@@ -386,6 +482,31 @@
       </text>
     </comment>
     <comment ref="R22" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>dk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+In R2: map/
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="R23" authorId="0">
       <text>
         <r>
           <rPr>
@@ -634,7 +755,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Y6" authorId="0">
+    <comment ref="AA6" authorId="0">
       <text>
         <r>
           <rPr>
@@ -759,12 +880,87 @@
         </r>
       </text>
     </comment>
+    <comment ref="R23" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>dk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+In R2: vector/
+In R3: name:/value/…</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="R24" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>dk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+In R2: image/
+In R3: name:/value/…</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="R25" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>dk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+In R2: pair/
+In R3: name:/value/…</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="899" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="929" uniqueCount="253">
   <si>
     <t>Red Datatype Comparison Matrix</t>
   </si>
@@ -1499,6 +1695,36 @@
   </si>
   <si>
     <t>New string from binary (decode UTF-8)</t>
+  </si>
+  <si>
+    <t>FORM map</t>
+  </si>
+  <si>
+    <t>FORM vector</t>
+  </si>
+  <si>
+    <t>FORM image</t>
+  </si>
+  <si>
+    <t>image/</t>
+  </si>
+  <si>
+    <t>New binary from image pixels</t>
+  </si>
+  <si>
+    <t>New image from binary</t>
+  </si>
+  <si>
+    <t>FORM pair</t>
+  </si>
+  <si>
+    <t>pair/</t>
+  </si>
+  <si>
+    <t>New pair from a list of two numbers</t>
+  </si>
+  <si>
+    <t>New image of size pair</t>
   </si>
 </sst>
 </file>
@@ -2129,7 +2355,7 @@
     <a:spDef>
       <a:spPr>
         <a:blipFill rotWithShape="1">
-          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
           <a:srcRect/>
           <a:tile tx="0" ty="0" sx="100000" sy="100000" flip="none" algn="tl"/>
         </a:blipFill>
@@ -3026,8 +3252,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:Y23"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q12" sqref="Q12"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3939,7 +4165,7 @@
   <dimension ref="B3:Y23"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="R23" sqref="R23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4804,7 +5030,7 @@
         <v>221</v>
       </c>
       <c r="R23" s="23" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
       <c r="S23" s="25"/>
       <c r="T23" s="25"/>
@@ -4823,10 +5049,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:Y23"/>
+  <dimension ref="B3:AA25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q12" sqref="Q12"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4838,10 +5064,10 @@
     <col min="15" max="15" width="14" style="18" customWidth="1"/>
     <col min="16" max="16" width="13.7109375" style="18" customWidth="1"/>
     <col min="17" max="18" width="11.85546875" style="18" customWidth="1"/>
-    <col min="19" max="22" width="13.28515625" style="18" customWidth="1"/>
+    <col min="19" max="24" width="13.28515625" style="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:25" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:27" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="21" t="s">
         <v>109</v>
       </c>
@@ -4905,8 +5131,14 @@
       <c r="V3" s="20" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="4" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W3" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="X3" s="20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="2:27" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="19" t="s">
         <v>24</v>
       </c>
@@ -4952,12 +5184,14 @@
       <c r="T4" s="25"/>
       <c r="U4" s="25"/>
       <c r="V4" s="25"/>
-      <c r="X4" s="22"/>
-      <c r="Y4" s="26" t="s">
+      <c r="W4" s="25"/>
+      <c r="X4" s="25"/>
+      <c r="Z4" s="22"/>
+      <c r="AA4" s="26" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="5" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:27" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="19" t="s">
         <v>223</v>
       </c>
@@ -5001,12 +5235,14 @@
       <c r="T5" s="25"/>
       <c r="U5" s="25"/>
       <c r="V5" s="25"/>
+      <c r="W5" s="25"/>
       <c r="X5" s="25"/>
-      <c r="Y5" s="27" t="s">
+      <c r="Z5" s="25"/>
+      <c r="AA5" s="27" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="6" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:27" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="19" t="s">
         <v>50</v>
       </c>
@@ -5046,8 +5282,10 @@
       <c r="T6" s="25"/>
       <c r="U6" s="25"/>
       <c r="V6" s="25"/>
-    </row>
-    <row r="7" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W6" s="25"/>
+      <c r="X6" s="25"/>
+    </row>
+    <row r="7" spans="2:27" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="19" t="s">
         <v>9</v>
       </c>
@@ -5093,8 +5331,10 @@
       <c r="T7" s="25"/>
       <c r="U7" s="25"/>
       <c r="V7" s="25"/>
-    </row>
-    <row r="8" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W7" s="25"/>
+      <c r="X7" s="25"/>
+    </row>
+    <row r="8" spans="2:27" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="19" t="s">
         <v>51</v>
       </c>
@@ -5132,8 +5372,10 @@
       <c r="T8" s="25"/>
       <c r="U8" s="25"/>
       <c r="V8" s="25"/>
-    </row>
-    <row r="9" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W8" s="25"/>
+      <c r="X8" s="25"/>
+    </row>
+    <row r="9" spans="2:27" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="19" t="s">
         <v>33</v>
       </c>
@@ -5165,8 +5407,10 @@
       <c r="T9" s="25"/>
       <c r="U9" s="25"/>
       <c r="V9" s="25"/>
-    </row>
-    <row r="10" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W9" s="25"/>
+      <c r="X9" s="25"/>
+    </row>
+    <row r="10" spans="2:27" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="19" t="s">
         <v>31</v>
       </c>
@@ -5202,8 +5446,10 @@
       <c r="T10" s="25"/>
       <c r="U10" s="25"/>
       <c r="V10" s="25"/>
-    </row>
-    <row r="11" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W10" s="25"/>
+      <c r="X10" s="25"/>
+    </row>
+    <row r="11" spans="2:27" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="19" t="s">
         <v>12</v>
       </c>
@@ -5241,8 +5487,10 @@
       <c r="T11" s="25"/>
       <c r="U11" s="25"/>
       <c r="V11" s="25"/>
-    </row>
-    <row r="12" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W11" s="25"/>
+      <c r="X11" s="25"/>
+    </row>
+    <row r="12" spans="2:27" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="19" t="s">
         <v>52</v>
       </c>
@@ -5278,8 +5526,10 @@
       <c r="T12" s="25"/>
       <c r="U12" s="25"/>
       <c r="V12" s="25"/>
-    </row>
-    <row r="13" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W12" s="25"/>
+      <c r="X12" s="25"/>
+    </row>
+    <row r="13" spans="2:27" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="19" t="s">
         <v>6</v>
       </c>
@@ -5319,8 +5569,10 @@
       <c r="T13" s="25"/>
       <c r="U13" s="25"/>
       <c r="V13" s="25"/>
-    </row>
-    <row r="14" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W13" s="25"/>
+      <c r="X13" s="25"/>
+    </row>
+    <row r="14" spans="2:27" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="19" t="s">
         <v>53</v>
       </c>
@@ -5354,8 +5606,10 @@
       <c r="T14" s="25"/>
       <c r="U14" s="25"/>
       <c r="V14" s="25"/>
-    </row>
-    <row r="15" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W14" s="25"/>
+      <c r="X14" s="25"/>
+    </row>
+    <row r="15" spans="2:27" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="19" t="s">
         <v>7</v>
       </c>
@@ -5403,8 +5657,12 @@
       <c r="T15" s="25"/>
       <c r="U15" s="25"/>
       <c r="V15" s="25"/>
-    </row>
-    <row r="16" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W15" s="24" t="s">
+        <v>248</v>
+      </c>
+      <c r="X15" s="25"/>
+    </row>
+    <row r="16" spans="2:27" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="19" t="s">
         <v>104</v>
       </c>
@@ -5440,8 +5698,10 @@
       <c r="T16" s="25"/>
       <c r="U16" s="25"/>
       <c r="V16" s="25"/>
-    </row>
-    <row r="17" spans="2:22" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W16" s="25"/>
+      <c r="X16" s="25"/>
+    </row>
+    <row r="17" spans="2:24" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="19" t="s">
         <v>105</v>
       </c>
@@ -5493,8 +5753,10 @@
       <c r="T17" s="25"/>
       <c r="U17" s="25"/>
       <c r="V17" s="25"/>
-    </row>
-    <row r="18" spans="2:22" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W17" s="25"/>
+      <c r="X17" s="25"/>
+    </row>
+    <row r="18" spans="2:24" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="19" t="s">
         <v>106</v>
       </c>
@@ -5540,8 +5802,12 @@
         <v>209</v>
       </c>
       <c r="V18" s="25"/>
-    </row>
-    <row r="19" spans="2:22" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W18" s="25"/>
+      <c r="X18" s="24" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="19" spans="2:24" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="19" t="s">
         <v>107</v>
       </c>
@@ -5577,8 +5843,10 @@
       <c r="T19" s="25"/>
       <c r="U19" s="25"/>
       <c r="V19" s="25"/>
-    </row>
-    <row r="20" spans="2:22" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W19" s="25"/>
+      <c r="X19" s="25"/>
+    </row>
+    <row r="20" spans="2:24" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="19" t="s">
         <v>108</v>
       </c>
@@ -5614,8 +5882,10 @@
       <c r="T20" s="25"/>
       <c r="U20" s="25"/>
       <c r="V20" s="25"/>
-    </row>
-    <row r="21" spans="2:22" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W20" s="25"/>
+      <c r="X20" s="25"/>
+    </row>
+    <row r="21" spans="2:24" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="19" t="s">
         <v>34</v>
       </c>
@@ -5651,8 +5921,10 @@
       <c r="T21" s="25"/>
       <c r="U21" s="25"/>
       <c r="V21" s="25"/>
-    </row>
-    <row r="22" spans="2:22" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W21" s="25"/>
+      <c r="X21" s="25"/>
+    </row>
+    <row r="22" spans="2:24" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="19" t="s">
         <v>29</v>
       </c>
@@ -5676,7 +5948,7 @@
       <c r="N22" s="25"/>
       <c r="O22" s="25"/>
       <c r="P22" s="23" t="s">
-        <v>139</v>
+        <v>243</v>
       </c>
       <c r="Q22" s="23" t="s">
         <v>220</v>
@@ -5690,8 +5962,10 @@
         <v>208</v>
       </c>
       <c r="V22" s="25"/>
-    </row>
-    <row r="23" spans="2:22" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W22" s="25"/>
+      <c r="X22" s="25"/>
+    </row>
+    <row r="23" spans="2:24" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="19" t="s">
         <v>56</v>
       </c>
@@ -5715,7 +5989,7 @@
       <c r="N23" s="25"/>
       <c r="O23" s="25"/>
       <c r="P23" s="23" t="s">
-        <v>139</v>
+        <v>244</v>
       </c>
       <c r="Q23" s="23" t="s">
         <v>221</v>
@@ -5727,6 +6001,86 @@
       <c r="T23" s="25"/>
       <c r="U23" s="25"/>
       <c r="V23" s="25"/>
+      <c r="W23" s="25"/>
+      <c r="X23" s="25"/>
+    </row>
+    <row r="24" spans="2:24" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" s="25"/>
+      <c r="D24" s="25"/>
+      <c r="E24" s="25"/>
+      <c r="F24" s="25"/>
+      <c r="G24" s="25"/>
+      <c r="H24" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="I24" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="J24" s="25"/>
+      <c r="K24" s="25"/>
+      <c r="L24" s="25"/>
+      <c r="M24" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="N24" s="24" t="s">
+        <v>247</v>
+      </c>
+      <c r="O24" s="25"/>
+      <c r="P24" s="23" t="s">
+        <v>245</v>
+      </c>
+      <c r="Q24" s="25"/>
+      <c r="R24" s="23" t="s">
+        <v>246</v>
+      </c>
+      <c r="S24" s="25"/>
+      <c r="T24" s="25"/>
+      <c r="U24" s="25"/>
+      <c r="V24" s="25"/>
+      <c r="W24" s="22" t="s">
+        <v>208</v>
+      </c>
+      <c r="X24" s="25"/>
+    </row>
+    <row r="25" spans="2:24" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="C25" s="25"/>
+      <c r="D25" s="25"/>
+      <c r="E25" s="25"/>
+      <c r="F25" s="25"/>
+      <c r="G25" s="25"/>
+      <c r="H25" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="I25" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="J25" s="25"/>
+      <c r="K25" s="25"/>
+      <c r="L25" s="25"/>
+      <c r="M25" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="N25" s="25"/>
+      <c r="O25" s="25"/>
+      <c r="P25" s="23" t="s">
+        <v>249</v>
+      </c>
+      <c r="Q25" s="25"/>
+      <c r="R25" s="23" t="s">
+        <v>250</v>
+      </c>
+      <c r="S25" s="25"/>
+      <c r="T25" s="25"/>
+      <c r="U25" s="25"/>
+      <c r="V25" s="25"/>
+      <c r="W25" s="25"/>
+      <c r="X25" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5737,10 +6091,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:Y23"/>
+  <dimension ref="B3:AA25"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+      <selection activeCell="W25" sqref="W25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5755,9 +6109,10 @@
     <col min="19" max="20" width="13.28515625" style="18" customWidth="1"/>
     <col min="21" max="21" width="14.7109375" style="18" customWidth="1"/>
     <col min="22" max="22" width="14.28515625" style="18" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="13.28515625" style="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:25" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:27" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="21" t="s">
         <v>109</v>
       </c>
@@ -5821,8 +6176,14 @@
       <c r="V3" s="20" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="4" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W3" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="X3" s="20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="2:27" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="19" t="s">
         <v>24</v>
       </c>
@@ -5872,12 +6233,14 @@
       <c r="V4" s="28" t="s">
         <v>211</v>
       </c>
-      <c r="X4" s="22"/>
-      <c r="Y4" s="26" t="s">
+      <c r="W4" s="25"/>
+      <c r="X4" s="25"/>
+      <c r="Z4" s="22"/>
+      <c r="AA4" s="26" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="5" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:27" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="19" t="s">
         <v>223</v>
       </c>
@@ -5925,12 +6288,14 @@
       <c r="V5" s="28" t="s">
         <v>238</v>
       </c>
+      <c r="W5" s="25"/>
       <c r="X5" s="25"/>
-      <c r="Y5" s="27" t="s">
+      <c r="Z5" s="25"/>
+      <c r="AA5" s="27" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="6" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:27" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="19" t="s">
         <v>50</v>
       </c>
@@ -5966,12 +6331,14 @@
       <c r="T6" s="25"/>
       <c r="U6" s="25"/>
       <c r="V6" s="25"/>
-      <c r="X6" s="29"/>
-      <c r="Y6" s="27" t="s">
+      <c r="W6" s="25"/>
+      <c r="X6" s="25"/>
+      <c r="Z6" s="29"/>
+      <c r="AA6" s="27" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="7" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:27" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="19" t="s">
         <v>9</v>
       </c>
@@ -6013,8 +6380,10 @@
       <c r="T7" s="25"/>
       <c r="U7" s="25"/>
       <c r="V7" s="25"/>
-    </row>
-    <row r="8" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W7" s="25"/>
+      <c r="X7" s="25"/>
+    </row>
+    <row r="8" spans="2:27" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="19" t="s">
         <v>51</v>
       </c>
@@ -6048,8 +6417,10 @@
       <c r="T8" s="25"/>
       <c r="U8" s="25"/>
       <c r="V8" s="25"/>
-    </row>
-    <row r="9" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W8" s="25"/>
+      <c r="X8" s="25"/>
+    </row>
+    <row r="9" spans="2:27" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="19" t="s">
         <v>33</v>
       </c>
@@ -6077,8 +6448,10 @@
       <c r="T9" s="25"/>
       <c r="U9" s="25"/>
       <c r="V9" s="25"/>
-    </row>
-    <row r="10" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W9" s="25"/>
+      <c r="X9" s="25"/>
+    </row>
+    <row r="10" spans="2:27" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="19" t="s">
         <v>31</v>
       </c>
@@ -6112,8 +6485,10 @@
       <c r="T10" s="25"/>
       <c r="U10" s="25"/>
       <c r="V10" s="25"/>
-    </row>
-    <row r="11" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W10" s="25"/>
+      <c r="X10" s="25"/>
+    </row>
+    <row r="11" spans="2:27" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="19" t="s">
         <v>12</v>
       </c>
@@ -6147,8 +6522,10 @@
       <c r="T11" s="25"/>
       <c r="U11" s="25"/>
       <c r="V11" s="25"/>
-    </row>
-    <row r="12" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W11" s="25"/>
+      <c r="X11" s="25"/>
+    </row>
+    <row r="12" spans="2:27" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="19" t="s">
         <v>52</v>
       </c>
@@ -6180,8 +6557,10 @@
       <c r="T12" s="25"/>
       <c r="U12" s="25"/>
       <c r="V12" s="25"/>
-    </row>
-    <row r="13" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W12" s="25"/>
+      <c r="X12" s="25"/>
+    </row>
+    <row r="13" spans="2:27" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="19" t="s">
         <v>6</v>
       </c>
@@ -6217,8 +6596,10 @@
       <c r="T13" s="25"/>
       <c r="U13" s="25"/>
       <c r="V13" s="25"/>
-    </row>
-    <row r="14" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W13" s="25"/>
+      <c r="X13" s="25"/>
+    </row>
+    <row r="14" spans="2:27" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="19" t="s">
         <v>53</v>
       </c>
@@ -6248,8 +6629,10 @@
       <c r="T14" s="25"/>
       <c r="U14" s="25"/>
       <c r="V14" s="25"/>
-    </row>
-    <row r="15" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W14" s="25"/>
+      <c r="X14" s="25"/>
+    </row>
+    <row r="15" spans="2:27" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="19" t="s">
         <v>7</v>
       </c>
@@ -6297,8 +6680,12 @@
       <c r="T15" s="25"/>
       <c r="U15" s="25"/>
       <c r="V15" s="25"/>
-    </row>
-    <row r="16" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W15" s="24" t="s">
+        <v>248</v>
+      </c>
+      <c r="X15" s="25"/>
+    </row>
+    <row r="16" spans="2:27" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="19" t="s">
         <v>104</v>
       </c>
@@ -6330,8 +6717,10 @@
       <c r="T16" s="25"/>
       <c r="U16" s="25"/>
       <c r="V16" s="25"/>
-    </row>
-    <row r="17" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W16" s="25"/>
+      <c r="X16" s="25"/>
+    </row>
+    <row r="17" spans="2:27" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="19" t="s">
         <v>105</v>
       </c>
@@ -6383,8 +6772,10 @@
       <c r="T17" s="25"/>
       <c r="U17" s="25"/>
       <c r="V17" s="25"/>
-    </row>
-    <row r="18" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W17" s="25"/>
+      <c r="X17" s="25"/>
+    </row>
+    <row r="18" spans="2:27" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="19" t="s">
         <v>106</v>
       </c>
@@ -6432,8 +6823,12 @@
       <c r="V18" s="28" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="19" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W18" s="25"/>
+      <c r="X18" s="24" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="19" spans="2:27" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="19" t="s">
         <v>107</v>
       </c>
@@ -6469,8 +6864,10 @@
       <c r="T19" s="25"/>
       <c r="U19" s="25"/>
       <c r="V19" s="25"/>
-    </row>
-    <row r="20" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W19" s="25"/>
+      <c r="X19" s="25"/>
+    </row>
+    <row r="20" spans="2:27" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="19" t="s">
         <v>108</v>
       </c>
@@ -6502,8 +6899,10 @@
       <c r="T20" s="25"/>
       <c r="U20" s="25"/>
       <c r="V20" s="25"/>
-    </row>
-    <row r="21" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W20" s="25"/>
+      <c r="X20" s="25"/>
+    </row>
+    <row r="21" spans="2:27" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="19" t="s">
         <v>34</v>
       </c>
@@ -6537,11 +6936,13 @@
       <c r="T21" s="25"/>
       <c r="U21" s="25"/>
       <c r="V21" s="25"/>
-      <c r="W21" s="30"/>
-      <c r="X21" s="30"/>
+      <c r="W21" s="25"/>
+      <c r="X21" s="25"/>
       <c r="Y21" s="30"/>
-    </row>
-    <row r="22" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Z21" s="30"/>
+      <c r="AA21" s="30"/>
+    </row>
+    <row r="22" spans="2:27" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="19" t="s">
         <v>29</v>
       </c>
@@ -6565,7 +6966,7 @@
       <c r="N22" s="25"/>
       <c r="O22" s="25"/>
       <c r="P22" s="23" t="s">
-        <v>139</v>
+        <v>243</v>
       </c>
       <c r="Q22" s="23" t="s">
         <v>220</v>
@@ -6579,11 +6980,13 @@
         <v>208</v>
       </c>
       <c r="V22" s="25"/>
-      <c r="W22" s="30"/>
-      <c r="X22" s="30"/>
+      <c r="W22" s="25"/>
+      <c r="X22" s="25"/>
       <c r="Y22" s="30"/>
-    </row>
-    <row r="23" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Z22" s="30"/>
+      <c r="AA22" s="30"/>
+    </row>
+    <row r="23" spans="2:27" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="19" t="s">
         <v>56</v>
       </c>
@@ -6607,21 +7010,98 @@
       <c r="N23" s="25"/>
       <c r="O23" s="25"/>
       <c r="P23" s="23" t="s">
-        <v>139</v>
+        <v>244</v>
       </c>
       <c r="Q23" s="23" t="s">
         <v>221</v>
       </c>
-      <c r="R23" s="23" t="s">
-        <v>218</v>
-      </c>
+      <c r="R23" s="28"/>
       <c r="S23" s="25"/>
       <c r="T23" s="25"/>
       <c r="U23" s="25"/>
       <c r="V23" s="25"/>
-      <c r="W23" s="30"/>
-      <c r="X23" s="30"/>
+      <c r="W23" s="25"/>
+      <c r="X23" s="25"/>
       <c r="Y23" s="30"/>
+      <c r="Z23" s="30"/>
+      <c r="AA23" s="30"/>
+    </row>
+    <row r="24" spans="2:27" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" s="25"/>
+      <c r="D24" s="25"/>
+      <c r="E24" s="25"/>
+      <c r="F24" s="25"/>
+      <c r="G24" s="25"/>
+      <c r="H24" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="I24" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="J24" s="25"/>
+      <c r="K24" s="25"/>
+      <c r="L24" s="25"/>
+      <c r="M24" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="N24" s="24" t="s">
+        <v>247</v>
+      </c>
+      <c r="O24" s="25"/>
+      <c r="P24" s="23" t="s">
+        <v>245</v>
+      </c>
+      <c r="Q24" s="25"/>
+      <c r="R24" s="28"/>
+      <c r="S24" s="25"/>
+      <c r="T24" s="25"/>
+      <c r="U24" s="25"/>
+      <c r="V24" s="25"/>
+      <c r="W24" s="22" t="s">
+        <v>208</v>
+      </c>
+      <c r="X24" s="25"/>
+      <c r="Y24" s="30"/>
+    </row>
+    <row r="25" spans="2:27" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="C25" s="25"/>
+      <c r="D25" s="25"/>
+      <c r="E25" s="25"/>
+      <c r="F25" s="25"/>
+      <c r="G25" s="25"/>
+      <c r="H25" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="I25" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="J25" s="25"/>
+      <c r="K25" s="25"/>
+      <c r="L25" s="25"/>
+      <c r="M25" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="N25" s="25"/>
+      <c r="O25" s="25"/>
+      <c r="P25" s="23" t="s">
+        <v>249</v>
+      </c>
+      <c r="Q25" s="25"/>
+      <c r="R25" s="28"/>
+      <c r="S25" s="25"/>
+      <c r="T25" s="25"/>
+      <c r="U25" s="25"/>
+      <c r="V25" s="25"/>
+      <c r="W25" s="28" t="s">
+        <v>252</v>
+      </c>
+      <c r="X25" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
FIX: adds some missing Red MAKE conversion descriptions.
</commit_message>
<xml_diff>
--- a/docs/conversion-matrix.xlsx
+++ b/docs/conversion-matrix.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr date1904="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="18075" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="18075" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="R3 TO matrix" sheetId="2" r:id="rId1"/>
@@ -960,7 +960,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="929" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="930" uniqueCount="254">
   <si>
     <t>Red Datatype Comparison Matrix</t>
   </si>
@@ -1725,6 +1725,9 @@
   </si>
   <si>
     <t>New image of size pair</t>
+  </si>
+  <si>
+    <t>New any-function from list spec</t>
   </si>
 </sst>
 </file>
@@ -5051,7 +5054,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:AA25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
@@ -6093,8 +6096,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:AA25"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="W25" sqref="W25"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="S18" sqref="S18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6815,7 +6818,9 @@
       <c r="R18" s="23" t="s">
         <v>154</v>
       </c>
-      <c r="S18" s="25"/>
+      <c r="S18" s="28" t="s">
+        <v>253</v>
+      </c>
       <c r="T18" s="25"/>
       <c r="U18" s="28" t="s">
         <v>214</v>

</xml_diff>

<commit_message>
FIX: adds missing source types to pair! and any-float! columns for TO/MAKE.
</commit_message>
<xml_diff>
--- a/docs/conversion-matrix.xlsx
+++ b/docs/conversion-matrix.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr date1904="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="18075" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="18075" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="R3 TO matrix" sheetId="2" r:id="rId1"/>
@@ -960,7 +960,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="930" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="936" uniqueCount="257">
   <si>
     <t>Red Datatype Comparison Matrix</t>
   </si>
@@ -1728,6 +1728,15 @@
   </si>
   <si>
     <t>New any-function from list spec</t>
+  </si>
+  <si>
+    <t>New pair from integer</t>
+  </si>
+  <si>
+    <t>New pair from truncated any-float</t>
+  </si>
+  <si>
+    <t>New any-float from list of 2 numbers</t>
   </si>
 </sst>
 </file>
@@ -5054,8 +5063,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:AA25"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5188,7 +5197,9 @@
       <c r="U4" s="25"/>
       <c r="V4" s="25"/>
       <c r="W4" s="25"/>
-      <c r="X4" s="25"/>
+      <c r="X4" s="24" t="s">
+        <v>254</v>
+      </c>
       <c r="Z4" s="22"/>
       <c r="AA4" s="26" t="s">
         <v>112</v>
@@ -5239,7 +5250,9 @@
       <c r="U5" s="25"/>
       <c r="V5" s="25"/>
       <c r="W5" s="25"/>
-      <c r="X5" s="25"/>
+      <c r="X5" s="24" t="s">
+        <v>255</v>
+      </c>
       <c r="Z5" s="25"/>
       <c r="AA5" s="27" t="s">
         <v>113</v>
@@ -5764,7 +5777,9 @@
         <v>106</v>
       </c>
       <c r="C18" s="25"/>
-      <c r="D18" s="25"/>
+      <c r="D18" s="24" t="s">
+        <v>256</v>
+      </c>
       <c r="E18" s="25"/>
       <c r="F18" s="25"/>
       <c r="G18" s="23" t="s">
@@ -6096,8 +6111,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:AA25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S18" sqref="S18"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6237,7 +6252,9 @@
         <v>211</v>
       </c>
       <c r="W4" s="25"/>
-      <c r="X4" s="25"/>
+      <c r="X4" s="24" t="s">
+        <v>254</v>
+      </c>
       <c r="Z4" s="22"/>
       <c r="AA4" s="26" t="s">
         <v>112</v>
@@ -6292,7 +6309,9 @@
         <v>238</v>
       </c>
       <c r="W5" s="25"/>
-      <c r="X5" s="25"/>
+      <c r="X5" s="24" t="s">
+        <v>255</v>
+      </c>
       <c r="Z5" s="25"/>
       <c r="AA5" s="27" t="s">
         <v>113</v>
@@ -6783,7 +6802,9 @@
         <v>106</v>
       </c>
       <c r="C18" s="25"/>
-      <c r="D18" s="25"/>
+      <c r="D18" s="24" t="s">
+        <v>256</v>
+      </c>
       <c r="E18" s="25"/>
       <c r="F18" s="25"/>
       <c r="G18" s="23" t="s">

</xml_diff>

<commit_message>
FEAT: relocates unset! column/rows in matrices.
</commit_message>
<xml_diff>
--- a/docs/conversion-matrix.xlsx
+++ b/docs/conversion-matrix.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr date1904="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="18075" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="18075" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="R3 TO matrix" sheetId="2" r:id="rId1"/>
@@ -23,6 +23,54 @@
     <author>dk</author>
   </authors>
   <commentList>
+    <comment ref="O3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>dk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+In R3, includes issue!</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>dk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+In R2, includes issue!</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="I4" authorId="0">
       <text>
         <r>
@@ -212,6 +260,54 @@
     <author>dk</author>
   </authors>
   <commentList>
+    <comment ref="O3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>dk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+In R2, includes issue!</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>dk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+In R2, includes issue!</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="M4" authorId="0">
       <text>
         <r>
@@ -386,6 +482,31 @@
       </text>
     </comment>
     <comment ref="R22" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>dk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+In R2: map/
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="R23" authorId="0">
       <text>
         <r>
           <rPr>
@@ -634,7 +755,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Y6" authorId="0">
+    <comment ref="AA6" authorId="0">
       <text>
         <r>
           <rPr>
@@ -759,12 +880,87 @@
         </r>
       </text>
     </comment>
+    <comment ref="R23" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>dk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+In R2: vector/
+In R3: name:/value/…</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="R24" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>dk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+In R2: image/
+In R3: name:/value/…</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="R25" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>dk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+In R2: pair/
+In R3: name:/value/…</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="899" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="936" uniqueCount="257">
   <si>
     <t>Red Datatype Comparison Matrix</t>
   </si>
@@ -1432,12 +1628,6 @@
     <t>New list from BODY-OF object</t>
   </si>
   <si>
-    <t>New map from BODY-OF object</t>
-  </si>
-  <si>
-    <t>New vector from BODY-OF object</t>
-  </si>
-  <si>
     <t>object/</t>
   </si>
   <si>
@@ -1499,6 +1689,54 @@
   </si>
   <si>
     <t>New string from binary (decode UTF-8)</t>
+  </si>
+  <si>
+    <t>FORM map</t>
+  </si>
+  <si>
+    <t>FORM vector</t>
+  </si>
+  <si>
+    <t>FORM image</t>
+  </si>
+  <si>
+    <t>image/</t>
+  </si>
+  <si>
+    <t>New binary from image pixels</t>
+  </si>
+  <si>
+    <t>New image from binary</t>
+  </si>
+  <si>
+    <t>FORM pair</t>
+  </si>
+  <si>
+    <t>pair/</t>
+  </si>
+  <si>
+    <t>New pair from a list of two numbers</t>
+  </si>
+  <si>
+    <t>New image of size pair</t>
+  </si>
+  <si>
+    <t>New any-function from list spec</t>
+  </si>
+  <si>
+    <t>New pair from integer</t>
+  </si>
+  <si>
+    <t>New pair from truncated any-float</t>
+  </si>
+  <si>
+    <t>New any-float from list of 2 numbers</t>
+  </si>
+  <si>
+    <t>New list from BODY-OF map</t>
+  </si>
+  <si>
+    <t>New list from BODY-OF vector</t>
   </si>
 </sst>
 </file>
@@ -3026,8 +3264,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:Y23"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q22" sqref="Q22:Q23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3134,7 +3372,7 @@
       <c r="K4" s="25"/>
       <c r="L4" s="25"/>
       <c r="M4" s="23" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="N4" s="23" t="s">
         <v>178</v>
@@ -3590,7 +3828,7 @@
       </c>
       <c r="O15" s="25"/>
       <c r="P15" s="23" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="Q15" s="23" t="s">
         <v>149</v>
@@ -3677,7 +3915,7 @@
         <v>124</v>
       </c>
       <c r="O17" s="23" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="P17" s="22" t="s">
         <v>208</v>
@@ -3702,7 +3940,7 @@
       <c r="E18" s="25"/>
       <c r="F18" s="25"/>
       <c r="G18" s="23" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="H18" s="23" t="s">
         <v>116</v>
@@ -3875,10 +4113,10 @@
       <c r="N22" s="25"/>
       <c r="O22" s="25"/>
       <c r="P22" s="23" t="s">
-        <v>139</v>
+        <v>241</v>
       </c>
       <c r="Q22" s="23" t="s">
-        <v>220</v>
+        <v>255</v>
       </c>
       <c r="R22" s="23" t="s">
         <v>207</v>
@@ -3914,10 +4152,10 @@
       <c r="N23" s="25"/>
       <c r="O23" s="25"/>
       <c r="P23" s="23" t="s">
-        <v>139</v>
+        <v>242</v>
       </c>
       <c r="Q23" s="23" t="s">
-        <v>221</v>
+        <v>256</v>
       </c>
       <c r="R23" s="23" t="s">
         <v>218</v>
@@ -3938,8 +4176,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:Y23"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q22" sqref="Q22:Q23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4046,7 +4284,7 @@
       <c r="K4" s="25"/>
       <c r="L4" s="25"/>
       <c r="M4" s="23" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="N4" s="28" t="s">
         <v>193</v>
@@ -4478,7 +4716,7 @@
       <c r="N15" s="22"/>
       <c r="O15" s="25"/>
       <c r="P15" s="23" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="Q15" s="28" t="s">
         <v>201</v>
@@ -4561,7 +4799,7 @@
         <v>124</v>
       </c>
       <c r="O17" s="23" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="P17" s="22"/>
       <c r="Q17" s="23" t="s">
@@ -4757,7 +4995,7 @@
         <v>139</v>
       </c>
       <c r="Q22" s="23" t="s">
-        <v>220</v>
+        <v>255</v>
       </c>
       <c r="R22" s="23" t="s">
         <v>207</v>
@@ -4801,10 +5039,10 @@
         <v>139</v>
       </c>
       <c r="Q23" s="23" t="s">
-        <v>221</v>
+        <v>256</v>
       </c>
       <c r="R23" s="23" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
       <c r="S23" s="25"/>
       <c r="T23" s="25"/>
@@ -4823,10 +5061,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:Y23"/>
+  <dimension ref="B3:AA25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q22" sqref="Q22:Q23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4838,10 +5076,10 @@
     <col min="15" max="15" width="14" style="18" customWidth="1"/>
     <col min="16" max="16" width="13.7109375" style="18" customWidth="1"/>
     <col min="17" max="18" width="11.85546875" style="18" customWidth="1"/>
-    <col min="19" max="22" width="13.28515625" style="18" customWidth="1"/>
+    <col min="19" max="24" width="13.28515625" style="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:25" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:27" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="21" t="s">
         <v>109</v>
       </c>
@@ -4849,7 +5087,7 @@
         <v>24</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="E3" s="20" t="s">
         <v>50</v>
@@ -4905,8 +5143,14 @@
       <c r="V3" s="20" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="4" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W3" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="X3" s="20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="2:27" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="19" t="s">
         <v>24</v>
       </c>
@@ -4933,7 +5177,7 @@
       <c r="K4" s="25"/>
       <c r="L4" s="25"/>
       <c r="M4" s="23" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="N4" s="23" t="s">
         <v>178</v>
@@ -4952,24 +5196,28 @@
       <c r="T4" s="25"/>
       <c r="U4" s="25"/>
       <c r="V4" s="25"/>
-      <c r="X4" s="22"/>
-      <c r="Y4" s="26" t="s">
+      <c r="W4" s="25"/>
+      <c r="X4" s="24" t="s">
+        <v>252</v>
+      </c>
+      <c r="Z4" s="22"/>
+      <c r="AA4" s="26" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="5" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:27" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="19" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C5" s="23" t="s">
         <v>169</v>
       </c>
       <c r="D5" s="22"/>
       <c r="E5" s="23" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="F5" s="23" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="G5" s="25"/>
       <c r="H5" s="23" t="s">
@@ -4985,28 +5233,32 @@
       <c r="L5" s="25"/>
       <c r="M5" s="25"/>
       <c r="N5" s="23" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="O5" s="25"/>
       <c r="P5" s="23" t="s">
+        <v>224</v>
+      </c>
+      <c r="Q5" s="23" t="s">
+        <v>225</v>
+      </c>
+      <c r="R5" s="23" t="s">
         <v>226</v>
-      </c>
-      <c r="Q5" s="23" t="s">
-        <v>227</v>
-      </c>
-      <c r="R5" s="23" t="s">
-        <v>228</v>
       </c>
       <c r="S5" s="25"/>
       <c r="T5" s="25"/>
       <c r="U5" s="25"/>
       <c r="V5" s="25"/>
-      <c r="X5" s="25"/>
-      <c r="Y5" s="27" t="s">
+      <c r="W5" s="25"/>
+      <c r="X5" s="24" t="s">
+        <v>253</v>
+      </c>
+      <c r="Z5" s="25"/>
+      <c r="AA5" s="27" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="6" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:27" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="19" t="s">
         <v>50</v>
       </c>
@@ -5046,8 +5298,10 @@
       <c r="T6" s="25"/>
       <c r="U6" s="25"/>
       <c r="V6" s="25"/>
-    </row>
-    <row r="7" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W6" s="25"/>
+      <c r="X6" s="25"/>
+    </row>
+    <row r="7" spans="2:27" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="19" t="s">
         <v>9</v>
       </c>
@@ -5055,7 +5309,7 @@
         <v>184</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="E7" s="25"/>
       <c r="F7" s="22"/>
@@ -5093,8 +5347,10 @@
       <c r="T7" s="25"/>
       <c r="U7" s="25"/>
       <c r="V7" s="25"/>
-    </row>
-    <row r="8" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W7" s="25"/>
+      <c r="X7" s="25"/>
+    </row>
+    <row r="8" spans="2:27" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="19" t="s">
         <v>51</v>
       </c>
@@ -5132,8 +5388,10 @@
       <c r="T8" s="25"/>
       <c r="U8" s="25"/>
       <c r="V8" s="25"/>
-    </row>
-    <row r="9" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W8" s="25"/>
+      <c r="X8" s="25"/>
+    </row>
+    <row r="9" spans="2:27" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="19" t="s">
         <v>33</v>
       </c>
@@ -5165,8 +5423,10 @@
       <c r="T9" s="25"/>
       <c r="U9" s="25"/>
       <c r="V9" s="25"/>
-    </row>
-    <row r="10" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W9" s="25"/>
+      <c r="X9" s="25"/>
+    </row>
+    <row r="10" spans="2:27" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="19" t="s">
         <v>31</v>
       </c>
@@ -5202,8 +5462,10 @@
       <c r="T10" s="25"/>
       <c r="U10" s="25"/>
       <c r="V10" s="25"/>
-    </row>
-    <row r="11" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W10" s="25"/>
+      <c r="X10" s="25"/>
+    </row>
+    <row r="11" spans="2:27" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="19" t="s">
         <v>53</v>
       </c>
@@ -5237,8 +5499,10 @@
       <c r="T11" s="25"/>
       <c r="U11" s="25"/>
       <c r="V11" s="25"/>
-    </row>
-    <row r="12" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W11" s="25"/>
+      <c r="X11" s="25"/>
+    </row>
+    <row r="12" spans="2:27" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="19" t="s">
         <v>12</v>
       </c>
@@ -5276,8 +5540,10 @@
       <c r="T12" s="25"/>
       <c r="U12" s="25"/>
       <c r="V12" s="25"/>
-    </row>
-    <row r="13" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W12" s="25"/>
+      <c r="X12" s="25"/>
+    </row>
+    <row r="13" spans="2:27" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="19" t="s">
         <v>52</v>
       </c>
@@ -5313,8 +5579,10 @@
       <c r="T13" s="25"/>
       <c r="U13" s="25"/>
       <c r="V13" s="25"/>
-    </row>
-    <row r="14" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W13" s="25"/>
+      <c r="X13" s="25"/>
+    </row>
+    <row r="14" spans="2:27" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="19" t="s">
         <v>6</v>
       </c>
@@ -5354,8 +5622,10 @@
       <c r="T14" s="25"/>
       <c r="U14" s="25"/>
       <c r="V14" s="25"/>
-    </row>
-    <row r="15" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W14" s="25"/>
+      <c r="X14" s="25"/>
+    </row>
+    <row r="15" spans="2:27" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="19" t="s">
         <v>7</v>
       </c>
@@ -5363,7 +5633,7 @@
         <v>185</v>
       </c>
       <c r="D15" s="23" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="E15" s="25"/>
       <c r="F15" s="23" t="s">
@@ -5391,7 +5661,7 @@
       </c>
       <c r="O15" s="25"/>
       <c r="P15" s="23" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="Q15" s="23" t="s">
         <v>149</v>
@@ -5403,8 +5673,12 @@
       <c r="T15" s="25"/>
       <c r="U15" s="25"/>
       <c r="V15" s="25"/>
-    </row>
-    <row r="16" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W15" s="24" t="s">
+        <v>246</v>
+      </c>
+      <c r="X15" s="25"/>
+    </row>
+    <row r="16" spans="2:27" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="19" t="s">
         <v>104</v>
       </c>
@@ -5440,8 +5714,10 @@
       <c r="T16" s="25"/>
       <c r="U16" s="25"/>
       <c r="V16" s="25"/>
-    </row>
-    <row r="17" spans="2:22" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W16" s="25"/>
+      <c r="X16" s="25"/>
+    </row>
+    <row r="17" spans="2:24" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="19" t="s">
         <v>105</v>
       </c>
@@ -5449,7 +5725,7 @@
         <v>187</v>
       </c>
       <c r="D17" s="23" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E17" s="23" t="s">
         <v>189</v>
@@ -5478,7 +5754,7 @@
         <v>124</v>
       </c>
       <c r="O17" s="23" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="P17" s="22" t="s">
         <v>208</v>
@@ -5493,17 +5769,21 @@
       <c r="T17" s="25"/>
       <c r="U17" s="25"/>
       <c r="V17" s="25"/>
-    </row>
-    <row r="18" spans="2:22" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W17" s="25"/>
+      <c r="X17" s="25"/>
+    </row>
+    <row r="18" spans="2:24" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="19" t="s">
         <v>106</v>
       </c>
       <c r="C18" s="25"/>
-      <c r="D18" s="25"/>
+      <c r="D18" s="24" t="s">
+        <v>254</v>
+      </c>
       <c r="E18" s="25"/>
       <c r="F18" s="25"/>
       <c r="G18" s="23" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="H18" s="23" t="s">
         <v>116</v>
@@ -5540,8 +5820,12 @@
         <v>209</v>
       </c>
       <c r="V18" s="25"/>
-    </row>
-    <row r="19" spans="2:22" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W18" s="25"/>
+      <c r="X18" s="24" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="19" spans="2:24" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="19" t="s">
         <v>107</v>
       </c>
@@ -5577,8 +5861,10 @@
       <c r="T19" s="25"/>
       <c r="U19" s="25"/>
       <c r="V19" s="25"/>
-    </row>
-    <row r="20" spans="2:22" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W19" s="25"/>
+      <c r="X19" s="25"/>
+    </row>
+    <row r="20" spans="2:24" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="19" t="s">
         <v>108</v>
       </c>
@@ -5614,8 +5900,10 @@
       <c r="T20" s="25"/>
       <c r="U20" s="25"/>
       <c r="V20" s="25"/>
-    </row>
-    <row r="21" spans="2:22" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W20" s="25"/>
+      <c r="X20" s="25"/>
+    </row>
+    <row r="21" spans="2:24" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="19" t="s">
         <v>34</v>
       </c>
@@ -5645,14 +5933,16 @@
         <v>219</v>
       </c>
       <c r="R21" s="23" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="S21" s="25"/>
       <c r="T21" s="25"/>
       <c r="U21" s="25"/>
       <c r="V21" s="25"/>
-    </row>
-    <row r="22" spans="2:22" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W21" s="25"/>
+      <c r="X21" s="25"/>
+    </row>
+    <row r="22" spans="2:24" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="19" t="s">
         <v>29</v>
       </c>
@@ -5676,10 +5966,10 @@
       <c r="N22" s="25"/>
       <c r="O22" s="25"/>
       <c r="P22" s="23" t="s">
-        <v>139</v>
+        <v>241</v>
       </c>
       <c r="Q22" s="23" t="s">
-        <v>220</v>
+        <v>255</v>
       </c>
       <c r="R22" s="23" t="s">
         <v>217</v>
@@ -5690,8 +5980,10 @@
         <v>208</v>
       </c>
       <c r="V22" s="25"/>
-    </row>
-    <row r="23" spans="2:22" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W22" s="25"/>
+      <c r="X22" s="25"/>
+    </row>
+    <row r="23" spans="2:24" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="19" t="s">
         <v>56</v>
       </c>
@@ -5715,10 +6007,10 @@
       <c r="N23" s="25"/>
       <c r="O23" s="25"/>
       <c r="P23" s="23" t="s">
-        <v>139</v>
+        <v>242</v>
       </c>
       <c r="Q23" s="23" t="s">
-        <v>221</v>
+        <v>256</v>
       </c>
       <c r="R23" s="23" t="s">
         <v>218</v>
@@ -5727,6 +6019,86 @@
       <c r="T23" s="25"/>
       <c r="U23" s="25"/>
       <c r="V23" s="25"/>
+      <c r="W23" s="25"/>
+      <c r="X23" s="25"/>
+    </row>
+    <row r="24" spans="2:24" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" s="25"/>
+      <c r="D24" s="25"/>
+      <c r="E24" s="25"/>
+      <c r="F24" s="25"/>
+      <c r="G24" s="25"/>
+      <c r="H24" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="I24" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="J24" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="K24" s="25"/>
+      <c r="L24" s="25"/>
+      <c r="M24" s="25"/>
+      <c r="N24" s="24" t="s">
+        <v>245</v>
+      </c>
+      <c r="O24" s="25"/>
+      <c r="P24" s="23" t="s">
+        <v>243</v>
+      </c>
+      <c r="Q24" s="25"/>
+      <c r="R24" s="23" t="s">
+        <v>244</v>
+      </c>
+      <c r="S24" s="25"/>
+      <c r="T24" s="25"/>
+      <c r="U24" s="25"/>
+      <c r="V24" s="25"/>
+      <c r="W24" s="22" t="s">
+        <v>208</v>
+      </c>
+      <c r="X24" s="25"/>
+    </row>
+    <row r="25" spans="2:24" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="C25" s="25"/>
+      <c r="D25" s="25"/>
+      <c r="E25" s="25"/>
+      <c r="F25" s="25"/>
+      <c r="G25" s="25"/>
+      <c r="H25" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="I25" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="J25" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="K25" s="25"/>
+      <c r="L25" s="25"/>
+      <c r="M25" s="25"/>
+      <c r="N25" s="25"/>
+      <c r="O25" s="25"/>
+      <c r="P25" s="23" t="s">
+        <v>247</v>
+      </c>
+      <c r="Q25" s="25"/>
+      <c r="R25" s="23" t="s">
+        <v>248</v>
+      </c>
+      <c r="S25" s="25"/>
+      <c r="T25" s="25"/>
+      <c r="U25" s="25"/>
+      <c r="V25" s="25"/>
+      <c r="W25" s="25"/>
+      <c r="X25" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5737,10 +6109,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:Y23"/>
+  <dimension ref="B3:AA25"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O25" sqref="O25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5755,9 +6127,10 @@
     <col min="19" max="20" width="13.28515625" style="18" customWidth="1"/>
     <col min="21" max="21" width="14.7109375" style="18" customWidth="1"/>
     <col min="22" max="22" width="14.28515625" style="18" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="13.28515625" style="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:25" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:27" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="21" t="s">
         <v>109</v>
       </c>
@@ -5765,7 +6138,7 @@
         <v>24</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="E3" s="20" t="s">
         <v>50</v>
@@ -5821,8 +6194,14 @@
       <c r="V3" s="20" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="4" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W3" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="X3" s="20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="2:27" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="19" t="s">
         <v>24</v>
       </c>
@@ -5849,7 +6228,7 @@
       <c r="K4" s="25"/>
       <c r="L4" s="25"/>
       <c r="M4" s="23" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="N4" s="28" t="s">
         <v>193</v>
@@ -5872,24 +6251,28 @@
       <c r="V4" s="28" t="s">
         <v>211</v>
       </c>
-      <c r="X4" s="22"/>
-      <c r="Y4" s="26" t="s">
+      <c r="W4" s="25"/>
+      <c r="X4" s="24" t="s">
+        <v>252</v>
+      </c>
+      <c r="Z4" s="22"/>
+      <c r="AA4" s="26" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="5" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:27" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="19" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C5" s="23" t="s">
         <v>169</v>
       </c>
       <c r="D5" s="22"/>
       <c r="E5" s="23" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="F5" s="23" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="G5" s="25"/>
       <c r="H5" s="23" t="s">
@@ -5905,32 +6288,36 @@
       <c r="L5" s="25"/>
       <c r="M5" s="25"/>
       <c r="N5" s="28" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="O5" s="25"/>
       <c r="P5" s="28" t="s">
+        <v>231</v>
+      </c>
+      <c r="Q5" s="28" t="s">
+        <v>232</v>
+      </c>
+      <c r="R5" s="28" t="s">
         <v>233</v>
-      </c>
-      <c r="Q5" s="28" t="s">
-        <v>234</v>
-      </c>
-      <c r="R5" s="28" t="s">
-        <v>235</v>
       </c>
       <c r="S5" s="25"/>
       <c r="T5" s="25"/>
       <c r="U5" s="28" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="V5" s="28" t="s">
-        <v>238</v>
-      </c>
-      <c r="X5" s="25"/>
-      <c r="Y5" s="27" t="s">
+        <v>236</v>
+      </c>
+      <c r="W5" s="25"/>
+      <c r="X5" s="24" t="s">
+        <v>253</v>
+      </c>
+      <c r="Z5" s="25"/>
+      <c r="AA5" s="27" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="6" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:27" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="19" t="s">
         <v>50</v>
       </c>
@@ -5966,12 +6353,14 @@
       <c r="T6" s="25"/>
       <c r="U6" s="25"/>
       <c r="V6" s="25"/>
-      <c r="X6" s="29"/>
-      <c r="Y6" s="27" t="s">
+      <c r="W6" s="25"/>
+      <c r="X6" s="25"/>
+      <c r="Z6" s="29"/>
+      <c r="AA6" s="27" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="7" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:27" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="19" t="s">
         <v>9</v>
       </c>
@@ -5979,7 +6368,7 @@
         <v>184</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="E7" s="25"/>
       <c r="F7" s="22"/>
@@ -6013,8 +6402,10 @@
       <c r="T7" s="25"/>
       <c r="U7" s="25"/>
       <c r="V7" s="25"/>
-    </row>
-    <row r="8" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W7" s="25"/>
+      <c r="X7" s="25"/>
+    </row>
+    <row r="8" spans="2:27" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="19" t="s">
         <v>51</v>
       </c>
@@ -6048,8 +6439,10 @@
       <c r="T8" s="25"/>
       <c r="U8" s="25"/>
       <c r="V8" s="25"/>
-    </row>
-    <row r="9" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W8" s="25"/>
+      <c r="X8" s="25"/>
+    </row>
+    <row r="9" spans="2:27" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="19" t="s">
         <v>33</v>
       </c>
@@ -6077,8 +6470,10 @@
       <c r="T9" s="25"/>
       <c r="U9" s="25"/>
       <c r="V9" s="25"/>
-    </row>
-    <row r="10" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W9" s="25"/>
+      <c r="X9" s="25"/>
+    </row>
+    <row r="10" spans="2:27" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="19" t="s">
         <v>31</v>
       </c>
@@ -6112,8 +6507,10 @@
       <c r="T10" s="25"/>
       <c r="U10" s="25"/>
       <c r="V10" s="25"/>
-    </row>
-    <row r="11" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W10" s="25"/>
+      <c r="X10" s="25"/>
+    </row>
+    <row r="11" spans="2:27" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="19" t="s">
         <v>53</v>
       </c>
@@ -6143,8 +6540,10 @@
       <c r="T11" s="25"/>
       <c r="U11" s="25"/>
       <c r="V11" s="25"/>
-    </row>
-    <row r="12" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W11" s="25"/>
+      <c r="X11" s="25"/>
+    </row>
+    <row r="12" spans="2:27" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="19" t="s">
         <v>12</v>
       </c>
@@ -6178,8 +6577,10 @@
       <c r="T12" s="25"/>
       <c r="U12" s="25"/>
       <c r="V12" s="25"/>
-    </row>
-    <row r="13" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W12" s="25"/>
+      <c r="X12" s="25"/>
+    </row>
+    <row r="13" spans="2:27" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="19" t="s">
         <v>52</v>
       </c>
@@ -6211,8 +6612,10 @@
       <c r="T13" s="25"/>
       <c r="U13" s="25"/>
       <c r="V13" s="25"/>
-    </row>
-    <row r="14" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W13" s="25"/>
+      <c r="X13" s="25"/>
+    </row>
+    <row r="14" spans="2:27" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="19" t="s">
         <v>6</v>
       </c>
@@ -6248,8 +6651,10 @@
       <c r="T14" s="25"/>
       <c r="U14" s="25"/>
       <c r="V14" s="25"/>
-    </row>
-    <row r="15" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W14" s="25"/>
+      <c r="X14" s="25"/>
+    </row>
+    <row r="15" spans="2:27" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="19" t="s">
         <v>7</v>
       </c>
@@ -6257,7 +6662,7 @@
         <v>185</v>
       </c>
       <c r="D15" s="23" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="E15" s="25"/>
       <c r="F15" s="23" t="s">
@@ -6285,7 +6690,7 @@
       </c>
       <c r="O15" s="25"/>
       <c r="P15" s="23" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="Q15" s="28" t="s">
         <v>201</v>
@@ -6297,8 +6702,12 @@
       <c r="T15" s="25"/>
       <c r="U15" s="25"/>
       <c r="V15" s="25"/>
-    </row>
-    <row r="16" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W15" s="24" t="s">
+        <v>246</v>
+      </c>
+      <c r="X15" s="25"/>
+    </row>
+    <row r="16" spans="2:27" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="19" t="s">
         <v>104</v>
       </c>
@@ -6330,8 +6739,10 @@
       <c r="T16" s="25"/>
       <c r="U16" s="25"/>
       <c r="V16" s="25"/>
-    </row>
-    <row r="17" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W16" s="25"/>
+      <c r="X16" s="25"/>
+    </row>
+    <row r="17" spans="2:27" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="19" t="s">
         <v>105</v>
       </c>
@@ -6339,7 +6750,7 @@
         <v>187</v>
       </c>
       <c r="D17" s="23" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E17" s="23" t="s">
         <v>189</v>
@@ -6368,7 +6779,7 @@
         <v>124</v>
       </c>
       <c r="O17" s="23" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="P17" s="22" t="s">
         <v>208</v>
@@ -6383,13 +6794,17 @@
       <c r="T17" s="25"/>
       <c r="U17" s="25"/>
       <c r="V17" s="25"/>
-    </row>
-    <row r="18" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W17" s="25"/>
+      <c r="X17" s="25"/>
+    </row>
+    <row r="18" spans="2:27" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="19" t="s">
         <v>106</v>
       </c>
       <c r="C18" s="25"/>
-      <c r="D18" s="25"/>
+      <c r="D18" s="24" t="s">
+        <v>254</v>
+      </c>
       <c r="E18" s="25"/>
       <c r="F18" s="25"/>
       <c r="G18" s="23" t="s">
@@ -6424,7 +6839,9 @@
       <c r="R18" s="23" t="s">
         <v>154</v>
       </c>
-      <c r="S18" s="25"/>
+      <c r="S18" s="28" t="s">
+        <v>251</v>
+      </c>
       <c r="T18" s="25"/>
       <c r="U18" s="28" t="s">
         <v>214</v>
@@ -6432,8 +6849,12 @@
       <c r="V18" s="28" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="19" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W18" s="25"/>
+      <c r="X18" s="24" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="19" spans="2:27" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="19" t="s">
         <v>107</v>
       </c>
@@ -6469,8 +6890,10 @@
       <c r="T19" s="25"/>
       <c r="U19" s="25"/>
       <c r="V19" s="25"/>
-    </row>
-    <row r="20" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W19" s="25"/>
+      <c r="X19" s="25"/>
+    </row>
+    <row r="20" spans="2:27" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="19" t="s">
         <v>108</v>
       </c>
@@ -6502,8 +6925,10 @@
       <c r="T20" s="25"/>
       <c r="U20" s="25"/>
       <c r="V20" s="25"/>
-    </row>
-    <row r="21" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W20" s="25"/>
+      <c r="X20" s="25"/>
+    </row>
+    <row r="21" spans="2:27" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="19" t="s">
         <v>34</v>
       </c>
@@ -6537,11 +6962,13 @@
       <c r="T21" s="25"/>
       <c r="U21" s="25"/>
       <c r="V21" s="25"/>
-      <c r="W21" s="30"/>
-      <c r="X21" s="30"/>
+      <c r="W21" s="25"/>
+      <c r="X21" s="25"/>
       <c r="Y21" s="30"/>
-    </row>
-    <row r="22" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Z21" s="30"/>
+      <c r="AA21" s="30"/>
+    </row>
+    <row r="22" spans="2:27" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="19" t="s">
         <v>29</v>
       </c>
@@ -6565,10 +6992,10 @@
       <c r="N22" s="25"/>
       <c r="O22" s="25"/>
       <c r="P22" s="23" t="s">
-        <v>139</v>
+        <v>241</v>
       </c>
       <c r="Q22" s="23" t="s">
-        <v>220</v>
+        <v>255</v>
       </c>
       <c r="R22" s="28"/>
       <c r="S22" s="25"/>
@@ -6579,11 +7006,13 @@
         <v>208</v>
       </c>
       <c r="V22" s="25"/>
-      <c r="W22" s="30"/>
-      <c r="X22" s="30"/>
+      <c r="W22" s="25"/>
+      <c r="X22" s="25"/>
       <c r="Y22" s="30"/>
-    </row>
-    <row r="23" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Z22" s="30"/>
+      <c r="AA22" s="30"/>
+    </row>
+    <row r="23" spans="2:27" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="19" t="s">
         <v>56</v>
       </c>
@@ -6607,21 +7036,98 @@
       <c r="N23" s="25"/>
       <c r="O23" s="25"/>
       <c r="P23" s="23" t="s">
-        <v>139</v>
+        <v>242</v>
       </c>
       <c r="Q23" s="23" t="s">
-        <v>221</v>
-      </c>
-      <c r="R23" s="23" t="s">
-        <v>218</v>
-      </c>
+        <v>256</v>
+      </c>
+      <c r="R23" s="28"/>
       <c r="S23" s="25"/>
       <c r="T23" s="25"/>
       <c r="U23" s="25"/>
       <c r="V23" s="25"/>
-      <c r="W23" s="30"/>
-      <c r="X23" s="30"/>
+      <c r="W23" s="25"/>
+      <c r="X23" s="25"/>
       <c r="Y23" s="30"/>
+      <c r="Z23" s="30"/>
+      <c r="AA23" s="30"/>
+    </row>
+    <row r="24" spans="2:27" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" s="25"/>
+      <c r="D24" s="25"/>
+      <c r="E24" s="25"/>
+      <c r="F24" s="25"/>
+      <c r="G24" s="25"/>
+      <c r="H24" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="I24" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="J24" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="K24" s="25"/>
+      <c r="L24" s="25"/>
+      <c r="M24" s="25"/>
+      <c r="N24" s="24" t="s">
+        <v>245</v>
+      </c>
+      <c r="O24" s="25"/>
+      <c r="P24" s="23" t="s">
+        <v>243</v>
+      </c>
+      <c r="Q24" s="25"/>
+      <c r="R24" s="28"/>
+      <c r="S24" s="25"/>
+      <c r="T24" s="25"/>
+      <c r="U24" s="25"/>
+      <c r="V24" s="25"/>
+      <c r="W24" s="22" t="s">
+        <v>208</v>
+      </c>
+      <c r="X24" s="25"/>
+      <c r="Y24" s="30"/>
+    </row>
+    <row r="25" spans="2:27" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="C25" s="25"/>
+      <c r="D25" s="25"/>
+      <c r="E25" s="25"/>
+      <c r="F25" s="25"/>
+      <c r="G25" s="25"/>
+      <c r="H25" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="I25" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="J25" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="K25" s="25"/>
+      <c r="L25" s="25"/>
+      <c r="M25" s="25"/>
+      <c r="N25" s="25"/>
+      <c r="O25" s="25"/>
+      <c r="P25" s="23" t="s">
+        <v>247</v>
+      </c>
+      <c r="Q25" s="25"/>
+      <c r="R25" s="28"/>
+      <c r="S25" s="25"/>
+      <c r="T25" s="25"/>
+      <c r="U25" s="25"/>
+      <c r="V25" s="25"/>
+      <c r="W25" s="28" t="s">
+        <v>250</v>
+      </c>
+      <c r="X25" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
FIX: missing TO error! from any-list! conversion in Red matrices.
</commit_message>
<xml_diff>
--- a/docs/conversion-matrix.xlsx
+++ b/docs/conversion-matrix.xlsx
@@ -853,6 +853,32 @@
         </r>
       </text>
     </comment>
+    <comment ref="O17" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>dk:
+Only string! to any-word!</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Checks if string contains valid characters for a word.
+</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="R21" authorId="0">
       <text>
         <r>
@@ -1095,6 +1121,32 @@
         </r>
       </text>
     </comment>
+    <comment ref="O17" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>dk:
+Only string! to any-word!</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Checks if string contains valid characters for a word.
+</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="R21" authorId="0">
       <text>
         <r>
@@ -1296,7 +1348,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="955" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="955" uniqueCount="263">
   <si>
     <t>From \ To</t>
   </si>
@@ -2088,13 +2140,16 @@
   </si>
   <si>
     <t>New error! from any-list spec</t>
+  </si>
+  <si>
+    <t>LOAD valid string! as any-word</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -2141,6 +2196,19 @@
       <sz val="8"/>
       <name val="Tahoma"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="9">
@@ -2421,6 +2489,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2432,9 +2503,6 @@
     </xf>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5388,7 +5456,7 @@
   <dimension ref="B3:AB26"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -6095,7 +6163,7 @@
         <v>92</v>
       </c>
       <c r="O17" s="23" t="s">
-        <v>93</v>
+        <v>262</v>
       </c>
       <c r="P17" s="22" t="s">
         <v>80</v>
@@ -6506,7 +6574,7 @@
   <dimension ref="B3:AB26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q14" sqref="Q14"/>
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -7191,7 +7259,7 @@
         <v>92</v>
       </c>
       <c r="O17" s="23" t="s">
-        <v>93</v>
+        <v>262</v>
       </c>
       <c r="P17" s="22" t="s">
         <v>80</v>
@@ -7268,7 +7336,7 @@
       <c r="X18" s="26" t="s">
         <v>155</v>
       </c>
-      <c r="Y18" s="35" t="s">
+      <c r="Y18" s="31" t="s">
         <v>261</v>
       </c>
     </row>
@@ -7621,66 +7689,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:58" ht="27.95" customHeight="1">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="32" t="s">
         <v>174</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
-      <c r="N1" s="31"/>
-      <c r="O1" s="31"/>
-      <c r="P1" s="31"/>
-      <c r="Q1" s="31"/>
-      <c r="R1" s="31"/>
-      <c r="S1" s="31"/>
-      <c r="T1" s="31"/>
-      <c r="U1" s="31"/>
-      <c r="V1" s="31"/>
-      <c r="W1" s="31"/>
-      <c r="X1" s="31"/>
-      <c r="Y1" s="31"/>
-      <c r="Z1" s="31"/>
-      <c r="AA1" s="31"/>
-      <c r="AB1" s="31"/>
-      <c r="AC1" s="31"/>
-      <c r="AD1" s="31"/>
-      <c r="AE1" s="31"/>
-      <c r="AF1" s="31"/>
-      <c r="AG1" s="31"/>
-      <c r="AH1" s="31"/>
-      <c r="AI1" s="31"/>
-      <c r="AJ1" s="31"/>
-      <c r="AK1" s="31"/>
-      <c r="AL1" s="31"/>
-      <c r="AM1" s="31"/>
-      <c r="AN1" s="31"/>
-      <c r="AO1" s="31"/>
-      <c r="AP1" s="31"/>
-      <c r="AQ1" s="31"/>
-      <c r="AR1" s="31"/>
-      <c r="AS1" s="31"/>
-      <c r="AT1" s="31"/>
-      <c r="AU1" s="31"/>
-      <c r="AV1" s="31"/>
-      <c r="AW1" s="31"/>
-      <c r="AX1" s="31"/>
-      <c r="AY1" s="31"/>
-      <c r="AZ1" s="31"/>
-      <c r="BA1" s="31"/>
-      <c r="BB1" s="31"/>
-      <c r="BC1" s="31"/>
-      <c r="BD1" s="31"/>
-      <c r="BE1" s="31"/>
-      <c r="BF1" s="31"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
+      <c r="L1" s="32"/>
+      <c r="M1" s="32"/>
+      <c r="N1" s="32"/>
+      <c r="O1" s="32"/>
+      <c r="P1" s="32"/>
+      <c r="Q1" s="32"/>
+      <c r="R1" s="32"/>
+      <c r="S1" s="32"/>
+      <c r="T1" s="32"/>
+      <c r="U1" s="32"/>
+      <c r="V1" s="32"/>
+      <c r="W1" s="32"/>
+      <c r="X1" s="32"/>
+      <c r="Y1" s="32"/>
+      <c r="Z1" s="32"/>
+      <c r="AA1" s="32"/>
+      <c r="AB1" s="32"/>
+      <c r="AC1" s="32"/>
+      <c r="AD1" s="32"/>
+      <c r="AE1" s="32"/>
+      <c r="AF1" s="32"/>
+      <c r="AG1" s="32"/>
+      <c r="AH1" s="32"/>
+      <c r="AI1" s="32"/>
+      <c r="AJ1" s="32"/>
+      <c r="AK1" s="32"/>
+      <c r="AL1" s="32"/>
+      <c r="AM1" s="32"/>
+      <c r="AN1" s="32"/>
+      <c r="AO1" s="32"/>
+      <c r="AP1" s="32"/>
+      <c r="AQ1" s="32"/>
+      <c r="AR1" s="32"/>
+      <c r="AS1" s="32"/>
+      <c r="AT1" s="32"/>
+      <c r="AU1" s="32"/>
+      <c r="AV1" s="32"/>
+      <c r="AW1" s="32"/>
+      <c r="AX1" s="32"/>
+      <c r="AY1" s="32"/>
+      <c r="AZ1" s="32"/>
+      <c r="BA1" s="32"/>
+      <c r="BB1" s="32"/>
+      <c r="BC1" s="32"/>
+      <c r="BD1" s="32"/>
+      <c r="BE1" s="32"/>
+      <c r="BF1" s="32"/>
     </row>
     <row r="2" spans="1:58" ht="20.65" customHeight="1">
       <c r="A2" s="2"/>
@@ -7857,7 +7925,7 @@
       </c>
     </row>
     <row r="3" spans="1:58" ht="32.65" customHeight="1">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="33" t="s">
         <v>176</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -8033,7 +8101,7 @@
       </c>
     </row>
     <row r="4" spans="1:58" ht="44.45" customHeight="1">
-      <c r="A4" s="33"/>
+      <c r="A4" s="34"/>
       <c r="B4" s="7"/>
       <c r="C4" s="8" t="s">
         <v>217</v>
@@ -8133,7 +8201,7 @@
       <c r="BF4" s="9"/>
     </row>
     <row r="5" spans="1:58" ht="68.45" customHeight="1">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="35" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="10" t="s">
@@ -8309,7 +8377,7 @@
       </c>
     </row>
     <row r="6" spans="1:58" ht="68.45" customHeight="1">
-      <c r="A6" s="33"/>
+      <c r="A6" s="34"/>
       <c r="B6" s="7"/>
       <c r="C6" s="12"/>
       <c r="D6" s="9"/>

</xml_diff>

<commit_message>
FEAT: adds issue! specific conversions to any-word! rows/columns in Red matrices.
</commit_message>
<xml_diff>
--- a/docs/conversion-matrix.xlsx
+++ b/docs/conversion-matrix.xlsx
@@ -693,6 +693,30 @@
     <author>dk</author>
   </authors>
   <commentList>
+    <comment ref="O3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>dk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Issue! is part of any-word!</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="I4" authorId="0">
       <text>
         <r>
@@ -853,6 +877,30 @@
         </r>
       </text>
     </comment>
+    <comment ref="B16" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>dk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Issue! is part of any-word!</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="O17" authorId="0">
       <text>
         <r>
@@ -863,8 +911,8 @@
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
-          <t>dk:
-Only string! to any-word!</t>
+          <t xml:space="preserve">dk:
+</t>
         </r>
         <r>
           <rPr>
@@ -873,8 +921,7 @@
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">
-Checks if string contains valid characters for a word.
+          <t xml:space="preserve">Checks if string contains valid characters for a word.
 </t>
         </r>
       </text>
@@ -967,6 +1014,30 @@
     <author>dk</author>
   </authors>
   <commentList>
+    <comment ref="O3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>dk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Issue! is part of any-word!</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="M4" authorId="0">
       <text>
         <r>
@@ -1121,6 +1192,30 @@
         </r>
       </text>
     </comment>
+    <comment ref="B16" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>dk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Issue! is part of any-word!</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="O17" authorId="0">
       <text>
         <r>
@@ -1131,8 +1226,8 @@
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
-          <t>dk:
-Only string! to any-word!</t>
+          <t xml:space="preserve">dk:
+</t>
         </r>
         <r>
           <rPr>
@@ -1141,8 +1236,7 @@
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">
-Checks if string contains valid characters for a word.
+          <t xml:space="preserve">Checks if string contains valid characters for a word.
 </t>
         </r>
       </text>
@@ -1348,7 +1442,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="955" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="958" uniqueCount="266">
   <si>
     <t>From \ To</t>
   </si>
@@ -2142,7 +2236,16 @@
     <t>New error! from any-list spec</t>
   </si>
   <si>
-    <t>LOAD valid string! as any-word</t>
+    <t>FORM error</t>
+  </si>
+  <si>
+    <t>New tuple from issue as hex bytes</t>
+  </si>
+  <si>
+    <t>New binary from issue as hex bytes</t>
+  </si>
+  <si>
+    <t>LOAD valid string as any-word</t>
   </si>
 </sst>
 </file>
@@ -5456,7 +5559,7 @@
   <dimension ref="B3:AB26"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O17" sqref="O17"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -5464,7 +5567,7 @@
     <col min="1" max="1" width="9.42578125" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" customWidth="1"/>
     <col min="3" max="12" width="11.85546875" style="18" customWidth="1"/>
-    <col min="13" max="13" width="13.42578125" style="18" customWidth="1"/>
+    <col min="13" max="13" width="12.140625" style="18" customWidth="1"/>
     <col min="14" max="14" width="13.85546875" style="18" customWidth="1"/>
     <col min="15" max="15" width="14" style="18" customWidth="1"/>
     <col min="16" max="16" width="13.7109375" style="18" customWidth="1"/>
@@ -6094,7 +6197,9 @@
       <c r="D16" s="24"/>
       <c r="E16" s="24"/>
       <c r="F16" s="24"/>
-      <c r="G16" s="24"/>
+      <c r="G16" s="26" t="s">
+        <v>263</v>
+      </c>
       <c r="H16" s="23" t="s">
         <v>24</v>
       </c>
@@ -6107,7 +6212,9 @@
       <c r="K16" s="24"/>
       <c r="L16" s="24"/>
       <c r="M16" s="24"/>
-      <c r="N16" s="24"/>
+      <c r="N16" s="26" t="s">
+        <v>264</v>
+      </c>
       <c r="O16" s="22"/>
       <c r="P16" s="23" t="s">
         <v>83</v>
@@ -6163,7 +6270,7 @@
         <v>92</v>
       </c>
       <c r="O17" s="23" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="P17" s="22" t="s">
         <v>80</v>
@@ -6195,7 +6302,7 @@
       <c r="E18" s="24"/>
       <c r="F18" s="24"/>
       <c r="G18" s="23" t="s">
-        <v>96</v>
+        <v>134</v>
       </c>
       <c r="H18" s="23" t="s">
         <v>24</v>
@@ -6574,7 +6681,7 @@
   <dimension ref="B3:AB26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O17" sqref="O17"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -7194,7 +7301,9 @@
       <c r="D16" s="24"/>
       <c r="E16" s="24"/>
       <c r="F16" s="24"/>
-      <c r="G16" s="24"/>
+      <c r="G16" s="26" t="s">
+        <v>263</v>
+      </c>
       <c r="H16" s="23" t="s">
         <v>24</v>
       </c>
@@ -7207,7 +7316,9 @@
       <c r="K16" s="24"/>
       <c r="L16" s="24"/>
       <c r="M16" s="24"/>
-      <c r="N16" s="24"/>
+      <c r="N16" s="26" t="s">
+        <v>264</v>
+      </c>
       <c r="O16" s="22"/>
       <c r="P16" s="23" t="s">
         <v>83</v>
@@ -7259,7 +7370,7 @@
         <v>92</v>
       </c>
       <c r="O17" s="23" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="P17" s="22" t="s">
         <v>80</v>
@@ -7646,12 +7757,10 @@
       <c r="N26" s="24"/>
       <c r="O26" s="24"/>
       <c r="P26" s="23" t="s">
-        <v>163</v>
+        <v>262</v>
       </c>
       <c r="Q26" s="24"/>
-      <c r="R26" s="23" t="s">
-        <v>164</v>
-      </c>
+      <c r="R26" s="25"/>
       <c r="S26" s="24"/>
       <c r="T26" s="24"/>
       <c r="U26" s="24"/>

</xml_diff>

<commit_message>
FEAT: adds MAKE/TO image! face! conversions to Red matrices.
</commit_message>
<xml_diff>
--- a/docs/conversion-matrix.xlsx
+++ b/docs/conversion-matrix.xlsx
@@ -1442,7 +1442,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="958" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="960" uniqueCount="267">
   <si>
     <t>From \ To</t>
   </si>
@@ -2246,6 +2246,9 @@
   </si>
   <si>
     <t>LOAD valid string as any-word</t>
+  </si>
+  <si>
+    <t>New image from face! objects only</t>
   </si>
 </sst>
 </file>
@@ -5558,8 +5561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:AB26"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="W21" sqref="W21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -6461,7 +6464,9 @@
       <c r="T21" s="24"/>
       <c r="U21" s="24"/>
       <c r="V21" s="24"/>
-      <c r="W21" s="24"/>
+      <c r="W21" s="26" t="s">
+        <v>266</v>
+      </c>
       <c r="X21" s="24"/>
       <c r="Y21" s="24"/>
     </row>
@@ -6681,7 +6686,7 @@
   <dimension ref="B3:AB26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="T21" sqref="T21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -7561,7 +7566,9 @@
       <c r="T21" s="24"/>
       <c r="U21" s="24"/>
       <c r="V21" s="24"/>
-      <c r="W21" s="24"/>
+      <c r="W21" s="26" t="s">
+        <v>266</v>
+      </c>
       <c r="X21" s="24"/>
       <c r="Y21" s="24"/>
       <c r="Z21" s="30"/>

</xml_diff>

<commit_message>
FEAT: activates the changes tracking mode.
</commit_message>
<xml_diff>
--- a/docs/conversion-matrix.xlsx
+++ b/docs/conversion-matrix.xlsx
@@ -7,13 +7,16 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="28365" windowHeight="13845" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="R3 TO matrix" sheetId="2" r:id="rId1"/>
-    <sheet name="R3 MAKE matrix" sheetId="3" r:id="rId2"/>
-    <sheet name="Red TO matrix" sheetId="5" r:id="rId3"/>
-    <sheet name="Red MAKE matrix" sheetId="6" r:id="rId4"/>
-    <sheet name="Sheet 1 - Red Datatype Comparis" sheetId="1" r:id="rId5"/>
+    <sheet name="R3 TO matrix" sheetId="1" r:id="rId1"/>
+    <sheet name="R3 MAKE matrix" sheetId="2" r:id="rId2"/>
+    <sheet name="Red TO matrix" sheetId="3" r:id="rId3"/>
+    <sheet name="Red MAKE matrix" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet 1 - Red Datatype Comparis" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="144525"/>
+  <customWorkbookViews>
+    <customWorkbookView name="dk - Personal View" guid="{DC8FA253-E57B-4689-B148-2145DC64729C}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1920" windowHeight="1063" activeSheetId="4"/>
+  </customWorkbookViews>
 </workbook>
 </file>
 
@@ -23,7 +26,7 @@
     <author>dk</author>
   </authors>
   <commentList>
-    <comment ref="O3" authorId="0">
+    <comment ref="O3" authorId="0" guid="{2416CB28-009A-45BE-A267-78FE278F65F2}">
       <text>
         <r>
           <rPr>
@@ -53,7 +56,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P3" authorId="0">
+    <comment ref="P3" authorId="0" guid="{2607A368-0303-4826-BDDD-8B0F0CE5CA6D}">
       <text>
         <r>
           <rPr>
@@ -83,7 +86,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I4" authorId="0">
+    <comment ref="I4" authorId="0" guid="{ED0C478D-9C80-481A-B477-9EB404BF0C93}">
       <text>
         <r>
           <rPr>
@@ -132,7 +135,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M4" authorId="0">
+    <comment ref="M4" authorId="0" guid="{E41B2BEA-5401-4296-8509-A74117F43BA8}">
       <text>
         <r>
           <rPr>
@@ -163,7 +166,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C6" authorId="0">
+    <comment ref="C6" authorId="0" guid="{DF10D5A9-2B76-4D51-B90D-6C832A5ED0EE}">
       <text>
         <r>
           <rPr>
@@ -194,7 +197,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C10" authorId="0">
+    <comment ref="C10" authorId="0" guid="{6C10BD0F-A3AD-45F1-80D9-6816010CA0EB}">
       <text>
         <r>
           <rPr>
@@ -243,7 +246,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O10" authorId="0">
+    <comment ref="O10" authorId="0" guid="{F42EED44-92FA-460E-8112-008F5A232A14}">
       <text>
         <r>
           <rPr>
@@ -274,7 +277,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R21" authorId="0">
+    <comment ref="R21" authorId="0" guid="{916ACD79-0E32-4318-AD56-81B9B624D038}">
       <text>
         <r>
           <rPr>
@@ -305,7 +308,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R22" authorId="0">
+    <comment ref="R22" authorId="0" guid="{8F6013B1-B0BF-4F5F-9F16-AF564F01299F}">
       <text>
         <r>
           <rPr>
@@ -346,7 +349,7 @@
     <author>dk</author>
   </authors>
   <commentList>
-    <comment ref="O3" authorId="0">
+    <comment ref="O3" authorId="0" guid="{79453CF4-9E50-4B15-8503-25F9220C56B8}">
       <text>
         <r>
           <rPr>
@@ -376,7 +379,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P3" authorId="0">
+    <comment ref="P3" authorId="0" guid="{29B44EBC-FAFE-49AD-A964-7ABB5F3E44EB}">
       <text>
         <r>
           <rPr>
@@ -406,7 +409,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M4" authorId="0">
+    <comment ref="M4" authorId="0" guid="{A299FFF8-0EC7-4E14-99BC-16D4A0570BF1}">
       <text>
         <r>
           <rPr>
@@ -437,7 +440,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C6" authorId="0">
+    <comment ref="C6" authorId="0" guid="{1B7D160F-721C-40F8-849F-044C6D4D9282}">
       <text>
         <r>
           <rPr>
@@ -468,7 +471,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Y6" authorId="0">
+    <comment ref="Y6" authorId="0" guid="{7DDDCAA1-D6D0-42B7-9CC4-05B174DBE1AA}">
       <text>
         <r>
           <rPr>
@@ -498,7 +501,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q9" authorId="0">
+    <comment ref="Q9" authorId="0" guid="{A54830FC-D978-4E1F-B4D0-F56175A6176E}">
       <text>
         <r>
           <rPr>
@@ -529,7 +532,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R9" authorId="0">
+    <comment ref="R9" authorId="0" guid="{BE5C1617-0A1C-4D1C-A675-575A912A381F}">
       <text>
         <r>
           <rPr>
@@ -560,7 +563,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O10" authorId="0">
+    <comment ref="O10" authorId="0" guid="{213122DD-736C-4A72-80F2-73E3ED4984DE}">
       <text>
         <r>
           <rPr>
@@ -590,7 +593,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R21" authorId="0">
+    <comment ref="R21" authorId="0" guid="{525F130D-B6D3-4363-964B-47D5F3C6DF60}">
       <text>
         <r>
           <rPr>
@@ -621,7 +624,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R22" authorId="0">
+    <comment ref="R22" authorId="0" guid="{3657B928-F115-4F71-8F82-BD5A74E26C67}">
       <text>
         <r>
           <rPr>
@@ -652,7 +655,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R23" authorId="0">
+    <comment ref="R23" authorId="0" guid="{2500CCBD-8A30-4039-8271-DD220F373673}">
       <text>
         <r>
           <rPr>
@@ -693,7 +696,7 @@
     <author>dk</author>
   </authors>
   <commentList>
-    <comment ref="O3" authorId="0">
+    <comment ref="O3" authorId="0" guid="{3EA23033-0597-4F26-BA7B-CC92AA980256}">
       <text>
         <r>
           <rPr>
@@ -717,7 +720,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I4" authorId="0">
+    <comment ref="I4" authorId="0" guid="{EAFC00BB-B70B-447B-A865-E7D113D09D18}">
       <text>
         <r>
           <rPr>
@@ -766,7 +769,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M4" authorId="0">
+    <comment ref="M4" authorId="0" guid="{E7754DBE-BC8E-4AEA-8683-257400ADB710}">
       <text>
         <r>
           <rPr>
@@ -797,7 +800,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C6" authorId="0">
+    <comment ref="C6" authorId="0" guid="{EFED36B3-D103-44D3-8274-F65EC1DC0EA7}">
       <text>
         <r>
           <rPr>
@@ -828,7 +831,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C10" authorId="0">
+    <comment ref="C10" authorId="0" guid="{61F5B90E-545C-429F-997B-7DE8C2C23315}">
       <text>
         <r>
           <rPr>
@@ -877,7 +880,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B16" authorId="0">
+    <comment ref="B16" authorId="0" guid="{1DDE07E4-DB93-4EF4-ADC2-5A52CFB90FB8}">
       <text>
         <r>
           <rPr>
@@ -901,7 +904,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O17" authorId="0">
+    <comment ref="O17" authorId="0" guid="{7EC96390-9C63-463F-AFAC-48CC3C91E88B}">
       <text>
         <r>
           <rPr>
@@ -926,7 +929,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R21" authorId="0">
+    <comment ref="R21" authorId="0" guid="{F6585264-2767-498C-B975-896F0CB0F6E3}">
       <text>
         <r>
           <rPr>
@@ -965,7 +968,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R22" authorId="0">
+    <comment ref="R22" authorId="0" guid="{F6457AC1-BA4D-400E-A156-2DB2AC116F51}">
       <text>
         <r>
           <rPr>
@@ -1014,7 +1017,7 @@
     <author>dk</author>
   </authors>
   <commentList>
-    <comment ref="O3" authorId="0">
+    <comment ref="O3" authorId="0" guid="{ECB3D93B-6AAE-4C79-80CD-6847038E0716}">
       <text>
         <r>
           <rPr>
@@ -1038,7 +1041,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M4" authorId="0">
+    <comment ref="M4" authorId="0" guid="{459E9D6E-CB97-40A9-BE20-935978E22FF0}">
       <text>
         <r>
           <rPr>
@@ -1069,7 +1072,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C6" authorId="0">
+    <comment ref="C6" authorId="0" guid="{C2E1826F-370A-4FFE-B670-3802A52257CF}">
       <text>
         <r>
           <rPr>
@@ -1100,7 +1103,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AB6" authorId="0">
+    <comment ref="AB6" authorId="0" guid="{0BDF1013-D58D-4951-A727-A729D363E38A}">
       <text>
         <r>
           <rPr>
@@ -1130,7 +1133,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q9" authorId="0">
+    <comment ref="Q9" authorId="0" guid="{ADAE1E2A-5037-4AA2-B386-3659ECBC0B2A}">
       <text>
         <r>
           <rPr>
@@ -1161,7 +1164,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R9" authorId="0">
+    <comment ref="R9" authorId="0" guid="{494C1674-AD9C-44FE-833C-B861DF4981E0}">
       <text>
         <r>
           <rPr>
@@ -1192,7 +1195,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B16" authorId="0">
+    <comment ref="B16" authorId="0" guid="{4F4E8030-A705-4B8B-B4A6-3BCC5D513E84}">
       <text>
         <r>
           <rPr>
@@ -1216,7 +1219,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O17" authorId="0">
+    <comment ref="O17" authorId="0" guid="{3BC863B9-C0D9-4F3B-A87C-8B28179340DC}">
       <text>
         <r>
           <rPr>
@@ -1241,7 +1244,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R21" authorId="0">
+    <comment ref="R21" authorId="0" guid="{388A97B7-6AEF-411B-B8D6-0ACB030EEC05}">
       <text>
         <r>
           <rPr>
@@ -1281,7 +1284,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R22" authorId="0">
+    <comment ref="R22" authorId="0" guid="{42531486-3275-4E45-9037-453611746CBD}">
       <text>
         <r>
           <rPr>
@@ -1320,7 +1323,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R23" authorId="0">
+    <comment ref="R23" authorId="0" guid="{A781D05B-035F-4197-8D64-175B07D4FBB3}">
       <text>
         <r>
           <rPr>
@@ -1359,7 +1362,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R24" authorId="0">
+    <comment ref="R24" authorId="0" guid="{F599D45C-B612-482E-8409-438C7457968A}">
       <text>
         <r>
           <rPr>
@@ -1398,7 +1401,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R25" authorId="0">
+    <comment ref="R25" authorId="0" guid="{B8942FE7-917C-44EB-AB6B-DD2B4BDC9879}">
       <text>
         <r>
           <rPr>
@@ -2690,6 +2693,28 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{9FFB1614-79BA-4BC5-903A-E94B28A6F5C6}">
+  <header guid="{9FFB1614-79BA-4BC5-903A-E94B28A6F5C6}" dateTime="2016-11-14T19:29:56" maxSheetId="6" userName="dk" r:id="rId1">
+    <sheetIdMap count="5">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+    </sheetIdMap>
+  </header>
+</headers>
+</file>
+
+<file path=xl/revisions/revisionLog1.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac"/>
+</file>
+
+<file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4664,6 +4689,13 @@
       <c r="V23" s="24"/>
     </row>
   </sheetData>
+  <customSheetViews>
+    <customSheetView guid="{DC8FA253-E57B-4689-B148-2145DC64729C}" scale="85" topLeftCell="A10">
+      <selection activeCell="Q22" sqref="Q22:Q23"/>
+      <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait"/>
+    </customSheetView>
+  </customSheetViews>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <legacyDrawing r:id="rId1"/>
@@ -5551,6 +5583,13 @@
       <c r="Y23" s="30"/>
     </row>
   </sheetData>
+  <customSheetViews>
+    <customSheetView guid="{DC8FA253-E57B-4689-B148-2145DC64729C}" scale="85" topLeftCell="A7">
+      <selection activeCell="Q22" sqref="Q22:Q23"/>
+      <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait"/>
+    </customSheetView>
+  </customSheetViews>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <legacyDrawing r:id="rId1"/>
@@ -5561,7 +5600,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:AB26"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="W21" sqref="W21"/>
     </sheetView>
   </sheetViews>
@@ -6675,6 +6714,13 @@
       </c>
     </row>
   </sheetData>
+  <customSheetViews>
+    <customSheetView guid="{DC8FA253-E57B-4689-B148-2145DC64729C}" scale="85">
+      <selection activeCell="W21" sqref="W21"/>
+      <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait"/>
+    </customSheetView>
+  </customSheetViews>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <legacyDrawing r:id="rId1"/>
@@ -6685,8 +6731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:AB26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="T21" sqref="T21"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -7779,6 +7825,13 @@
       </c>
     </row>
   </sheetData>
+  <customSheetViews>
+    <customSheetView guid="{DC8FA253-E57B-4689-B148-2145DC64729C}" scale="85" topLeftCell="A7">
+      <selection activeCell="T21" sqref="T21"/>
+      <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait"/>
+    </customSheetView>
+  </customSheetViews>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <legacyDrawing r:id="rId1"/>
@@ -9599,6 +9652,17 @@
       <c r="BF23" s="14"/>
     </row>
   </sheetData>
+  <customSheetViews>
+    <customSheetView guid="{DC8FA253-E57B-4689-B148-2145DC64729C}" showGridLines="0" fitToPage="1">
+      <pane xSplit="1" ySplit="2" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+      <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.27777777777777801" footer="0.27777777777777801"/>
+      <pageSetup orientation="portrait"/>
+      <headerFooter>
+        <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+      </headerFooter>
+    </customSheetView>
+  </customSheetViews>
   <mergeCells count="3">
     <mergeCell ref="A1:BF1"/>
     <mergeCell ref="A3:A4"/>

</xml_diff>

<commit_message>
FIX: improves MAKE/TO image! <type> conversions in Red matrices.
</commit_message>
<xml_diff>
--- a/docs/conversion-matrix.xlsx
+++ b/docs/conversion-matrix.xlsx
@@ -1445,7 +1445,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="960" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="959" uniqueCount="267">
   <si>
     <t>From \ To</t>
   </si>
@@ -1908,9 +1908,6 @@
     <t>base 16 binary as any-float</t>
   </si>
   <si>
-    <t>New image from binary</t>
-  </si>
-  <si>
     <t>LOAD string as any-float</t>
   </si>
   <si>
@@ -2252,6 +2249,9 @@
   </si>
   <si>
     <t>New image from face! objects only</t>
+  </si>
+  <si>
+    <t>New image from spec list</t>
   </si>
 </sst>
 </file>
@@ -2696,8 +2696,17 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{9FFB1614-79BA-4BC5-903A-E94B28A6F5C6}">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{55E251B5-98E1-4201-A738-B9370268DF37}" diskRevisions="1" revisionId="3" version="2">
   <header guid="{9FFB1614-79BA-4BC5-903A-E94B28A6F5C6}" dateTime="2016-11-14T19:29:56" maxSheetId="6" userName="dk" r:id="rId1">
+    <sheetIdMap count="5">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{55E251B5-98E1-4201-A738-B9370268DF37}" dateTime="2016-11-14T19:36:14" maxSheetId="6" userName="dk" r:id="rId2" minRId="1" maxRId="3">
     <sheetIdMap count="5">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -2711,6 +2720,71 @@
 
 <file path=xl/revisions/revisionLog1.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac"/>
+</file>
+
+<file path=xl/revisions/revisionLog2.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1" sId="3" odxf="1" dxf="1">
+    <oc r="W15" t="inlineStr">
+      <is>
+        <t>New image from binary</t>
+      </is>
+    </oc>
+    <nc r="W15"/>
+    <odxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </odxf>
+    <ndxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="8" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </ndxf>
+  </rcc>
+  <rfmt sheetId="4" sqref="W18" start="0" length="0">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79995117038483843"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </rfmt>
+  <rcc rId="2" sId="4">
+    <nc r="W18" t="inlineStr">
+      <is>
+        <t>New image from spec list</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="3" sId="4" odxf="1" dxf="1">
+    <oc r="W15" t="inlineStr">
+      <is>
+        <t>New image from binary</t>
+      </is>
+    </oc>
+    <nc r="W15"/>
+    <odxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </odxf>
+    <ndxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="8" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </ndxf>
+  </rcc>
+</revisions>
 </file>
 
 <file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5601,7 +5675,7 @@
   <dimension ref="B3:AB26"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="W21" sqref="W21"/>
+      <selection activeCell="V17" sqref="V17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -6225,9 +6299,7 @@
       <c r="T15" s="24"/>
       <c r="U15" s="24"/>
       <c r="V15" s="24"/>
-      <c r="W15" s="26" t="s">
-        <v>152</v>
-      </c>
+      <c r="W15" s="24"/>
       <c r="X15" s="24"/>
       <c r="Y15" s="24"/>
     </row>
@@ -6240,7 +6312,7 @@
       <c r="E16" s="24"/>
       <c r="F16" s="24"/>
       <c r="G16" s="26" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="H16" s="23" t="s">
         <v>24</v>
@@ -6255,7 +6327,7 @@
       <c r="L16" s="24"/>
       <c r="M16" s="24"/>
       <c r="N16" s="26" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="O16" s="22"/>
       <c r="P16" s="23" t="s">
@@ -6283,7 +6355,7 @@
         <v>86</v>
       </c>
       <c r="D17" s="23" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E17" s="23" t="s">
         <v>88</v>
@@ -6312,7 +6384,7 @@
         <v>92</v>
       </c>
       <c r="O17" s="23" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="P17" s="22" t="s">
         <v>80</v>
@@ -6330,7 +6402,7 @@
       <c r="W17" s="24"/>
       <c r="X17" s="24"/>
       <c r="Y17" s="26" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="18" spans="2:25" ht="43.5" customHeight="1">
@@ -6339,7 +6411,7 @@
       </c>
       <c r="C18" s="24"/>
       <c r="D18" s="26" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E18" s="24"/>
       <c r="F18" s="24"/>
@@ -6383,7 +6455,7 @@
       <c r="V18" s="24"/>
       <c r="W18" s="24"/>
       <c r="X18" s="26" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="Y18" s="24"/>
     </row>
@@ -6497,14 +6569,14 @@
         <v>109</v>
       </c>
       <c r="R21" s="23" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="S21" s="24"/>
       <c r="T21" s="24"/>
       <c r="U21" s="24"/>
       <c r="V21" s="24"/>
       <c r="W21" s="26" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="X21" s="24"/>
       <c r="Y21" s="24"/>
@@ -6539,7 +6611,7 @@
         <v>112</v>
       </c>
       <c r="R22" s="23" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="S22" s="24"/>
       <c r="T22" s="24"/>
@@ -6613,15 +6685,15 @@
       <c r="L24" s="24"/>
       <c r="M24" s="24"/>
       <c r="N24" s="26" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="O24" s="24"/>
       <c r="P24" s="23" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="Q24" s="24"/>
       <c r="R24" s="23" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="S24" s="24"/>
       <c r="T24" s="24"/>
@@ -6657,11 +6729,11 @@
       <c r="N25" s="24"/>
       <c r="O25" s="24"/>
       <c r="P25" s="23" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="Q25" s="24"/>
       <c r="R25" s="23" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="S25" s="24"/>
       <c r="T25" s="24"/>
@@ -6697,11 +6769,11 @@
       <c r="N26" s="24"/>
       <c r="O26" s="24"/>
       <c r="P26" s="23" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="Q26" s="24"/>
       <c r="R26" s="23" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="S26" s="24"/>
       <c r="T26" s="24"/>
@@ -6731,8 +6803,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:AB26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="W16" sqref="W16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -6879,7 +6951,7 @@
         <v>142</v>
       </c>
       <c r="Y4" s="25" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="AA4" s="22"/>
       <c r="AB4" s="27" t="s">
@@ -6914,25 +6986,25 @@
       <c r="L5" s="24"/>
       <c r="M5" s="24"/>
       <c r="N5" s="25" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="O5" s="24"/>
       <c r="P5" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="Q5" s="25" t="s">
         <v>167</v>
       </c>
-      <c r="Q5" s="25" t="s">
+      <c r="R5" s="25" t="s">
         <v>168</v>
-      </c>
-      <c r="R5" s="25" t="s">
-        <v>169</v>
       </c>
       <c r="S5" s="24"/>
       <c r="T5" s="24"/>
       <c r="U5" s="25" t="s">
+        <v>169</v>
+      </c>
+      <c r="V5" s="25" t="s">
         <v>170</v>
-      </c>
-      <c r="V5" s="25" t="s">
-        <v>171</v>
       </c>
       <c r="W5" s="24"/>
       <c r="X5" s="26" t="s">
@@ -7338,9 +7410,7 @@
       <c r="T15" s="24"/>
       <c r="U15" s="24"/>
       <c r="V15" s="24"/>
-      <c r="W15" s="26" t="s">
-        <v>152</v>
-      </c>
+      <c r="W15" s="24"/>
       <c r="X15" s="24"/>
       <c r="Y15" s="24"/>
     </row>
@@ -7353,7 +7423,7 @@
       <c r="E16" s="24"/>
       <c r="F16" s="24"/>
       <c r="G16" s="26" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="H16" s="23" t="s">
         <v>24</v>
@@ -7368,7 +7438,7 @@
       <c r="L16" s="24"/>
       <c r="M16" s="24"/>
       <c r="N16" s="26" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="O16" s="22"/>
       <c r="P16" s="23" t="s">
@@ -7392,7 +7462,7 @@
         <v>86</v>
       </c>
       <c r="D17" s="23" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E17" s="23" t="s">
         <v>88</v>
@@ -7421,7 +7491,7 @@
         <v>92</v>
       </c>
       <c r="O17" s="23" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="P17" s="22" t="s">
         <v>80</v>
@@ -7439,7 +7509,7 @@
       <c r="W17" s="24"/>
       <c r="X17" s="24"/>
       <c r="Y17" s="26" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="18" spans="2:28" ht="43.5" customHeight="1">
@@ -7448,7 +7518,7 @@
       </c>
       <c r="C18" s="24"/>
       <c r="D18" s="26" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E18" s="24"/>
       <c r="F18" s="24"/>
@@ -7485,7 +7555,7 @@
         <v>101</v>
       </c>
       <c r="S18" s="25" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="T18" s="24"/>
       <c r="U18" s="25" t="s">
@@ -7494,12 +7564,14 @@
       <c r="V18" s="25" t="s">
         <v>136</v>
       </c>
-      <c r="W18" s="24"/>
+      <c r="W18" s="25" t="s">
+        <v>266</v>
+      </c>
       <c r="X18" s="26" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="Y18" s="31" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="19" spans="2:28" ht="43.5" customHeight="1">
@@ -7613,7 +7685,7 @@
       <c r="U21" s="24"/>
       <c r="V21" s="24"/>
       <c r="W21" s="26" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="X21" s="24"/>
       <c r="Y21" s="24"/>
@@ -7729,11 +7801,11 @@
       <c r="L24" s="24"/>
       <c r="M24" s="24"/>
       <c r="N24" s="26" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="O24" s="24"/>
       <c r="P24" s="23" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="Q24" s="24"/>
       <c r="R24" s="25"/>
@@ -7772,7 +7844,7 @@
       <c r="N25" s="24"/>
       <c r="O25" s="24"/>
       <c r="P25" s="23" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="Q25" s="24"/>
       <c r="R25" s="25"/>
@@ -7781,7 +7853,7 @@
       <c r="U25" s="24"/>
       <c r="V25" s="24"/>
       <c r="W25" s="25" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="X25" s="22"/>
       <c r="Y25" s="24"/>
@@ -7810,7 +7882,7 @@
       <c r="N26" s="24"/>
       <c r="O26" s="24"/>
       <c r="P26" s="23" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="Q26" s="24"/>
       <c r="R26" s="25"/>
@@ -7847,8 +7919,8 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -7859,7 +7931,7 @@
   <sheetData>
     <row r="1" spans="1:58" ht="27.95" customHeight="1">
       <c r="A1" s="32" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B1" s="32"/>
       <c r="C1" s="32"/>
@@ -7922,19 +7994,19 @@
     <row r="2" spans="1:58" ht="20.65" customHeight="1">
       <c r="A2" s="2"/>
       <c r="B2" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>178</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>179</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>11</v>
@@ -7943,49 +8015,49 @@
         <v>12</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="K2" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="L2" s="3" t="s">
         <v>181</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>182</v>
       </c>
       <c r="M2" s="3" t="s">
         <v>9</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="O2" s="3" t="s">
         <v>2</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="Q2" s="3" t="s">
         <v>141</v>
       </c>
       <c r="R2" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="S2" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="T2" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="T2" s="3" t="s">
+      <c r="U2" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="U2" s="3" t="s">
+      <c r="V2" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="V2" s="3" t="s">
+      <c r="W2" s="3" t="s">
         <v>189</v>
-      </c>
-      <c r="W2" s="3" t="s">
-        <v>190</v>
       </c>
       <c r="X2" s="3" t="s">
         <v>139</v>
@@ -7994,28 +8066,28 @@
         <v>1</v>
       </c>
       <c r="Z2" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="AA2" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="AA2" s="3" t="s">
+      <c r="AB2" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="AB2" s="3" t="s">
+      <c r="AC2" s="3" t="s">
         <v>193</v>
-      </c>
-      <c r="AC2" s="3" t="s">
-        <v>194</v>
       </c>
       <c r="AD2" s="3" t="s">
         <v>19</v>
       </c>
       <c r="AE2" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="AF2" s="3" t="s">
         <v>7</v>
       </c>
       <c r="AG2" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AH2" s="3" t="s">
         <v>6</v>
@@ -8024,49 +8096,49 @@
         <v>18</v>
       </c>
       <c r="AJ2" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="AK2" s="3" t="s">
         <v>140</v>
       </c>
       <c r="AL2" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="AM2" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="AM2" s="3" t="s">
+      <c r="AN2" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="AN2" s="3" t="s">
+      <c r="AO2" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="AO2" s="3" t="s">
+      <c r="AP2" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="AP2" s="3" t="s">
+      <c r="AQ2" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="AQ2" s="3" t="s">
+      <c r="AR2" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="AR2" s="3" t="s">
+      <c r="AS2" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="AS2" s="3" t="s">
+      <c r="AT2" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="AT2" s="3" t="s">
+      <c r="AU2" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="AU2" s="3" t="s">
+      <c r="AV2" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="AV2" s="3" t="s">
+      <c r="AW2" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="AW2" s="3" t="s">
+      <c r="AX2" s="3" t="s">
         <v>209</v>
-      </c>
-      <c r="AX2" s="3" t="s">
-        <v>210</v>
       </c>
       <c r="AY2" s="3" t="s">
         <v>3</v>
@@ -8081,209 +8153,209 @@
         <v>8</v>
       </c>
       <c r="BC2" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="BD2" s="3" t="s">
         <v>211</v>
-      </c>
-      <c r="BD2" s="3" t="s">
-        <v>212</v>
       </c>
       <c r="BE2" s="3" t="s">
         <v>20</v>
       </c>
       <c r="BF2" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="3" spans="1:58" ht="32.65" customHeight="1">
       <c r="A3" s="33" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="F3" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="G3" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="H3" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="O3" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="P3" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="Q3" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="R3" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="S3" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="T3" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="U3" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="V3" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="W3" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="X3" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="Y3" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="Z3" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="AA3" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="AB3" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="AC3" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="AD3" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="AE3" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="AF3" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="AG3" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="AH3" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="AI3" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="AJ3" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="AK3" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="AL3" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="AM3" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="AN3" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="AO3" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="AP3" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="AQ3" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="AR3" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="AS3" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="AT3" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="AU3" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="AV3" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="AW3" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="AX3" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="AY3" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="AZ3" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="BA3" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="BB3" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="BC3" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="BD3" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="F3" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="H3" s="5" t="s">
+      <c r="BE3" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="BF3" s="5" t="s">
         <v>214</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="K3" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="M3" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="N3" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="O3" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="P3" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="Q3" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="R3" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="S3" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="T3" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="U3" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="V3" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="W3" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="X3" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="Y3" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="Z3" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="AA3" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="AB3" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="AC3" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="AD3" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="AE3" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="AF3" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="AG3" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="AH3" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="AI3" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="AJ3" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="AK3" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="AL3" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="AM3" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="AN3" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="AO3" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="AP3" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="AQ3" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="AR3" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="AS3" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="AT3" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="AU3" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="AV3" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="AW3" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="AX3" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="AY3" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="AZ3" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="BA3" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="BB3" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="BC3" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="BD3" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="BE3" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="BF3" s="5" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="4" spans="1:58" ht="44.45" customHeight="1">
       <c r="A4" s="34"/>
       <c r="B4" s="7"/>
       <c r="C4" s="8" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
       <c r="G4" s="9"/>
       <c r="H4" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="I4" s="8" t="s">
         <v>218</v>
-      </c>
-      <c r="I4" s="8" t="s">
-        <v>219</v>
       </c>
       <c r="J4" s="9"/>
       <c r="K4" s="9"/>
@@ -8292,52 +8364,52 @@
       <c r="N4" s="9"/>
       <c r="O4" s="9"/>
       <c r="P4" s="8" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="Q4" s="9"/>
       <c r="R4" s="8" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="S4" s="9"/>
       <c r="T4" s="9"/>
       <c r="U4" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="V4" s="8" t="s">
         <v>222</v>
-      </c>
-      <c r="V4" s="8" t="s">
-        <v>223</v>
       </c>
       <c r="W4" s="9"/>
       <c r="X4" s="9"/>
       <c r="Y4" s="9"/>
       <c r="Z4" s="9"/>
       <c r="AA4" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="AB4" s="8" t="s">
         <v>224</v>
-      </c>
-      <c r="AB4" s="8" t="s">
-        <v>225</v>
       </c>
       <c r="AC4" s="9"/>
       <c r="AD4" s="9"/>
       <c r="AE4" s="9"/>
       <c r="AF4" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="AG4" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="AH4" s="8" t="s">
         <v>226</v>
-      </c>
-      <c r="AG4" s="8" t="s">
-        <v>226</v>
-      </c>
-      <c r="AH4" s="8" t="s">
-        <v>227</v>
       </c>
       <c r="AI4" s="9"/>
       <c r="AJ4" s="8" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="AK4" s="9"/>
       <c r="AL4" s="8" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="AM4" s="8" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="AN4" s="9"/>
       <c r="AO4" s="9"/>
@@ -8346,24 +8418,24 @@
       <c r="AR4" s="9"/>
       <c r="AS4" s="9"/>
       <c r="AT4" s="8" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="AU4" s="9"/>
       <c r="AV4" s="8" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="AW4" s="9"/>
       <c r="AX4" s="8" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="AY4" s="9"/>
       <c r="AZ4" s="9"/>
       <c r="BA4" s="8" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="BB4" s="9"/>
       <c r="BC4" s="8" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="BD4" s="9"/>
       <c r="BE4" s="9"/>
@@ -8374,175 +8446,175 @@
         <v>1</v>
       </c>
       <c r="B5" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>232</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>233</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>234</v>
+      </c>
+      <c r="J5" s="11" t="s">
+        <v>235</v>
+      </c>
+      <c r="K5" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="L5" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="M5" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="N5" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="O5" s="11" t="s">
+        <v>236</v>
+      </c>
+      <c r="P5" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="Q5" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="R5" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="S5" s="11" t="s">
+        <v>237</v>
+      </c>
+      <c r="T5" s="11" t="s">
+        <v>238</v>
+      </c>
+      <c r="U5" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="V5" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="W5" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="X5" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="Y5" s="11" t="s">
+        <v>239</v>
+      </c>
+      <c r="Z5" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="AA5" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="AB5" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="AC5" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="AD5" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="AE5" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="AF5" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="AG5" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="AH5" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="AI5" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="AJ5" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="AK5" s="11" t="s">
+        <v>240</v>
+      </c>
+      <c r="AL5" s="11" t="s">
+        <v>241</v>
+      </c>
+      <c r="AM5" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="AN5" s="11" t="s">
+        <v>242</v>
+      </c>
+      <c r="AO5" s="11" t="s">
+        <v>243</v>
+      </c>
+      <c r="AP5" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="AQ5" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="AR5" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="AS5" s="11" t="s">
+        <v>244</v>
+      </c>
+      <c r="AT5" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="AU5" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="AV5" s="11" t="s">
+        <v>245</v>
+      </c>
+      <c r="AW5" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="AX5" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="AY5" s="11" t="s">
+        <v>246</v>
+      </c>
+      <c r="AZ5" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="BA5" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="BB5" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="BC5" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="BD5" s="11" t="s">
         <v>215</v>
       </c>
-      <c r="C5" s="11" t="s">
-        <v>215</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>215</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>233</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>234</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>215</v>
-      </c>
-      <c r="H5" s="11" t="s">
+      <c r="BE5" s="11" t="s">
+        <v>247</v>
+      </c>
+      <c r="BF5" s="11" t="s">
         <v>214</v>
-      </c>
-      <c r="I5" s="11" t="s">
-        <v>235</v>
-      </c>
-      <c r="J5" s="11" t="s">
-        <v>236</v>
-      </c>
-      <c r="K5" s="11" t="s">
-        <v>215</v>
-      </c>
-      <c r="L5" s="11" t="s">
-        <v>215</v>
-      </c>
-      <c r="M5" s="11" t="s">
-        <v>215</v>
-      </c>
-      <c r="N5" s="11" t="s">
-        <v>215</v>
-      </c>
-      <c r="O5" s="11" t="s">
-        <v>237</v>
-      </c>
-      <c r="P5" s="11" t="s">
-        <v>214</v>
-      </c>
-      <c r="Q5" s="11" t="s">
-        <v>215</v>
-      </c>
-      <c r="R5" s="11" t="s">
-        <v>214</v>
-      </c>
-      <c r="S5" s="11" t="s">
-        <v>238</v>
-      </c>
-      <c r="T5" s="11" t="s">
-        <v>239</v>
-      </c>
-      <c r="U5" s="11" t="s">
-        <v>215</v>
-      </c>
-      <c r="V5" s="11" t="s">
-        <v>215</v>
-      </c>
-      <c r="W5" s="11" t="s">
-        <v>215</v>
-      </c>
-      <c r="X5" s="11" t="s">
-        <v>215</v>
-      </c>
-      <c r="Y5" s="11" t="s">
-        <v>240</v>
-      </c>
-      <c r="Z5" s="11" t="s">
-        <v>215</v>
-      </c>
-      <c r="AA5" s="11" t="s">
-        <v>214</v>
-      </c>
-      <c r="AB5" s="11" t="s">
-        <v>215</v>
-      </c>
-      <c r="AC5" s="11" t="s">
-        <v>215</v>
-      </c>
-      <c r="AD5" s="11" t="s">
-        <v>215</v>
-      </c>
-      <c r="AE5" s="11" t="s">
-        <v>215</v>
-      </c>
-      <c r="AF5" s="11" t="s">
-        <v>214</v>
-      </c>
-      <c r="AG5" s="11" t="s">
-        <v>215</v>
-      </c>
-      <c r="AH5" s="11" t="s">
-        <v>214</v>
-      </c>
-      <c r="AI5" s="11" t="s">
-        <v>215</v>
-      </c>
-      <c r="AJ5" s="11" t="s">
-        <v>215</v>
-      </c>
-      <c r="AK5" s="11" t="s">
-        <v>241</v>
-      </c>
-      <c r="AL5" s="11" t="s">
-        <v>242</v>
-      </c>
-      <c r="AM5" s="11" t="s">
-        <v>214</v>
-      </c>
-      <c r="AN5" s="11" t="s">
-        <v>243</v>
-      </c>
-      <c r="AO5" s="11" t="s">
-        <v>244</v>
-      </c>
-      <c r="AP5" s="11" t="s">
-        <v>215</v>
-      </c>
-      <c r="AQ5" s="11" t="s">
-        <v>215</v>
-      </c>
-      <c r="AR5" s="11" t="s">
-        <v>215</v>
-      </c>
-      <c r="AS5" s="11" t="s">
-        <v>245</v>
-      </c>
-      <c r="AT5" s="11" t="s">
-        <v>215</v>
-      </c>
-      <c r="AU5" s="11" t="s">
-        <v>215</v>
-      </c>
-      <c r="AV5" s="11" t="s">
-        <v>246</v>
-      </c>
-      <c r="AW5" s="11" t="s">
-        <v>215</v>
-      </c>
-      <c r="AX5" s="11" t="s">
-        <v>214</v>
-      </c>
-      <c r="AY5" s="11" t="s">
-        <v>247</v>
-      </c>
-      <c r="AZ5" s="11" t="s">
-        <v>214</v>
-      </c>
-      <c r="BA5" s="11" t="s">
-        <v>214</v>
-      </c>
-      <c r="BB5" s="11" t="s">
-        <v>215</v>
-      </c>
-      <c r="BC5" s="11" t="s">
-        <v>214</v>
-      </c>
-      <c r="BD5" s="11" t="s">
-        <v>216</v>
-      </c>
-      <c r="BE5" s="11" t="s">
-        <v>248</v>
-      </c>
-      <c r="BF5" s="11" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="6" spans="1:58" ht="68.45" customHeight="1">
@@ -8554,11 +8626,11 @@
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
       <c r="H6" s="8" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="I6" s="8"/>
       <c r="J6" s="8" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="K6" s="9"/>
       <c r="L6" s="9"/>
@@ -8566,11 +8638,11 @@
       <c r="N6" s="9"/>
       <c r="O6" s="9"/>
       <c r="P6" s="8" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="Q6" s="9"/>
       <c r="R6" s="8" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="S6" s="9"/>
       <c r="T6" s="9"/>
@@ -8581,25 +8653,25 @@
       <c r="Y6" s="9"/>
       <c r="Z6" s="9"/>
       <c r="AA6" s="8" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="AB6" s="12"/>
       <c r="AC6" s="9"/>
       <c r="AD6" s="9"/>
       <c r="AE6" s="9"/>
       <c r="AF6" s="8" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="AG6" s="8"/>
       <c r="AH6" s="8" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="AI6" s="9"/>
       <c r="AJ6" s="8"/>
       <c r="AK6" s="9"/>
       <c r="AL6" s="8"/>
       <c r="AM6" s="8" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="AN6" s="9"/>
       <c r="AO6" s="9"/>
@@ -8612,21 +8684,21 @@
       <c r="AV6" s="12"/>
       <c r="AW6" s="9"/>
       <c r="AX6" s="8" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="AY6" s="9"/>
       <c r="AZ6" s="8" t="s">
+        <v>256</v>
+      </c>
+      <c r="BA6" s="8" t="s">
         <v>257</v>
-      </c>
-      <c r="BA6" s="8" t="s">
-        <v>258</v>
       </c>
       <c r="BB6" s="9"/>
       <c r="BC6" s="8" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="BD6" s="8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="BE6" s="9"/>
       <c r="BF6" s="9"/>

</xml_diff>

<commit_message>
FIX: changes any-string! MAKE/TO conversion rules to any-list! and any-path!.
</commit_message>
<xml_diff>
--- a/docs/conversion-matrix.xlsx
+++ b/docs/conversion-matrix.xlsx
@@ -1445,7 +1445,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="959" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="957" uniqueCount="272">
   <si>
     <t>From \ To</t>
   </si>
@@ -2252,6 +2252,21 @@
   </si>
   <si>
     <t>New image from spec list</t>
+  </si>
+  <si>
+    <t>LOAD/ALL to string! binary</t>
+  </si>
+  <si>
+    <t>[binary]</t>
+  </si>
+  <si>
+    <t>[any-string]</t>
+  </si>
+  <si>
+    <t>binary/</t>
+  </si>
+  <si>
+    <t>any-string/</t>
   </si>
 </sst>
 </file>
@@ -2696,7 +2711,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{55E251B5-98E1-4201-A738-B9370268DF37}" diskRevisions="1" revisionId="3" version="2">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{B3DC3AF4-B424-4136-AA1D-EE8CCA86F786}" diskRevisions="1" revisionId="10" version="3">
   <header guid="{9FFB1614-79BA-4BC5-903A-E94B28A6F5C6}" dateTime="2016-11-14T19:29:56" maxSheetId="6" userName="dk" r:id="rId1">
     <sheetIdMap count="5">
       <sheetId val="1"/>
@@ -2707,6 +2722,15 @@
     </sheetIdMap>
   </header>
   <header guid="{55E251B5-98E1-4201-A738-B9370268DF37}" dateTime="2016-11-14T19:36:14" maxSheetId="6" userName="dk" r:id="rId2" minRId="1" maxRId="3">
+    <sheetIdMap count="5">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{B3DC3AF4-B424-4136-AA1D-EE8CCA86F786}" dateTime="2016-11-14T20:06:06" maxSheetId="6" userName="dk" r:id="rId3" minRId="4" maxRId="10">
     <sheetIdMap count="5">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -2780,6 +2804,101 @@
       <fill>
         <patternFill patternType="solid">
           <bgColor theme="8" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </ndxf>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog3.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="4" sId="1">
+    <oc r="Q15" t="inlineStr">
+      <is>
+        <t>LOAD to string! binary</t>
+      </is>
+    </oc>
+    <nc r="Q15" t="inlineStr">
+      <is>
+        <t>LOAD/ALL to string! binary</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="5" sId="3">
+    <oc r="Q15" t="inlineStr">
+      <is>
+        <t>LOAD to string! binary</t>
+      </is>
+    </oc>
+    <nc r="Q15" t="inlineStr">
+      <is>
+        <t>[binary]</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="6" sId="3">
+    <oc r="Q17" t="inlineStr">
+      <is>
+        <t>LOAD string as list</t>
+      </is>
+    </oc>
+    <nc r="Q17" t="inlineStr">
+      <is>
+        <t>[any-string]</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="7" sId="3">
+    <oc r="R15" t="inlineStr">
+      <is>
+        <t>LOAD to string! binary</t>
+      </is>
+    </oc>
+    <nc r="R15" t="inlineStr">
+      <is>
+        <t>binary/</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="8" sId="3">
+    <oc r="R17" t="inlineStr">
+      <is>
+        <t>to path! LOAD string</t>
+      </is>
+    </oc>
+    <nc r="R17" t="inlineStr">
+      <is>
+        <t>any-string/</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="9" sId="4" odxf="1" dxf="1">
+    <oc r="Q17" t="inlineStr">
+      <is>
+        <t>LOAD string as list</t>
+      </is>
+    </oc>
+    <nc r="Q17"/>
+    <ndxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="9" tint="0.79995117038483843"/>
+        </patternFill>
+      </fill>
+    </ndxf>
+  </rcc>
+  <rcc rId="10" sId="4" odxf="1" dxf="1">
+    <oc r="R17" t="inlineStr">
+      <is>
+        <t>to path! LOAD string</t>
+      </is>
+    </oc>
+    <nc r="R17"/>
+    <ndxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="9" tint="0.79995117038483843"/>
         </patternFill>
       </fill>
     </ndxf>
@@ -3861,8 +3980,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:Y23"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q22" sqref="Q22:Q23"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q15" sqref="Q15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -4428,7 +4547,7 @@
         <v>81</v>
       </c>
       <c r="Q15" s="23" t="s">
-        <v>82</v>
+        <v>267</v>
       </c>
       <c r="R15" s="23" t="s">
         <v>82</v>
@@ -4780,7 +4899,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:Y23"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="Q22" sqref="Q22:Q23"/>
     </sheetView>
   </sheetViews>
@@ -5675,7 +5794,7 @@
   <dimension ref="B3:AB26"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="V17" sqref="V17"/>
+      <selection activeCell="Q17" sqref="Q17:R17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -6290,10 +6409,10 @@
         <v>81</v>
       </c>
       <c r="Q15" s="23" t="s">
-        <v>82</v>
+        <v>268</v>
       </c>
       <c r="R15" s="23" t="s">
-        <v>82</v>
+        <v>270</v>
       </c>
       <c r="S15" s="24"/>
       <c r="T15" s="24"/>
@@ -6390,10 +6509,10 @@
         <v>80</v>
       </c>
       <c r="Q17" s="23" t="s">
-        <v>94</v>
+        <v>269</v>
       </c>
       <c r="R17" s="23" t="s">
-        <v>95</v>
+        <v>271</v>
       </c>
       <c r="S17" s="24"/>
       <c r="T17" s="24"/>
@@ -6804,7 +6923,7 @@
   <dimension ref="B3:AB26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="W16" sqref="W16"/>
+      <selection activeCell="S15" sqref="S15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -7496,12 +7615,8 @@
       <c r="P17" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="Q17" s="23" t="s">
-        <v>94</v>
-      </c>
-      <c r="R17" s="23" t="s">
-        <v>95</v>
-      </c>
+      <c r="Q17" s="25"/>
+      <c r="R17" s="25"/>
       <c r="S17" s="24"/>
       <c r="T17" s="24"/>
       <c r="U17" s="24"/>

</xml_diff>

<commit_message>
FEAT: adds TO pair! conversion and better handling MAKE image! action
</commit_message>
<xml_diff>
--- a/docs/conversion-matrix.xlsx
+++ b/docs/conversion-matrix.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28365" windowHeight="13845" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28365" windowHeight="13845" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="R3 TO matrix" sheetId="1" r:id="rId1"/>
@@ -15,6 +15,7 @@
   </sheets>
   <calcPr calcId="144525"/>
   <customWorkbookViews>
+    <customWorkbookView name="hnxxw - 个人视图" guid="{DC067ED4-8354-4BAD-AB55-4C7D933385E9}" mergeInterval="0" personalView="1" maximized="1" xWindow="1" yWindow="1" windowWidth="1920" windowHeight="1060" activeSheetId="3"/>
     <customWorkbookView name="dk - Personal View" guid="{DC8FA253-E57B-4689-B148-2145DC64729C}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1920" windowHeight="1063" activeSheetId="4"/>
   </customWorkbookViews>
 </workbook>
@@ -93,7 +94,7 @@
             <b/>
             <sz val="8"/>
             <rFont val="Tahoma"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t>dk:</t>
         </r>
@@ -101,7 +102,7 @@
           <rPr>
             <sz val="8"/>
             <rFont val="Tahoma"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -110,7 +111,7 @@
           <rPr>
             <sz val="8"/>
             <rFont val="Tahoma"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">In R2:
 </t>
@@ -119,7 +120,7 @@
           <rPr>
             <sz val="8"/>
             <rFont val="Tahoma"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">&lt;&gt; 0 =&gt; TRUE
 </t>
@@ -128,7 +129,7 @@
           <rPr>
             <sz val="8"/>
             <rFont val="Tahoma"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">0 =&gt; FALSE
 </t>
@@ -204,7 +205,7 @@
             <b/>
             <sz val="8"/>
             <rFont val="Tahoma"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t>dk:</t>
         </r>
@@ -212,7 +213,7 @@
           <rPr>
             <sz val="8"/>
             <rFont val="Tahoma"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -221,7 +222,7 @@
           <rPr>
             <sz val="8"/>
             <rFont val="Tahoma"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">In R2:
 </t>
@@ -230,7 +231,7 @@
           <rPr>
             <sz val="8"/>
             <rFont val="Tahoma"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">TRUE =&gt; 1
 </t>
@@ -239,7 +240,7 @@
           <rPr>
             <sz val="8"/>
             <rFont val="Tahoma"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> FALSE =&gt; 0
 </t>
@@ -478,7 +479,7 @@
             <b/>
             <sz val="8"/>
             <rFont val="Tahoma"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t>dk:</t>
         </r>
@@ -486,7 +487,7 @@
           <rPr>
             <sz val="8"/>
             <rFont val="Tahoma"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -495,7 +496,7 @@
           <rPr>
             <sz val="8"/>
             <rFont val="Tahoma"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t>Forbidden if empty cell</t>
         </r>
@@ -539,7 +540,7 @@
             <b/>
             <sz val="8"/>
             <rFont val="Tahoma"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t>dk:</t>
         </r>
@@ -547,7 +548,7 @@
           <rPr>
             <sz val="8"/>
             <rFont val="Tahoma"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -556,7 +557,7 @@
           <rPr>
             <sz val="8"/>
             <rFont val="Tahoma"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">R2: empty path
 </t>
@@ -727,7 +728,7 @@
             <b/>
             <sz val="8"/>
             <rFont val="Tahoma"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t>dk:</t>
         </r>
@@ -735,7 +736,7 @@
           <rPr>
             <sz val="8"/>
             <rFont val="Tahoma"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -744,7 +745,7 @@
           <rPr>
             <sz val="8"/>
             <rFont val="Tahoma"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">In R2:
 </t>
@@ -753,7 +754,7 @@
           <rPr>
             <sz val="8"/>
             <rFont val="Tahoma"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">&lt;&gt; 0 =&gt; TRUE
 </t>
@@ -762,7 +763,7 @@
           <rPr>
             <sz val="8"/>
             <rFont val="Tahoma"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">0 =&gt; FALSE
 </t>
@@ -838,7 +839,7 @@
             <b/>
             <sz val="8"/>
             <rFont val="Tahoma"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t>dk:</t>
         </r>
@@ -846,7 +847,7 @@
           <rPr>
             <sz val="8"/>
             <rFont val="Tahoma"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -855,7 +856,7 @@
           <rPr>
             <sz val="8"/>
             <rFont val="Tahoma"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">In R2:
 </t>
@@ -864,7 +865,7 @@
           <rPr>
             <sz val="8"/>
             <rFont val="Tahoma"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">TRUE =&gt; 1
 </t>
@@ -873,7 +874,7 @@
           <rPr>
             <sz val="8"/>
             <rFont val="Tahoma"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> FALSE =&gt; 0
 </t>
@@ -1110,7 +1111,7 @@
             <b/>
             <sz val="8"/>
             <rFont val="Tahoma"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t>dk:</t>
         </r>
@@ -1118,7 +1119,7 @@
           <rPr>
             <sz val="8"/>
             <rFont val="Tahoma"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -1127,7 +1128,7 @@
           <rPr>
             <sz val="8"/>
             <rFont val="Tahoma"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t>Forbidden if empty cell</t>
         </r>
@@ -1171,7 +1172,7 @@
             <b/>
             <sz val="8"/>
             <rFont val="Tahoma"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t>dk:</t>
         </r>
@@ -1179,7 +1180,7 @@
           <rPr>
             <sz val="8"/>
             <rFont val="Tahoma"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -1188,7 +1189,7 @@
           <rPr>
             <sz val="8"/>
             <rFont val="Tahoma"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">R2: empty path
 </t>
@@ -1445,7 +1446,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="957" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="956" uniqueCount="272">
   <si>
     <t>From \ To</t>
   </si>
@@ -2272,8 +2273,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -2284,20 +2285,20 @@
       <sz val="12"/>
       <color indexed="8"/>
       <name val="Helvetica"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
       <color indexed="8"/>
       <name val="Helvetica"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -2314,12 +2315,12 @@
       <b/>
       <sz val="8"/>
       <name val="Tahoma"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
       <name val="Tahoma"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
@@ -2333,6 +2334,11 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="9">
@@ -2630,7 +2636,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0"/>
@@ -2711,7 +2717,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{B3DC3AF4-B424-4136-AA1D-EE8CCA86F786}" diskRevisions="1" revisionId="10" version="3">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" guid="{9A1785F8-EE08-4DBB-8A76-FC5DF3B6DD3D}" diskRevisions="1" revisionId="11" version="4">
   <header guid="{9FFB1614-79BA-4BC5-903A-E94B28A6F5C6}" dateTime="2016-11-14T19:29:56" maxSheetId="6" userName="dk" r:id="rId1">
     <sheetIdMap count="5">
       <sheetId val="1"/>
@@ -2739,10 +2745,33 @@
       <sheetId val="5"/>
     </sheetIdMap>
   </header>
+  <header guid="{9A1785F8-EE08-4DBB-8A76-FC5DF3B6DD3D}" dateTime="2016-11-15T16:14:31" maxSheetId="6" userName="hnxxw" r:id="rId4" minRId="11">
+    <sheetIdMap count="5">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
 <file path=xl/revisions/revisionLog1.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcc rId="11" sId="3">
+    <oc r="X25" t="inlineStr">
+      <is>
+        <t>COPY</t>
+      </is>
+    </oc>
+    <nc r="X25"/>
+  </rcc>
+  <rcv guid="{DC067ED4-8354-4BAD-AB55-4C7D933385E9}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog11.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac"/>
 </file>
 
@@ -2907,7 +2936,7 @@
 </file>
 
 <file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
-<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="0"/>
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3977,7 +4006,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B3:Y23"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
@@ -4883,12 +4912,18 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{DC067ED4-8354-4BAD-AB55-4C7D933385E9}" scale="85">
+      <selection activeCell="Q15" sqref="Q15"/>
+      <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait"/>
+    </customSheetView>
     <customSheetView guid="{DC8FA253-E57B-4689-B148-2145DC64729C}" scale="85" topLeftCell="A10">
       <selection activeCell="Q22" sqref="Q22:Q23"/>
       <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
     </customSheetView>
   </customSheetViews>
+  <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <legacyDrawing r:id="rId1"/>
@@ -4896,7 +4931,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B3:Y23"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
@@ -5777,12 +5812,18 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{DC067ED4-8354-4BAD-AB55-4C7D933385E9}" scale="85">
+      <selection activeCell="Q22" sqref="Q22:Q23"/>
+      <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait"/>
+    </customSheetView>
     <customSheetView guid="{DC8FA253-E57B-4689-B148-2145DC64729C}" scale="85" topLeftCell="A7">
       <selection activeCell="Q22" sqref="Q22:Q23"/>
       <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
     </customSheetView>
   </customSheetViews>
+  <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <legacyDrawing r:id="rId1"/>
@@ -5790,11 +5831,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B3:AB26"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q17" sqref="Q17:R17"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="X25" sqref="X25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -6859,9 +6900,7 @@
       <c r="U25" s="24"/>
       <c r="V25" s="24"/>
       <c r="W25" s="24"/>
-      <c r="X25" s="22" t="s">
-        <v>80</v>
-      </c>
+      <c r="X25" s="22"/>
       <c r="Y25" s="24"/>
     </row>
     <row r="26" spans="2:25" ht="43.5" customHeight="1">
@@ -6906,12 +6945,18 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{DC067ED4-8354-4BAD-AB55-4C7D933385E9}" scale="85" topLeftCell="A10">
+      <selection activeCell="X25" sqref="X25"/>
+      <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait"/>
+    </customSheetView>
     <customSheetView guid="{DC8FA253-E57B-4689-B148-2145DC64729C}" scale="85">
       <selection activeCell="W21" sqref="W21"/>
       <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
     </customSheetView>
   </customSheetViews>
+  <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <legacyDrawing r:id="rId1"/>
@@ -6919,10 +6964,10 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B3:AB26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="S15" sqref="S15"/>
     </sheetView>
   </sheetViews>
@@ -8013,12 +8058,18 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{DC067ED4-8354-4BAD-AB55-4C7D933385E9}" scale="85" topLeftCell="D1">
+      <selection activeCell="S15" sqref="S15"/>
+      <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait"/>
+    </customSheetView>
     <customSheetView guid="{DC8FA253-E57B-4689-B148-2145DC64729C}" scale="85" topLeftCell="A7">
       <selection activeCell="T21" sqref="T21"/>
       <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
     </customSheetView>
   </customSheetViews>
+  <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <legacyDrawing r:id="rId1"/>
@@ -8026,7 +8077,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -9840,6 +9891,15 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{DC067ED4-8354-4BAD-AB55-4C7D933385E9}" showGridLines="0" fitToPage="1">
+      <pane xSplit="1" ySplit="2" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+      <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.27777777777777801" footer="0.27777777777777801"/>
+      <pageSetup orientation="portrait"/>
+      <headerFooter>
+        <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+      </headerFooter>
+    </customSheetView>
     <customSheetView guid="{DC8FA253-E57B-4689-B148-2145DC64729C}" showGridLines="0" fitToPage="1">
       <pane xSplit="1" ySplit="2" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
@@ -9855,6 +9915,7 @@
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="A5:A6"/>
   </mergeCells>
+  <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.27777777777777801" footer="0.27777777777777801"/>
   <pageSetup orientation="portrait"/>
   <headerFooter>

</xml_diff>

<commit_message>
FIX: some issues of TO actions (#2321, #2322, #2323 and #2324)
</commit_message>
<xml_diff>
--- a/docs/conversion-matrix.xlsx
+++ b/docs/conversion-matrix.xlsx
@@ -13,10 +13,10 @@
     <sheet name="Red MAKE matrix" sheetId="4" r:id="rId4"/>
     <sheet name="Sheet 1 - Red Datatype Comparis" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="124519"/>
   <customWorkbookViews>
+    <customWorkbookView name="dk - Personal View" guid="{DC8FA253-E57B-4689-B148-2145DC64729C}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1920" windowHeight="1063" activeSheetId="4"/>
     <customWorkbookView name="hnxxw - 个人视图" guid="{DC067ED4-8354-4BAD-AB55-4C7D933385E9}" mergeInterval="0" personalView="1" maximized="1" xWindow="1" yWindow="1" windowWidth="1920" windowHeight="1060" activeSheetId="3"/>
-    <customWorkbookView name="dk - Personal View" guid="{DC8FA253-E57B-4689-B148-2145DC64729C}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1920" windowHeight="1063" activeSheetId="4"/>
   </customWorkbookViews>
 </workbook>
 </file>
@@ -770,37 +770,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="M4" authorId="0" guid="{E7754DBE-BC8E-4AEA-8683-257400ADB710}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="8"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>dk:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Rounded up to multiple of 8
-</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="C6" authorId="0" guid="{EFED36B3-D103-44D3-8274-F65EC1DC0EA7}">
       <text>
         <r>
@@ -1446,7 +1415,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="956" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="959" uniqueCount="276">
   <si>
     <t>From \ To</t>
   </si>
@@ -2268,6 +2237,22 @@
   </si>
   <si>
     <t>any-string/</t>
+  </si>
+  <si>
+    <t>[function]</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>[image]</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>[pair]</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>[error]</t>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -2717,7 +2702,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" guid="{9A1785F8-EE08-4DBB-8A76-FC5DF3B6DD3D}" diskRevisions="1" revisionId="11" version="4">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" guid="{273594FE-1A83-42F5-99C8-7CA1D7644759}" diskRevisions="1" revisionId="21" version="7">
   <header guid="{9FFB1614-79BA-4BC5-903A-E94B28A6F5C6}" dateTime="2016-11-14T19:29:56" maxSheetId="6" userName="dk" r:id="rId1">
     <sheetIdMap count="5">
       <sheetId val="1"/>
@@ -2754,10 +2739,253 @@
       <sheetId val="5"/>
     </sheetIdMap>
   </header>
+  <header guid="{9CE14BDF-40B6-42DD-B996-5361A4CE930A}" dateTime="2016-11-17T19:58:34" maxSheetId="6" userName="hnxxw" r:id="rId5" minRId="12" maxRId="18">
+    <sheetIdMap count="5">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{444D6E5D-53CE-4089-98AF-D3E50F0A892B}" dateTime="2016-11-17T19:58:50" maxSheetId="6" userName="hnxxw" r:id="rId6" minRId="19" maxRId="20">
+    <sheetIdMap count="5">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{273594FE-1A83-42F5-99C8-7CA1D7644759}" dateTime="2016-11-17T19:59:08" maxSheetId="6" userName="hnxxw" r:id="rId7" minRId="21">
+    <sheetIdMap count="5">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
 <file path=xl/revisions/revisionLog1.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcc rId="21" sId="3" odxf="1" dxf="1">
+    <oc r="M4" t="inlineStr">
+      <is>
+        <t>New bitset with integer slots preallocated</t>
+      </is>
+    </oc>
+    <nc r="M4"/>
+    <odxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </odxf>
+    <ndxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="8" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </ndxf>
+  </rcc>
+  <rcmt sheetId="3" cell="M4" guid="{00000000-0000-0000-0000-000000000000}" action="delete" author="dk"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog11.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac"/>
+</file>
+
+<file path=xl/revisions/revisionLog12.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcc rId="19" sId="3" odxf="1" dxf="1">
+    <oc r="Y17" t="inlineStr">
+      <is>
+        <t>New error! from string (User error)</t>
+      </is>
+    </oc>
+    <nc r="Y17"/>
+    <odxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </odxf>
+    <ndxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="8" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </ndxf>
+  </rcc>
+  <rcc rId="20" sId="3" odxf="1" dxf="1">
+    <oc r="Y26" t="inlineStr">
+      <is>
+        <t>COPY</t>
+      </is>
+    </oc>
+    <nc r="Y26"/>
+    <odxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79995117038483843"/>
+        </patternFill>
+      </fill>
+    </odxf>
+    <ndxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </ndxf>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog121.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcc rId="12" sId="3">
+    <oc r="Q20" t="inlineStr">
+      <is>
+        <t>[function]</t>
+      </is>
+    </oc>
+    <nc r="Q20" t="inlineStr">
+      <is>
+        <t>[function]</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rfmt sheetId="3" sqref="Q24" start="0" length="0">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="3" sqref="Q25" start="0" length="0">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="3" sqref="Q26" start="0" length="0">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </rfmt>
+  <rcc rId="13" sId="3">
+    <nc r="Q24" t="inlineStr">
+      <is>
+        <t>[image]</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="14" sId="3">
+    <nc r="Q25" t="inlineStr">
+      <is>
+        <t>[pair]</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="15" sId="3">
+    <nc r="Q26" t="inlineStr">
+      <is>
+        <t>[error]</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="16" sId="4" odxf="1" dxf="1">
+    <nc r="Q24" t="inlineStr">
+      <is>
+        <t>[image]</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+    <odxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="8" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </odxf>
+    <ndxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </ndxf>
+  </rcc>
+  <rcc rId="17" sId="4" odxf="1" dxf="1">
+    <nc r="Q25" t="inlineStr">
+      <is>
+        <t>[pair]</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+    <odxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="8" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </odxf>
+    <ndxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </ndxf>
+  </rcc>
+  <rcc rId="18" sId="4" odxf="1" dxf="1">
+    <nc r="Q26" t="inlineStr">
+      <is>
+        <t>[error]</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+    <odxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="8" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </odxf>
+    <ndxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </ndxf>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog1211.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <rcc rId="11" sId="3">
     <oc r="X25" t="inlineStr">
@@ -2769,10 +2997,6 @@
   </rcc>
   <rcv guid="{DC067ED4-8354-4BAD-AB55-4C7D933385E9}" action="add"/>
 </revisions>
-</file>
-
-<file path=xl/revisions/revisionLog11.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac"/>
 </file>
 
 <file path=xl/revisions/revisionLog2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4912,13 +5136,13 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{DC067ED4-8354-4BAD-AB55-4C7D933385E9}" scale="85">
-      <selection activeCell="Q15" sqref="Q15"/>
+    <customSheetView guid="{DC8FA253-E57B-4689-B148-2145DC64729C}" scale="85" topLeftCell="A10">
+      <selection activeCell="Q22" sqref="Q22:Q23"/>
       <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
     </customSheetView>
-    <customSheetView guid="{DC8FA253-E57B-4689-B148-2145DC64729C}" scale="85" topLeftCell="A10">
-      <selection activeCell="Q22" sqref="Q22:Q23"/>
+    <customSheetView guid="{DC067ED4-8354-4BAD-AB55-4C7D933385E9}" scale="85">
+      <selection activeCell="Q15" sqref="Q15"/>
       <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
     </customSheetView>
@@ -5812,12 +6036,12 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{DC067ED4-8354-4BAD-AB55-4C7D933385E9}" scale="85">
+    <customSheetView guid="{DC8FA253-E57B-4689-B148-2145DC64729C}" scale="85" topLeftCell="A7">
       <selection activeCell="Q22" sqref="Q22:Q23"/>
       <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
     </customSheetView>
-    <customSheetView guid="{DC8FA253-E57B-4689-B148-2145DC64729C}" scale="85" topLeftCell="A7">
+    <customSheetView guid="{DC067ED4-8354-4BAD-AB55-4C7D933385E9}" scale="85">
       <selection activeCell="Q22" sqref="Q22:Q23"/>
       <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
@@ -5834,8 +6058,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B3:AB26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="X25" sqref="X25"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -5951,9 +6175,7 @@
       </c>
       <c r="K4" s="24"/>
       <c r="L4" s="24"/>
-      <c r="M4" s="23" t="s">
-        <v>26</v>
-      </c>
+      <c r="M4" s="24"/>
       <c r="N4" s="23" t="s">
         <v>27</v>
       </c>
@@ -6561,9 +6783,7 @@
       <c r="V17" s="24"/>
       <c r="W17" s="24"/>
       <c r="X17" s="24"/>
-      <c r="Y17" s="26" t="s">
-        <v>259</v>
-      </c>
+      <c r="Y17" s="24"/>
     </row>
     <row r="18" spans="2:25" ht="43.5" customHeight="1">
       <c r="B18" s="21" t="s">
@@ -6686,7 +6906,7 @@
         <v>105</v>
       </c>
       <c r="Q20" s="23" t="s">
-        <v>106</v>
+        <v>272</v>
       </c>
       <c r="R20" s="23" t="s">
         <v>107</v>
@@ -6851,7 +7071,9 @@
       <c r="P24" s="23" t="s">
         <v>158</v>
       </c>
-      <c r="Q24" s="24"/>
+      <c r="Q24" s="23" t="s">
+        <v>273</v>
+      </c>
       <c r="R24" s="23" t="s">
         <v>159</v>
       </c>
@@ -6891,7 +7113,9 @@
       <c r="P25" s="23" t="s">
         <v>160</v>
       </c>
-      <c r="Q25" s="24"/>
+      <c r="Q25" s="23" t="s">
+        <v>274</v>
+      </c>
       <c r="R25" s="23" t="s">
         <v>161</v>
       </c>
@@ -6929,7 +7153,9 @@
       <c r="P26" s="23" t="s">
         <v>162</v>
       </c>
-      <c r="Q26" s="24"/>
+      <c r="Q26" s="23" t="s">
+        <v>275</v>
+      </c>
       <c r="R26" s="23" t="s">
         <v>163</v>
       </c>
@@ -6939,19 +7165,17 @@
       <c r="V26" s="24"/>
       <c r="W26" s="24"/>
       <c r="X26" s="24"/>
-      <c r="Y26" s="22" t="s">
-        <v>80</v>
-      </c>
+      <c r="Y26" s="24"/>
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{DC067ED4-8354-4BAD-AB55-4C7D933385E9}" scale="85" topLeftCell="A10">
-      <selection activeCell="X25" sqref="X25"/>
+    <customSheetView guid="{DC8FA253-E57B-4689-B148-2145DC64729C}" scale="85">
+      <selection activeCell="W21" sqref="W21"/>
       <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
     </customSheetView>
-    <customSheetView guid="{DC8FA253-E57B-4689-B148-2145DC64729C}" scale="85">
-      <selection activeCell="W21" sqref="W21"/>
+    <customSheetView guid="{DC067ED4-8354-4BAD-AB55-4C7D933385E9}" scale="85" topLeftCell="A10">
+      <selection activeCell="X25" sqref="X25"/>
       <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
     </customSheetView>
@@ -6967,8 +7191,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B3:AB26"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S15" sqref="S15"/>
+    <sheetView topLeftCell="D10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -7967,7 +8191,9 @@
       <c r="P24" s="23" t="s">
         <v>158</v>
       </c>
-      <c r="Q24" s="24"/>
+      <c r="Q24" s="23" t="s">
+        <v>273</v>
+      </c>
       <c r="R24" s="25"/>
       <c r="S24" s="24"/>
       <c r="T24" s="24"/>
@@ -8006,7 +8232,9 @@
       <c r="P25" s="23" t="s">
         <v>160</v>
       </c>
-      <c r="Q25" s="24"/>
+      <c r="Q25" s="23" t="s">
+        <v>274</v>
+      </c>
       <c r="R25" s="25"/>
       <c r="S25" s="24"/>
       <c r="T25" s="24"/>
@@ -8044,7 +8272,9 @@
       <c r="P26" s="23" t="s">
         <v>261</v>
       </c>
-      <c r="Q26" s="24"/>
+      <c r="Q26" s="23" t="s">
+        <v>275</v>
+      </c>
       <c r="R26" s="25"/>
       <c r="S26" s="24"/>
       <c r="T26" s="24"/>
@@ -8058,13 +8288,13 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{DC067ED4-8354-4BAD-AB55-4C7D933385E9}" scale="85" topLeftCell="D1">
-      <selection activeCell="S15" sqref="S15"/>
+    <customSheetView guid="{DC8FA253-E57B-4689-B148-2145DC64729C}" scale="85" topLeftCell="A7">
+      <selection activeCell="T21" sqref="T21"/>
       <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
     </customSheetView>
-    <customSheetView guid="{DC8FA253-E57B-4689-B148-2145DC64729C}" scale="85" topLeftCell="A7">
-      <selection activeCell="T21" sqref="T21"/>
+    <customSheetView guid="{DC067ED4-8354-4BAD-AB55-4C7D933385E9}" scale="85" topLeftCell="D1">
+      <selection activeCell="S15" sqref="S15"/>
       <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
     </customSheetView>
@@ -9891,7 +10121,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{DC067ED4-8354-4BAD-AB55-4C7D933385E9}" showGridLines="0" fitToPage="1">
+    <customSheetView guid="{DC8FA253-E57B-4689-B148-2145DC64729C}" showGridLines="0" fitToPage="1">
       <pane xSplit="1" ySplit="2" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
       <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.27777777777777801" footer="0.27777777777777801"/>
@@ -9900,7 +10130,7 @@
         <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
       </headerFooter>
     </customSheetView>
-    <customSheetView guid="{DC8FA253-E57B-4689-B148-2145DC64729C}" showGridLines="0" fitToPage="1">
+    <customSheetView guid="{DC067ED4-8354-4BAD-AB55-4C7D933385E9}" showGridLines="0" fitToPage="1">
       <pane xSplit="1" ySplit="2" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
       <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.27777777777777801" footer="0.27777777777777801"/>

</xml_diff>

<commit_message>
FIX: issue #2331 (make any-list!/any-path! with a binary value does NOT treat the binary as a number to pre-allocate)
</commit_message>
<xml_diff>
--- a/docs/conversion-matrix.xlsx
+++ b/docs/conversion-matrix.xlsx
@@ -1434,7 +1434,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="957" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="955" uniqueCount="276">
   <si>
     <t>From \ To</t>
   </si>
@@ -2610,6 +2610,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2621,9 +2624,6 @@
     </xf>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2708,7 +2708,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{09654956-726C-4ECA-A9E8-F98CAB2211E6}" diskRevisions="1" revisionId="25" version="9">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{CD3130B6-9ADC-49C9-98E3-C570EBF80E4E}" diskRevisions="1" revisionId="27" version="10">
   <header guid="{9FFB1614-79BA-4BC5-903A-E94B28A6F5C6}" dateTime="2016-11-14T19:29:56" maxSheetId="6" userName="dk" r:id="rId1">
     <sheetIdMap count="5">
       <sheetId val="1"/>
@@ -2790,11 +2790,41 @@
       <sheetId val="5"/>
     </sheetIdMap>
   </header>
+  <header guid="{CD3130B6-9ADC-49C9-98E3-C570EBF80E4E}" dateTime="2016-11-19T00:04:01" maxSheetId="6" userName="dk" r:id="rId10" minRId="26" maxRId="27">
+    <sheetIdMap count="5">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
 <file path=xl/revisions/revisionLog1.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac"/>
+</file>
+
+<file path=xl/revisions/revisionLog10.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="26" sId="4">
+    <oc r="Q15" t="inlineStr">
+      <is>
+        <t>New list with (binary to integer) slots preallocated</t>
+      </is>
+    </oc>
+    <nc r="Q15"/>
+  </rcc>
+  <rcc rId="27" sId="4">
+    <oc r="R15" t="inlineStr">
+      <is>
+        <t>New path with (binary to integer) slots preallocated</t>
+      </is>
+    </oc>
+    <nc r="R15"/>
+  </rcc>
+</revisions>
 </file>
 
 <file path=xl/revisions/revisionLog2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7287,7 +7317,7 @@
   <dimension ref="B3:AB26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="R15" sqref="R15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -7883,12 +7913,8 @@
       <c r="P15" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="Q15" s="25" t="s">
-        <v>133</v>
-      </c>
-      <c r="R15" s="25" t="s">
-        <v>134</v>
-      </c>
+      <c r="Q15" s="25"/>
+      <c r="R15" s="25"/>
       <c r="S15" s="24"/>
       <c r="T15" s="24"/>
       <c r="U15" s="24"/>
@@ -7999,7 +8025,7 @@
       <c r="D18" s="26" t="s">
         <v>161</v>
       </c>
-      <c r="E18" s="36" t="s">
+      <c r="E18" s="32" t="s">
         <v>275</v>
       </c>
       <c r="F18" s="24"/>
@@ -8400,8 +8426,8 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -8411,66 +8437,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:58" ht="27.95" customHeight="1">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="33" t="s">
         <v>189</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="32"/>
-      <c r="O1" s="32"/>
-      <c r="P1" s="32"/>
-      <c r="Q1" s="32"/>
-      <c r="R1" s="32"/>
-      <c r="S1" s="32"/>
-      <c r="T1" s="32"/>
-      <c r="U1" s="32"/>
-      <c r="V1" s="32"/>
-      <c r="W1" s="32"/>
-      <c r="X1" s="32"/>
-      <c r="Y1" s="32"/>
-      <c r="Z1" s="32"/>
-      <c r="AA1" s="32"/>
-      <c r="AB1" s="32"/>
-      <c r="AC1" s="32"/>
-      <c r="AD1" s="32"/>
-      <c r="AE1" s="32"/>
-      <c r="AF1" s="32"/>
-      <c r="AG1" s="32"/>
-      <c r="AH1" s="32"/>
-      <c r="AI1" s="32"/>
-      <c r="AJ1" s="32"/>
-      <c r="AK1" s="32"/>
-      <c r="AL1" s="32"/>
-      <c r="AM1" s="32"/>
-      <c r="AN1" s="32"/>
-      <c r="AO1" s="32"/>
-      <c r="AP1" s="32"/>
-      <c r="AQ1" s="32"/>
-      <c r="AR1" s="32"/>
-      <c r="AS1" s="32"/>
-      <c r="AT1" s="32"/>
-      <c r="AU1" s="32"/>
-      <c r="AV1" s="32"/>
-      <c r="AW1" s="32"/>
-      <c r="AX1" s="32"/>
-      <c r="AY1" s="32"/>
-      <c r="AZ1" s="32"/>
-      <c r="BA1" s="32"/>
-      <c r="BB1" s="32"/>
-      <c r="BC1" s="32"/>
-      <c r="BD1" s="32"/>
-      <c r="BE1" s="32"/>
-      <c r="BF1" s="32"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="33"/>
+      <c r="O1" s="33"/>
+      <c r="P1" s="33"/>
+      <c r="Q1" s="33"/>
+      <c r="R1" s="33"/>
+      <c r="S1" s="33"/>
+      <c r="T1" s="33"/>
+      <c r="U1" s="33"/>
+      <c r="V1" s="33"/>
+      <c r="W1" s="33"/>
+      <c r="X1" s="33"/>
+      <c r="Y1" s="33"/>
+      <c r="Z1" s="33"/>
+      <c r="AA1" s="33"/>
+      <c r="AB1" s="33"/>
+      <c r="AC1" s="33"/>
+      <c r="AD1" s="33"/>
+      <c r="AE1" s="33"/>
+      <c r="AF1" s="33"/>
+      <c r="AG1" s="33"/>
+      <c r="AH1" s="33"/>
+      <c r="AI1" s="33"/>
+      <c r="AJ1" s="33"/>
+      <c r="AK1" s="33"/>
+      <c r="AL1" s="33"/>
+      <c r="AM1" s="33"/>
+      <c r="AN1" s="33"/>
+      <c r="AO1" s="33"/>
+      <c r="AP1" s="33"/>
+      <c r="AQ1" s="33"/>
+      <c r="AR1" s="33"/>
+      <c r="AS1" s="33"/>
+      <c r="AT1" s="33"/>
+      <c r="AU1" s="33"/>
+      <c r="AV1" s="33"/>
+      <c r="AW1" s="33"/>
+      <c r="AX1" s="33"/>
+      <c r="AY1" s="33"/>
+      <c r="AZ1" s="33"/>
+      <c r="BA1" s="33"/>
+      <c r="BB1" s="33"/>
+      <c r="BC1" s="33"/>
+      <c r="BD1" s="33"/>
+      <c r="BE1" s="33"/>
+      <c r="BF1" s="33"/>
     </row>
     <row r="2" spans="1:58" ht="20.65" customHeight="1">
       <c r="A2" s="2"/>
@@ -8647,7 +8673,7 @@
       </c>
     </row>
     <row r="3" spans="1:58" ht="32.65" customHeight="1">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="34" t="s">
         <v>191</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -8823,7 +8849,7 @@
       </c>
     </row>
     <row r="4" spans="1:58" ht="44.45" customHeight="1">
-      <c r="A4" s="34"/>
+      <c r="A4" s="35"/>
       <c r="B4" s="7"/>
       <c r="C4" s="8" t="s">
         <v>232</v>
@@ -8923,7 +8949,7 @@
       <c r="BF4" s="9"/>
     </row>
     <row r="5" spans="1:58" ht="68.45" customHeight="1">
-      <c r="A5" s="35" t="s">
+      <c r="A5" s="36" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="10" t="s">
@@ -9099,7 +9125,7 @@
       </c>
     </row>
     <row r="6" spans="1:58" ht="68.45" customHeight="1">
-      <c r="A6" s="34"/>
+      <c r="A6" s="35"/>
       <c r="B6" s="7"/>
       <c r="C6" s="12"/>
       <c r="D6" s="9"/>

</xml_diff>

<commit_message>
FIX: issue #2389 (`to-error` doesn't work at all)
</commit_message>
<xml_diff>
--- a/docs/conversion-matrix.xlsx
+++ b/docs/conversion-matrix.xlsx
@@ -2709,69 +2709,6 @@
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
 <headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{CD3130B6-9ADC-49C9-98E3-C570EBF80E4E}" diskRevisions="1" revisionId="27" version="10">
-  <header guid="{9FFB1614-79BA-4BC5-903A-E94B28A6F5C6}" dateTime="2016-11-14T19:29:56" maxSheetId="6" userName="dk" r:id="rId1">
-    <sheetIdMap count="5">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-      <sheetId val="4"/>
-      <sheetId val="5"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{55E251B5-98E1-4201-A738-B9370268DF37}" dateTime="2016-11-14T19:36:14" maxSheetId="6" userName="dk" r:id="rId2" minRId="1" maxRId="3">
-    <sheetIdMap count="5">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-      <sheetId val="4"/>
-      <sheetId val="5"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{B3DC3AF4-B424-4136-AA1D-EE8CCA86F786}" dateTime="2016-11-14T20:06:06" maxSheetId="6" userName="dk" r:id="rId3" minRId="4" maxRId="10">
-    <sheetIdMap count="5">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-      <sheetId val="4"/>
-      <sheetId val="5"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{9A1785F8-EE08-4DBB-8A76-FC5DF3B6DD3D}" dateTime="2016-11-15T16:14:31" maxSheetId="6" userName="hnxxw" r:id="rId4" minRId="11">
-    <sheetIdMap count="5">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-      <sheetId val="4"/>
-      <sheetId val="5"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{9CE14BDF-40B6-42DD-B996-5361A4CE930A}" dateTime="2016-11-17T19:58:34" maxSheetId="6" userName="hnxxw" r:id="rId5" minRId="12" maxRId="18">
-    <sheetIdMap count="5">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-      <sheetId val="4"/>
-      <sheetId val="5"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{444D6E5D-53CE-4089-98AF-D3E50F0A892B}" dateTime="2016-11-17T19:58:50" maxSheetId="6" userName="hnxxw" r:id="rId6" minRId="19" maxRId="20">
-    <sheetIdMap count="5">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-      <sheetId val="4"/>
-      <sheetId val="5"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{273594FE-1A83-42F5-99C8-7CA1D7644759}" dateTime="2016-11-17T19:59:08" maxSheetId="6" userName="hnxxw" r:id="rId7" minRId="21">
-    <sheetIdMap count="5">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-      <sheetId val="4"/>
-      <sheetId val="5"/>
-    </sheetIdMap>
-  </header>
   <header guid="{EB7A1191-CBBA-4B45-A8AB-97C58606F627}" dateTime="2016-11-18T10:22:06" maxSheetId="6" userName="qtxie" r:id="rId8" minRId="22" maxRId="24">
     <sheetIdMap count="5">
       <sheetId val="1"/>
@@ -2802,10 +2739,6 @@
 </headers>
 </file>
 
-<file path=xl/revisions/revisionLog1.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac"/>
-</file>
-
 <file path=xl/revisions/revisionLog10.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rcc rId="26" sId="4">
@@ -2824,392 +2757,6 @@
     </oc>
     <nc r="R15"/>
   </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog2.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="1" sId="3" odxf="1" dxf="1">
-    <oc r="W15" t="inlineStr">
-      <is>
-        <t>New image from binary</t>
-      </is>
-    </oc>
-    <nc r="W15"/>
-    <odxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </odxf>
-    <ndxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="8" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </ndxf>
-  </rcc>
-  <rfmt sheetId="4" sqref="W18" start="0" length="0">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79995117038483843"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </rfmt>
-  <rcc rId="2" sId="4">
-    <nc r="W18" t="inlineStr">
-      <is>
-        <t>New image from spec list</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="3" sId="4" odxf="1" dxf="1">
-    <oc r="W15" t="inlineStr">
-      <is>
-        <t>New image from binary</t>
-      </is>
-    </oc>
-    <nc r="W15"/>
-    <odxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </odxf>
-    <ndxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="8" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </ndxf>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog3.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="4" sId="1">
-    <oc r="Q15" t="inlineStr">
-      <is>
-        <t>LOAD to string! binary</t>
-      </is>
-    </oc>
-    <nc r="Q15" t="inlineStr">
-      <is>
-        <t>LOAD/ALL to string! binary</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="5" sId="3">
-    <oc r="Q15" t="inlineStr">
-      <is>
-        <t>LOAD to string! binary</t>
-      </is>
-    </oc>
-    <nc r="Q15" t="inlineStr">
-      <is>
-        <t>[binary]</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="6" sId="3">
-    <oc r="Q17" t="inlineStr">
-      <is>
-        <t>LOAD string as list</t>
-      </is>
-    </oc>
-    <nc r="Q17" t="inlineStr">
-      <is>
-        <t>[any-string]</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="7" sId="3">
-    <oc r="R15" t="inlineStr">
-      <is>
-        <t>LOAD to string! binary</t>
-      </is>
-    </oc>
-    <nc r="R15" t="inlineStr">
-      <is>
-        <t>binary/</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="8" sId="3">
-    <oc r="R17" t="inlineStr">
-      <is>
-        <t>to path! LOAD string</t>
-      </is>
-    </oc>
-    <nc r="R17" t="inlineStr">
-      <is>
-        <t>any-string/</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="9" sId="4" odxf="1" dxf="1">
-    <oc r="Q17" t="inlineStr">
-      <is>
-        <t>LOAD string as list</t>
-      </is>
-    </oc>
-    <nc r="Q17"/>
-    <ndxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="9" tint="0.79995117038483843"/>
-        </patternFill>
-      </fill>
-    </ndxf>
-  </rcc>
-  <rcc rId="10" sId="4" odxf="1" dxf="1">
-    <oc r="R17" t="inlineStr">
-      <is>
-        <t>to path! LOAD string</t>
-      </is>
-    </oc>
-    <nc r="R17"/>
-    <ndxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="9" tint="0.79995117038483843"/>
-        </patternFill>
-      </fill>
-    </ndxf>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog4.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rcc rId="11" sId="3">
-    <oc r="X25" t="inlineStr">
-      <is>
-        <t>COPY</t>
-      </is>
-    </oc>
-    <nc r="X25"/>
-  </rcc>
-  <rcv guid="{DC067ED4-8354-4BAD-AB55-4C7D933385E9}" action="add"/>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog5.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rcc rId="12" sId="3">
-    <oc r="Q20" t="inlineStr">
-      <is>
-        <t>[function]</t>
-      </is>
-    </oc>
-    <nc r="Q20" t="inlineStr">
-      <is>
-        <t>[function]</t>
-        <phoneticPr fontId="0" type="noConversion"/>
-      </is>
-    </nc>
-  </rcc>
-  <rfmt sheetId="3" sqref="Q24" start="0" length="0">
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="3" sqref="Q25" start="0" length="0">
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="3" sqref="Q26" start="0" length="0">
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </rfmt>
-  <rcc rId="13" sId="3">
-    <nc r="Q24" t="inlineStr">
-      <is>
-        <t>[image]</t>
-        <phoneticPr fontId="0" type="noConversion"/>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="14" sId="3">
-    <nc r="Q25" t="inlineStr">
-      <is>
-        <t>[pair]</t>
-        <phoneticPr fontId="0" type="noConversion"/>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="15" sId="3">
-    <nc r="Q26" t="inlineStr">
-      <is>
-        <t>[error]</t>
-        <phoneticPr fontId="0" type="noConversion"/>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="16" sId="4" odxf="1" dxf="1">
-    <nc r="Q24" t="inlineStr">
-      <is>
-        <t>[image]</t>
-        <phoneticPr fontId="0" type="noConversion"/>
-      </is>
-    </nc>
-    <odxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="8" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </odxf>
-    <ndxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </ndxf>
-  </rcc>
-  <rcc rId="17" sId="4" odxf="1" dxf="1">
-    <nc r="Q25" t="inlineStr">
-      <is>
-        <t>[pair]</t>
-        <phoneticPr fontId="0" type="noConversion"/>
-      </is>
-    </nc>
-    <odxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="8" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </odxf>
-    <ndxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </ndxf>
-  </rcc>
-  <rcc rId="18" sId="4" odxf="1" dxf="1">
-    <nc r="Q26" t="inlineStr">
-      <is>
-        <t>[error]</t>
-        <phoneticPr fontId="0" type="noConversion"/>
-      </is>
-    </nc>
-    <odxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="8" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </odxf>
-    <ndxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </ndxf>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog6.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rcc rId="19" sId="3" odxf="1" dxf="1">
-    <oc r="Y17" t="inlineStr">
-      <is>
-        <t>New error! from string (User error)</t>
-      </is>
-    </oc>
-    <nc r="Y17"/>
-    <odxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </odxf>
-    <ndxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="8" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </ndxf>
-  </rcc>
-  <rcc rId="20" sId="3" odxf="1" dxf="1">
-    <oc r="Y26" t="inlineStr">
-      <is>
-        <t>COPY</t>
-      </is>
-    </oc>
-    <nc r="Y26"/>
-    <odxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79995117038483843"/>
-        </patternFill>
-      </fill>
-    </odxf>
-    <ndxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </ndxf>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog7.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rcc rId="21" sId="3" odxf="1" dxf="1">
-    <oc r="M4" t="inlineStr">
-      <is>
-        <t>New bitset with integer slots preallocated</t>
-      </is>
-    </oc>
-    <nc r="M4"/>
-    <odxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </odxf>
-    <ndxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="8" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </ndxf>
-  </rcc>
-  <rcmt sheetId="3" cell="M4" guid="{00000000-0000-0000-0000-000000000000}" action="delete" author="dk"/>
 </revisions>
 </file>
 

</xml_diff>

<commit_message>
FIX: issue #2333 (make/to string! <block> is not compatible with make/to block! <string>)
</commit_message>
<xml_diff>
--- a/docs/conversion-matrix.xlsx
+++ b/docs/conversion-matrix.xlsx
@@ -1434,7 +1434,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="955" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="955" uniqueCount="277">
   <si>
     <t>From \ To</t>
   </si>
@@ -1740,9 +1740,6 @@
     <t>list of compatible values to binary</t>
   </si>
   <si>
-    <t>FORM list</t>
-  </si>
-  <si>
     <t>list values to path</t>
   </si>
   <si>
@@ -2268,6 +2265,12 @@
   </si>
   <si>
     <t>New time from list of parts</t>
+  </si>
+  <si>
+    <t>list of values to path</t>
+  </si>
+  <si>
+    <t>Concatenate each FORMed value</t>
   </si>
 </sst>
 </file>
@@ -2708,7 +2711,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{CD3130B6-9ADC-49C9-98E3-C570EBF80E4E}" diskRevisions="1" revisionId="27" version="10">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{D2638271-76ED-4E5F-AB9C-525B8411A55F}" diskRevisions="1" revisionId="33" version="11">
   <header guid="{EB7A1191-CBBA-4B45-A8AB-97C58606F627}" dateTime="2016-11-18T10:22:06" maxSheetId="6" userName="qtxie" r:id="rId8" minRId="22" maxRId="24">
     <sheetIdMap count="5">
       <sheetId val="1"/>
@@ -2736,7 +2739,93 @@
       <sheetId val="5"/>
     </sheetIdMap>
   </header>
+  <header guid="{D2638271-76ED-4E5F-AB9C-525B8411A55F}" dateTime="2017-02-20T18:58:13" maxSheetId="6" userName="dk" r:id="rId11" minRId="28" maxRId="33">
+    <sheetIdMap count="5">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+    </sheetIdMap>
+  </header>
 </headers>
+</file>
+
+<file path=xl/revisions/revisionLog1.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="28" sId="3">
+    <oc r="R18" t="inlineStr">
+      <is>
+        <t>list values to path</t>
+      </is>
+    </oc>
+    <nc r="R18" t="inlineStr">
+      <is>
+        <t>list of values to path</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="29" sId="4">
+    <oc r="R18" t="inlineStr">
+      <is>
+        <t>list values to path</t>
+      </is>
+    </oc>
+    <nc r="R18" t="inlineStr">
+      <is>
+        <t>list of values to path</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="30" sId="1">
+    <oc r="P18" t="inlineStr">
+      <is>
+        <t>FORM list</t>
+      </is>
+    </oc>
+    <nc r="P18" t="inlineStr">
+      <is>
+        <t>Concatenate each FORMed value</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="31" sId="2">
+    <oc r="P18" t="inlineStr">
+      <is>
+        <t>FORM list</t>
+      </is>
+    </oc>
+    <nc r="P18" t="inlineStr">
+      <is>
+        <t>Concatenate each FORMed value</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="32" sId="3">
+    <oc r="P18" t="inlineStr">
+      <is>
+        <t>FORM list</t>
+      </is>
+    </oc>
+    <nc r="P18" t="inlineStr">
+      <is>
+        <t>Concatenate each FORMed value</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="33" sId="4">
+    <oc r="P18" t="inlineStr">
+      <is>
+        <t>FORM list</t>
+      </is>
+    </oc>
+    <nc r="P18" t="inlineStr">
+      <is>
+        <t>Concatenate each FORMed value</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
 </file>
 
 <file path=xl/revisions/revisionLog10.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3924,7 +4013,7 @@
   <dimension ref="B3:Y23"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q15" sqref="Q15"/>
+      <selection activeCell="P18" sqref="P18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -4622,18 +4711,18 @@
       </c>
       <c r="O18" s="24"/>
       <c r="P18" s="23" t="s">
-        <v>101</v>
+        <v>276</v>
       </c>
       <c r="Q18" s="22" t="s">
         <v>80</v>
       </c>
       <c r="R18" s="23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="S18" s="24"/>
       <c r="T18" s="24"/>
       <c r="U18" s="26" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="V18" s="24"/>
     </row>
@@ -4661,10 +4750,10 @@
       <c r="N19" s="24"/>
       <c r="O19" s="24"/>
       <c r="P19" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q19" s="23" t="s">
         <v>104</v>
-      </c>
-      <c r="Q19" s="23" t="s">
-        <v>105</v>
       </c>
       <c r="R19" s="22" t="s">
         <v>80</v>
@@ -4698,13 +4787,13 @@
       <c r="N20" s="24"/>
       <c r="O20" s="24"/>
       <c r="P20" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q20" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="Q20" s="23" t="s">
+      <c r="R20" s="23" t="s">
         <v>107</v>
-      </c>
-      <c r="R20" s="23" t="s">
-        <v>108</v>
       </c>
       <c r="S20" s="24"/>
       <c r="T20" s="24"/>
@@ -4735,13 +4824,13 @@
       <c r="N21" s="24"/>
       <c r="O21" s="24"/>
       <c r="P21" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q21" s="23" t="s">
         <v>109</v>
       </c>
-      <c r="Q21" s="23" t="s">
+      <c r="R21" s="23" t="s">
         <v>110</v>
-      </c>
-      <c r="R21" s="23" t="s">
-        <v>111</v>
       </c>
       <c r="S21" s="24"/>
       <c r="T21" s="24"/>
@@ -4772,13 +4861,13 @@
       <c r="N22" s="24"/>
       <c r="O22" s="24"/>
       <c r="P22" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q22" s="23" t="s">
         <v>112</v>
       </c>
-      <c r="Q22" s="23" t="s">
-        <v>113</v>
-      </c>
       <c r="R22" s="23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="S22" s="24"/>
       <c r="T22" s="24"/>
@@ -4811,13 +4900,13 @@
       <c r="N23" s="24"/>
       <c r="O23" s="24"/>
       <c r="P23" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q23" s="23" t="s">
         <v>114</v>
       </c>
-      <c r="Q23" s="23" t="s">
+      <c r="R23" s="23" t="s">
         <v>115</v>
-      </c>
-      <c r="R23" s="23" t="s">
-        <v>116</v>
       </c>
       <c r="S23" s="24"/>
       <c r="T23" s="24"/>
@@ -4843,7 +4932,7 @@
   <dimension ref="B3:Y23"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q22" sqref="Q22:Q23"/>
+      <selection activeCell="P18" sqref="P18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -4942,7 +5031,7 @@
         <v>24</v>
       </c>
       <c r="I4" s="25" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J4" s="23" t="s">
         <v>25</v>
@@ -4953,25 +5042,25 @@
         <v>26</v>
       </c>
       <c r="N4" s="25" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="O4" s="24"/>
       <c r="P4" s="25" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q4" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="Q4" s="25" t="s">
+      <c r="R4" s="25" t="s">
         <v>120</v>
-      </c>
-      <c r="R4" s="25" t="s">
-        <v>121</v>
       </c>
       <c r="S4" s="24"/>
       <c r="T4" s="24"/>
       <c r="U4" s="25" t="s">
+        <v>121</v>
+      </c>
+      <c r="V4" s="25" t="s">
         <v>122</v>
-      </c>
-      <c r="V4" s="25" t="s">
-        <v>123</v>
       </c>
       <c r="X4" s="22"/>
       <c r="Y4" s="27" t="s">
@@ -4997,7 +5086,7 @@
         <v>24</v>
       </c>
       <c r="I5" s="25" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J5" s="23" t="s">
         <v>25</v>
@@ -5006,25 +5095,25 @@
       <c r="L5" s="24"/>
       <c r="M5" s="24"/>
       <c r="N5" s="25" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="O5" s="24"/>
       <c r="P5" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q5" s="25" t="s">
         <v>126</v>
       </c>
-      <c r="Q5" s="25" t="s">
+      <c r="R5" s="25" t="s">
         <v>127</v>
-      </c>
-      <c r="R5" s="25" t="s">
-        <v>128</v>
       </c>
       <c r="S5" s="24"/>
       <c r="T5" s="24"/>
       <c r="U5" s="25" t="s">
+        <v>128</v>
+      </c>
+      <c r="V5" s="25" t="s">
         <v>129</v>
-      </c>
-      <c r="V5" s="25" t="s">
-        <v>130</v>
       </c>
       <c r="X5" s="24"/>
       <c r="Y5" s="28" t="s">
@@ -5069,7 +5158,7 @@
       <c r="V6" s="24"/>
       <c r="X6" s="29"/>
       <c r="Y6" s="28" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="7" spans="2:25" ht="43.5" customHeight="1">
@@ -5184,7 +5273,7 @@
         <v>7</v>
       </c>
       <c r="C10" s="25" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D10" s="24"/>
       <c r="E10" s="24"/>
@@ -5385,10 +5474,10 @@
         <v>81</v>
       </c>
       <c r="Q15" s="25" t="s">
+        <v>132</v>
+      </c>
+      <c r="R15" s="25" t="s">
         <v>133</v>
-      </c>
-      <c r="R15" s="25" t="s">
-        <v>134</v>
       </c>
       <c r="S15" s="24"/>
       <c r="T15" s="24"/>
@@ -5488,7 +5577,7 @@
       <c r="E18" s="24"/>
       <c r="F18" s="24"/>
       <c r="G18" s="23" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H18" s="23" t="s">
         <v>24</v>
@@ -5511,19 +5600,19 @@
       </c>
       <c r="O18" s="24"/>
       <c r="P18" s="23" t="s">
-        <v>101</v>
+        <v>276</v>
       </c>
       <c r="Q18" s="22"/>
       <c r="R18" s="23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="S18" s="24"/>
       <c r="T18" s="24"/>
       <c r="U18" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="V18" s="25" t="s">
         <v>136</v>
-      </c>
-      <c r="V18" s="25" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="19" spans="2:25" ht="43.5" customHeight="1">
@@ -5550,10 +5639,10 @@
       <c r="N19" s="24"/>
       <c r="O19" s="24"/>
       <c r="P19" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q19" s="23" t="s">
         <v>104</v>
-      </c>
-      <c r="Q19" s="23" t="s">
-        <v>105</v>
       </c>
       <c r="R19" s="22"/>
       <c r="S19" s="24"/>
@@ -5585,7 +5674,7 @@
       <c r="N20" s="24"/>
       <c r="O20" s="24"/>
       <c r="P20" s="23" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="Q20" s="25"/>
       <c r="R20" s="25"/>
@@ -5618,13 +5707,13 @@
       <c r="N21" s="24"/>
       <c r="O21" s="24"/>
       <c r="P21" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q21" s="23" t="s">
         <v>109</v>
       </c>
-      <c r="Q21" s="23" t="s">
+      <c r="R21" s="23" t="s">
         <v>110</v>
-      </c>
-      <c r="R21" s="23" t="s">
-        <v>111</v>
       </c>
       <c r="S21" s="24"/>
       <c r="T21" s="24"/>
@@ -5658,17 +5747,17 @@
       <c r="N22" s="24"/>
       <c r="O22" s="24"/>
       <c r="P22" s="23" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="Q22" s="23" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="R22" s="23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="S22" s="24"/>
       <c r="T22" s="25" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="U22" s="22" t="s">
         <v>80</v>
@@ -5702,13 +5791,13 @@
       <c r="N23" s="24"/>
       <c r="O23" s="24"/>
       <c r="P23" s="23" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="Q23" s="23" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="R23" s="23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="S23" s="24"/>
       <c r="T23" s="24"/>
@@ -5737,7 +5826,7 @@
   <dimension ref="B3:AB26"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -5761,7 +5850,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E3" s="20" t="s">
         <v>3</v>
@@ -5818,13 +5907,13 @@
         <v>20</v>
       </c>
       <c r="W3" s="20" t="s">
+        <v>139</v>
+      </c>
+      <c r="X3" s="20" t="s">
         <v>140</v>
       </c>
-      <c r="X3" s="20" t="s">
+      <c r="Y3" s="20" t="s">
         <v>141</v>
-      </c>
-      <c r="Y3" s="20" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="4" spans="2:28" ht="43.5" customHeight="1">
@@ -5873,7 +5962,7 @@
       <c r="V4" s="24"/>
       <c r="W4" s="24"/>
       <c r="X4" s="26" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="Y4" s="24"/>
       <c r="AA4" s="22"/>
@@ -5883,17 +5972,17 @@
     </row>
     <row r="5" spans="2:28" ht="43.5" customHeight="1">
       <c r="B5" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C5" s="23" t="s">
         <v>32</v>
       </c>
       <c r="D5" s="22"/>
       <c r="E5" s="23" t="s">
+        <v>143</v>
+      </c>
+      <c r="F5" s="23" t="s">
         <v>144</v>
-      </c>
-      <c r="F5" s="23" t="s">
-        <v>145</v>
       </c>
       <c r="G5" s="24"/>
       <c r="H5" s="23" t="s">
@@ -5909,17 +5998,17 @@
       <c r="L5" s="24"/>
       <c r="M5" s="24"/>
       <c r="N5" s="23" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="O5" s="24"/>
       <c r="P5" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="Q5" s="23" t="s">
         <v>147</v>
       </c>
-      <c r="Q5" s="23" t="s">
+      <c r="R5" s="23" t="s">
         <v>148</v>
-      </c>
-      <c r="R5" s="23" t="s">
-        <v>149</v>
       </c>
       <c r="S5" s="24"/>
       <c r="T5" s="24"/>
@@ -5927,7 +6016,7 @@
       <c r="V5" s="24"/>
       <c r="W5" s="24"/>
       <c r="X5" s="26" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="Y5" s="24"/>
       <c r="AA5" s="24"/>
@@ -5987,7 +6076,7 @@
         <v>45</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E7" s="24"/>
       <c r="F7" s="22"/>
@@ -6319,7 +6408,7 @@
         <v>75</v>
       </c>
       <c r="D15" s="23" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E15" s="24"/>
       <c r="F15" s="23" t="s">
@@ -6350,10 +6439,10 @@
         <v>81</v>
       </c>
       <c r="Q15" s="23" t="s">
+        <v>152</v>
+      </c>
+      <c r="R15" s="23" t="s">
         <v>153</v>
-      </c>
-      <c r="R15" s="23" t="s">
-        <v>154</v>
       </c>
       <c r="S15" s="24"/>
       <c r="T15" s="24"/>
@@ -6372,7 +6461,7 @@
       <c r="E16" s="24"/>
       <c r="F16" s="24"/>
       <c r="G16" s="26" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H16" s="23" t="s">
         <v>24</v>
@@ -6387,7 +6476,7 @@
       <c r="L16" s="24"/>
       <c r="M16" s="24"/>
       <c r="N16" s="26" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O16" s="22"/>
       <c r="P16" s="23" t="s">
@@ -6415,7 +6504,7 @@
         <v>87</v>
       </c>
       <c r="D17" s="23" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E17" s="23" t="s">
         <v>89</v>
@@ -6444,16 +6533,16 @@
         <v>93</v>
       </c>
       <c r="O17" s="23" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="P17" s="22" t="s">
         <v>80</v>
       </c>
       <c r="Q17" s="23" t="s">
+        <v>158</v>
+      </c>
+      <c r="R17" s="23" t="s">
         <v>159</v>
-      </c>
-      <c r="R17" s="23" t="s">
-        <v>160</v>
       </c>
       <c r="S17" s="24"/>
       <c r="T17" s="24"/>
@@ -6469,12 +6558,12 @@
       </c>
       <c r="C18" s="24"/>
       <c r="D18" s="26" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E18" s="24"/>
       <c r="F18" s="24"/>
       <c r="G18" s="23" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H18" s="23" t="s">
         <v>24</v>
@@ -6497,23 +6586,23 @@
       </c>
       <c r="O18" s="24"/>
       <c r="P18" s="23" t="s">
-        <v>101</v>
+        <v>276</v>
       </c>
       <c r="Q18" s="22" t="s">
         <v>80</v>
       </c>
       <c r="R18" s="23" t="s">
-        <v>102</v>
+        <v>275</v>
       </c>
       <c r="S18" s="24"/>
       <c r="T18" s="24"/>
       <c r="U18" s="26" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="V18" s="24"/>
       <c r="W18" s="24"/>
       <c r="X18" s="26" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="Y18" s="24"/>
     </row>
@@ -6541,10 +6630,10 @@
       <c r="N19" s="24"/>
       <c r="O19" s="24"/>
       <c r="P19" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q19" s="23" t="s">
         <v>104</v>
-      </c>
-      <c r="Q19" s="23" t="s">
-        <v>105</v>
       </c>
       <c r="R19" s="22" t="s">
         <v>80</v>
@@ -6581,13 +6670,13 @@
       <c r="N20" s="24"/>
       <c r="O20" s="24"/>
       <c r="P20" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q20" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="Q20" s="23" t="s">
+      <c r="R20" s="23" t="s">
         <v>107</v>
-      </c>
-      <c r="R20" s="23" t="s">
-        <v>108</v>
       </c>
       <c r="S20" s="24"/>
       <c r="T20" s="24"/>
@@ -6621,20 +6710,20 @@
       <c r="N21" s="24"/>
       <c r="O21" s="24"/>
       <c r="P21" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q21" s="23" t="s">
         <v>109</v>
       </c>
-      <c r="Q21" s="23" t="s">
-        <v>110</v>
-      </c>
       <c r="R21" s="23" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="S21" s="24"/>
       <c r="T21" s="24"/>
       <c r="U21" s="24"/>
       <c r="V21" s="24"/>
       <c r="W21" s="26" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="X21" s="24"/>
       <c r="Y21" s="24"/>
@@ -6663,13 +6752,13 @@
       <c r="N22" s="24"/>
       <c r="O22" s="24"/>
       <c r="P22" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q22" s="23" t="s">
         <v>112</v>
       </c>
-      <c r="Q22" s="23" t="s">
-        <v>113</v>
-      </c>
       <c r="R22" s="23" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="S22" s="24"/>
       <c r="T22" s="24"/>
@@ -6705,13 +6794,13 @@
       <c r="N23" s="24"/>
       <c r="O23" s="24"/>
       <c r="P23" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q23" s="23" t="s">
         <v>114</v>
       </c>
-      <c r="Q23" s="23" t="s">
+      <c r="R23" s="23" t="s">
         <v>115</v>
-      </c>
-      <c r="R23" s="23" t="s">
-        <v>116</v>
       </c>
       <c r="S23" s="24"/>
       <c r="T23" s="24"/>
@@ -6723,7 +6812,7 @@
     </row>
     <row r="24" spans="2:25" ht="43.5" customHeight="1">
       <c r="B24" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C24" s="24"/>
       <c r="D24" s="24"/>
@@ -6743,17 +6832,17 @@
       <c r="L24" s="24"/>
       <c r="M24" s="24"/>
       <c r="N24" s="26" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="O24" s="24"/>
       <c r="P24" s="23" t="s">
+        <v>166</v>
+      </c>
+      <c r="Q24" s="23" t="s">
         <v>167</v>
       </c>
-      <c r="Q24" s="23" t="s">
+      <c r="R24" s="23" t="s">
         <v>168</v>
-      </c>
-      <c r="R24" s="23" t="s">
-        <v>169</v>
       </c>
       <c r="S24" s="24"/>
       <c r="T24" s="24"/>
@@ -6767,7 +6856,7 @@
     </row>
     <row r="25" spans="2:25" ht="43.5" customHeight="1">
       <c r="B25" s="21" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C25" s="24"/>
       <c r="D25" s="24"/>
@@ -6789,13 +6878,13 @@
       <c r="N25" s="24"/>
       <c r="O25" s="24"/>
       <c r="P25" s="23" t="s">
+        <v>169</v>
+      </c>
+      <c r="Q25" s="23" t="s">
         <v>170</v>
       </c>
-      <c r="Q25" s="23" t="s">
+      <c r="R25" s="23" t="s">
         <v>171</v>
-      </c>
-      <c r="R25" s="23" t="s">
-        <v>172</v>
       </c>
       <c r="S25" s="24"/>
       <c r="T25" s="24"/>
@@ -6807,7 +6896,7 @@
     </row>
     <row r="26" spans="2:25" ht="43.5" customHeight="1">
       <c r="B26" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C26" s="24"/>
       <c r="D26" s="24"/>
@@ -6829,13 +6918,13 @@
       <c r="N26" s="24"/>
       <c r="O26" s="24"/>
       <c r="P26" s="23" t="s">
+        <v>172</v>
+      </c>
+      <c r="Q26" s="23" t="s">
         <v>173</v>
       </c>
-      <c r="Q26" s="23" t="s">
+      <c r="R26" s="23" t="s">
         <v>174</v>
-      </c>
-      <c r="R26" s="23" t="s">
-        <v>175</v>
       </c>
       <c r="S26" s="24"/>
       <c r="T26" s="24"/>
@@ -6864,7 +6953,7 @@
   <dimension ref="B3:AB26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="R15" sqref="R15"/>
+      <selection activeCell="Q16" sqref="Q16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -6890,7 +6979,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E3" s="20" t="s">
         <v>3</v>
@@ -6947,13 +7036,13 @@
         <v>20</v>
       </c>
       <c r="W3" s="20" t="s">
+        <v>139</v>
+      </c>
+      <c r="X3" s="20" t="s">
         <v>140</v>
       </c>
-      <c r="X3" s="20" t="s">
+      <c r="Y3" s="20" t="s">
         <v>141</v>
-      </c>
-      <c r="Y3" s="20" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="4" spans="2:28" ht="43.5" customHeight="1">
@@ -6975,7 +7064,7 @@
         <v>24</v>
       </c>
       <c r="I4" s="25" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J4" s="23" t="s">
         <v>25</v>
@@ -6986,32 +7075,32 @@
         <v>26</v>
       </c>
       <c r="N4" s="25" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="O4" s="24"/>
       <c r="P4" s="25" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q4" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="Q4" s="25" t="s">
+      <c r="R4" s="25" t="s">
         <v>120</v>
-      </c>
-      <c r="R4" s="25" t="s">
-        <v>121</v>
       </c>
       <c r="S4" s="24"/>
       <c r="T4" s="24"/>
       <c r="U4" s="25" t="s">
+        <v>121</v>
+      </c>
+      <c r="V4" s="25" t="s">
         <v>122</v>
-      </c>
-      <c r="V4" s="25" t="s">
-        <v>123</v>
       </c>
       <c r="W4" s="24"/>
       <c r="X4" s="26" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="Y4" s="25" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AA4" s="22"/>
       <c r="AB4" s="27" t="s">
@@ -7020,24 +7109,24 @@
     </row>
     <row r="5" spans="2:28" ht="43.5" customHeight="1">
       <c r="B5" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C5" s="23" t="s">
         <v>32</v>
       </c>
       <c r="D5" s="22"/>
       <c r="E5" s="23" t="s">
+        <v>143</v>
+      </c>
+      <c r="F5" s="23" t="s">
         <v>144</v>
-      </c>
-      <c r="F5" s="23" t="s">
-        <v>145</v>
       </c>
       <c r="G5" s="24"/>
       <c r="H5" s="23" t="s">
         <v>24</v>
       </c>
       <c r="I5" s="25" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J5" s="23" t="s">
         <v>25</v>
@@ -7046,29 +7135,29 @@
       <c r="L5" s="24"/>
       <c r="M5" s="24"/>
       <c r="N5" s="25" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="O5" s="24"/>
       <c r="P5" s="25" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q5" s="25" t="s">
         <v>178</v>
       </c>
-      <c r="Q5" s="25" t="s">
+      <c r="R5" s="25" t="s">
         <v>179</v>
-      </c>
-      <c r="R5" s="25" t="s">
-        <v>180</v>
       </c>
       <c r="S5" s="24"/>
       <c r="T5" s="24"/>
       <c r="U5" s="25" t="s">
+        <v>180</v>
+      </c>
+      <c r="V5" s="25" t="s">
         <v>181</v>
-      </c>
-      <c r="V5" s="25" t="s">
-        <v>182</v>
       </c>
       <c r="W5" s="24"/>
       <c r="X5" s="26" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="Y5" s="24"/>
       <c r="AA5" s="24"/>
@@ -7117,7 +7206,7 @@
       <c r="Y6" s="24"/>
       <c r="AA6" s="29"/>
       <c r="AB6" s="28" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="7" spans="2:28" ht="43.5" customHeight="1">
@@ -7128,7 +7217,7 @@
         <v>45</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E7" s="24"/>
       <c r="F7" s="22"/>
@@ -7241,7 +7330,7 @@
         <v>7</v>
       </c>
       <c r="C10" s="25" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D10" s="24"/>
       <c r="E10" s="24"/>
@@ -7430,7 +7519,7 @@
         <v>75</v>
       </c>
       <c r="D15" s="23" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E15" s="24"/>
       <c r="F15" s="23" t="s">
@@ -7479,7 +7568,7 @@
       <c r="E16" s="24"/>
       <c r="F16" s="24"/>
       <c r="G16" s="26" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H16" s="23" t="s">
         <v>24</v>
@@ -7494,7 +7583,7 @@
       <c r="L16" s="24"/>
       <c r="M16" s="24"/>
       <c r="N16" s="26" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O16" s="22"/>
       <c r="P16" s="23" t="s">
@@ -7518,7 +7607,7 @@
         <v>87</v>
       </c>
       <c r="D17" s="23" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E17" s="23" t="s">
         <v>89</v>
@@ -7547,7 +7636,7 @@
         <v>93</v>
       </c>
       <c r="O17" s="23" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="P17" s="22" t="s">
         <v>80</v>
@@ -7561,7 +7650,7 @@
       <c r="W17" s="24"/>
       <c r="X17" s="24"/>
       <c r="Y17" s="26" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="18" spans="2:28" ht="43.5" customHeight="1">
@@ -7570,14 +7659,14 @@
       </c>
       <c r="C18" s="24"/>
       <c r="D18" s="26" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F18" s="24"/>
       <c r="G18" s="23" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H18" s="23" t="s">
         <v>24</v>
@@ -7600,32 +7689,32 @@
       </c>
       <c r="O18" s="24"/>
       <c r="P18" s="23" t="s">
-        <v>101</v>
+        <v>276</v>
       </c>
       <c r="Q18" s="22" t="s">
         <v>80</v>
       </c>
       <c r="R18" s="23" t="s">
-        <v>102</v>
+        <v>275</v>
       </c>
       <c r="S18" s="25" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="T18" s="24"/>
       <c r="U18" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="V18" s="25" t="s">
         <v>136</v>
       </c>
-      <c r="V18" s="25" t="s">
-        <v>137</v>
-      </c>
       <c r="W18" s="25" t="s">
+        <v>184</v>
+      </c>
+      <c r="X18" s="26" t="s">
+        <v>161</v>
+      </c>
+      <c r="Y18" s="30" t="s">
         <v>185</v>
-      </c>
-      <c r="X18" s="26" t="s">
-        <v>162</v>
-      </c>
-      <c r="Y18" s="30" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="19" spans="2:28" ht="43.5" customHeight="1">
@@ -7652,10 +7741,10 @@
       <c r="N19" s="24"/>
       <c r="O19" s="24"/>
       <c r="P19" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q19" s="23" t="s">
         <v>104</v>
-      </c>
-      <c r="Q19" s="23" t="s">
-        <v>105</v>
       </c>
       <c r="R19" s="22" t="s">
         <v>80</v>
@@ -7692,7 +7781,7 @@
       <c r="N20" s="24"/>
       <c r="O20" s="24"/>
       <c r="P20" s="23" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="Q20" s="25"/>
       <c r="R20" s="25"/>
@@ -7728,10 +7817,10 @@
       <c r="N21" s="24"/>
       <c r="O21" s="24"/>
       <c r="P21" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q21" s="23" t="s">
         <v>109</v>
-      </c>
-      <c r="Q21" s="23" t="s">
-        <v>110</v>
       </c>
       <c r="R21" s="25"/>
       <c r="S21" s="24"/>
@@ -7739,7 +7828,7 @@
       <c r="U21" s="24"/>
       <c r="V21" s="24"/>
       <c r="W21" s="26" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="X21" s="24"/>
       <c r="Y21" s="24"/>
@@ -7771,15 +7860,15 @@
       <c r="N22" s="24"/>
       <c r="O22" s="24"/>
       <c r="P22" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q22" s="23" t="s">
         <v>112</v>
-      </c>
-      <c r="Q22" s="23" t="s">
-        <v>113</v>
       </c>
       <c r="R22" s="25"/>
       <c r="S22" s="24"/>
       <c r="T22" s="25" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="U22" s="22" t="s">
         <v>80</v>
@@ -7816,10 +7905,10 @@
       <c r="N23" s="24"/>
       <c r="O23" s="24"/>
       <c r="P23" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q23" s="23" t="s">
         <v>114</v>
-      </c>
-      <c r="Q23" s="23" t="s">
-        <v>115</v>
       </c>
       <c r="R23" s="25"/>
       <c r="S23" s="24"/>
@@ -7835,7 +7924,7 @@
     </row>
     <row r="24" spans="2:28" ht="43.5" customHeight="1">
       <c r="B24" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C24" s="24"/>
       <c r="D24" s="24"/>
@@ -7855,11 +7944,11 @@
       <c r="L24" s="24"/>
       <c r="M24" s="24"/>
       <c r="N24" s="26" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="O24" s="24"/>
       <c r="P24" s="23" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="Q24" s="25"/>
       <c r="R24" s="25"/>
@@ -7876,7 +7965,7 @@
     </row>
     <row r="25" spans="2:28" ht="43.5" customHeight="1">
       <c r="B25" s="21" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C25" s="24"/>
       <c r="D25" s="24"/>
@@ -7898,7 +7987,7 @@
       <c r="N25" s="24"/>
       <c r="O25" s="24"/>
       <c r="P25" s="23" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="Q25" s="25"/>
       <c r="R25" s="25"/>
@@ -7907,14 +7996,14 @@
       <c r="U25" s="24"/>
       <c r="V25" s="24"/>
       <c r="W25" s="25" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="X25" s="22"/>
       <c r="Y25" s="24"/>
     </row>
     <row r="26" spans="2:28" ht="43.5" customHeight="1">
       <c r="B26" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C26" s="24"/>
       <c r="D26" s="24"/>
@@ -7936,7 +8025,7 @@
       <c r="N26" s="24"/>
       <c r="O26" s="24"/>
       <c r="P26" s="23" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="Q26" s="25"/>
       <c r="R26" s="25"/>
@@ -7985,7 +8074,7 @@
   <sheetData>
     <row r="1" spans="1:58" ht="27.95" customHeight="1">
       <c r="A1" s="33" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B1" s="33"/>
       <c r="C1" s="33"/>
@@ -8048,19 +8137,19 @@
     <row r="2" spans="1:58" ht="20.65" customHeight="1">
       <c r="A2" s="2"/>
       <c r="B2" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>193</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>194</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>11</v>
@@ -8069,79 +8158,79 @@
         <v>12</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="K2" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="L2" s="3" t="s">
         <v>196</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>197</v>
       </c>
       <c r="M2" s="3" t="s">
         <v>9</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="O2" s="3" t="s">
         <v>2</v>
       </c>
       <c r="P2" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="R2" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="Q2" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="R2" s="3" t="s">
+      <c r="S2" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="T2" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="T2" s="3" t="s">
+      <c r="U2" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="U2" s="3" t="s">
+      <c r="V2" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="V2" s="3" t="s">
+      <c r="W2" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="W2" s="3" t="s">
-        <v>205</v>
-      </c>
       <c r="X2" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Y2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="Z2" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="AA2" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="AA2" s="3" t="s">
+      <c r="AB2" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="AB2" s="3" t="s">
+      <c r="AC2" s="3" t="s">
         <v>208</v>
-      </c>
-      <c r="AC2" s="3" t="s">
-        <v>209</v>
       </c>
       <c r="AD2" s="3" t="s">
         <v>19</v>
       </c>
       <c r="AE2" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="AF2" s="3" t="s">
         <v>7</v>
       </c>
       <c r="AG2" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="AH2" s="3" t="s">
         <v>6</v>
@@ -8150,49 +8239,49 @@
         <v>18</v>
       </c>
       <c r="AJ2" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="AK2" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="AL2" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="AK2" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="AL2" s="3" t="s">
+      <c r="AM2" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="AM2" s="3" t="s">
+      <c r="AN2" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="AN2" s="3" t="s">
+      <c r="AO2" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="AO2" s="3" t="s">
+      <c r="AP2" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="AP2" s="3" t="s">
+      <c r="AQ2" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="AQ2" s="3" t="s">
+      <c r="AR2" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="AR2" s="3" t="s">
+      <c r="AS2" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="AS2" s="3" t="s">
+      <c r="AT2" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="AT2" s="3" t="s">
+      <c r="AU2" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="AU2" s="3" t="s">
+      <c r="AV2" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="AV2" s="3" t="s">
+      <c r="AW2" s="3" t="s">
         <v>223</v>
       </c>
-      <c r="AW2" s="3" t="s">
+      <c r="AX2" s="3" t="s">
         <v>224</v>
-      </c>
-      <c r="AX2" s="3" t="s">
-        <v>225</v>
       </c>
       <c r="AY2" s="3" t="s">
         <v>3</v>
@@ -8207,209 +8296,209 @@
         <v>8</v>
       </c>
       <c r="BC2" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="BD2" s="3" t="s">
         <v>226</v>
-      </c>
-      <c r="BD2" s="3" t="s">
-        <v>227</v>
       </c>
       <c r="BE2" s="3" t="s">
         <v>20</v>
       </c>
       <c r="BF2" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="3" spans="1:58" ht="32.65" customHeight="1">
       <c r="A3" s="34" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>229</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="F3" s="5" t="s">
         <v>229</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="G3" s="5" t="s">
         <v>229</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="H3" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="O3" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="P3" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q3" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="R3" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="S3" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="T3" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="U3" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="V3" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="W3" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="X3" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="Y3" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="Z3" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="AA3" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="AB3" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="AC3" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="AD3" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="AE3" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="AF3" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="AG3" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="AH3" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="AI3" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="AJ3" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="AK3" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="AL3" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="AM3" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="AN3" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="AO3" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="AP3" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="AQ3" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="AR3" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="AS3" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="AT3" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="AU3" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="AV3" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="AW3" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="AX3" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="AY3" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="AZ3" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="BA3" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="BB3" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="BC3" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="BD3" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="F3" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="H3" s="5" t="s">
+      <c r="BE3" s="5" t="s">
         <v>229</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="BF3" s="5" t="s">
         <v>229</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="K3" s="5" t="s">
-        <v>229</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="M3" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="N3" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="O3" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="P3" s="5" t="s">
-        <v>229</v>
-      </c>
-      <c r="Q3" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="R3" s="5" t="s">
-        <v>229</v>
-      </c>
-      <c r="S3" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="T3" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="U3" s="5" t="s">
-        <v>229</v>
-      </c>
-      <c r="V3" s="5" t="s">
-        <v>229</v>
-      </c>
-      <c r="W3" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="X3" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="Y3" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="Z3" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="AA3" s="5" t="s">
-        <v>229</v>
-      </c>
-      <c r="AB3" s="5" t="s">
-        <v>229</v>
-      </c>
-      <c r="AC3" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="AD3" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="AE3" s="5" t="s">
-        <v>229</v>
-      </c>
-      <c r="AF3" s="5" t="s">
-        <v>229</v>
-      </c>
-      <c r="AG3" s="5" t="s">
-        <v>229</v>
-      </c>
-      <c r="AH3" s="5" t="s">
-        <v>229</v>
-      </c>
-      <c r="AI3" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="AJ3" s="5" t="s">
-        <v>229</v>
-      </c>
-      <c r="AK3" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="AL3" s="5" t="s">
-        <v>229</v>
-      </c>
-      <c r="AM3" s="5" t="s">
-        <v>229</v>
-      </c>
-      <c r="AN3" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="AO3" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="AP3" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="AQ3" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="AR3" s="5" t="s">
-        <v>229</v>
-      </c>
-      <c r="AS3" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="AT3" s="5" t="s">
-        <v>229</v>
-      </c>
-      <c r="AU3" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="AV3" s="5" t="s">
-        <v>229</v>
-      </c>
-      <c r="AW3" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="AX3" s="5" t="s">
-        <v>229</v>
-      </c>
-      <c r="AY3" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="AZ3" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="BA3" s="5" t="s">
-        <v>229</v>
-      </c>
-      <c r="BB3" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="BC3" s="5" t="s">
-        <v>229</v>
-      </c>
-      <c r="BD3" s="5" t="s">
-        <v>231</v>
-      </c>
-      <c r="BE3" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="BF3" s="5" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="4" spans="1:58" ht="44.45" customHeight="1">
       <c r="A4" s="35"/>
       <c r="B4" s="7"/>
       <c r="C4" s="8" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
       <c r="G4" s="9"/>
       <c r="H4" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="I4" s="8" t="s">
         <v>233</v>
-      </c>
-      <c r="I4" s="8" t="s">
-        <v>234</v>
       </c>
       <c r="J4" s="9"/>
       <c r="K4" s="9"/>
@@ -8418,52 +8507,52 @@
       <c r="N4" s="9"/>
       <c r="O4" s="9"/>
       <c r="P4" s="8" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="Q4" s="9"/>
       <c r="R4" s="8" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="S4" s="9"/>
       <c r="T4" s="9"/>
       <c r="U4" s="8" t="s">
+        <v>236</v>
+      </c>
+      <c r="V4" s="8" t="s">
         <v>237</v>
-      </c>
-      <c r="V4" s="8" t="s">
-        <v>238</v>
       </c>
       <c r="W4" s="9"/>
       <c r="X4" s="9"/>
       <c r="Y4" s="9"/>
       <c r="Z4" s="9"/>
       <c r="AA4" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="AB4" s="8" t="s">
         <v>239</v>
-      </c>
-      <c r="AB4" s="8" t="s">
-        <v>240</v>
       </c>
       <c r="AC4" s="9"/>
       <c r="AD4" s="9"/>
       <c r="AE4" s="9"/>
       <c r="AF4" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="AG4" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="AH4" s="8" t="s">
         <v>241</v>
-      </c>
-      <c r="AG4" s="8" t="s">
-        <v>241</v>
-      </c>
-      <c r="AH4" s="8" t="s">
-        <v>242</v>
       </c>
       <c r="AI4" s="9"/>
       <c r="AJ4" s="8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AK4" s="9"/>
       <c r="AL4" s="8" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="AM4" s="8" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="AN4" s="9"/>
       <c r="AO4" s="9"/>
@@ -8472,24 +8561,24 @@
       <c r="AR4" s="9"/>
       <c r="AS4" s="9"/>
       <c r="AT4" s="8" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="AU4" s="9"/>
       <c r="AV4" s="8" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="AW4" s="9"/>
       <c r="AX4" s="8" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="AY4" s="9"/>
       <c r="AZ4" s="9"/>
       <c r="BA4" s="8" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="BB4" s="9"/>
       <c r="BC4" s="8" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="BD4" s="9"/>
       <c r="BE4" s="9"/>
@@ -8500,175 +8589,175 @@
         <v>1</v>
       </c>
       <c r="B5" s="10" t="s">
+        <v>229</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>247</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>248</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>249</v>
+      </c>
+      <c r="J5" s="11" t="s">
+        <v>250</v>
+      </c>
+      <c r="K5" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="L5" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="M5" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="N5" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="O5" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="P5" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q5" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="R5" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="S5" s="11" t="s">
+        <v>252</v>
+      </c>
+      <c r="T5" s="11" t="s">
+        <v>253</v>
+      </c>
+      <c r="U5" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="V5" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="W5" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="X5" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="Y5" s="11" t="s">
+        <v>254</v>
+      </c>
+      <c r="Z5" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="AA5" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="AB5" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="AC5" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="AD5" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="AE5" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="AF5" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="AG5" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="AH5" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="AI5" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="AJ5" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="AK5" s="11" t="s">
+        <v>255</v>
+      </c>
+      <c r="AL5" s="11" t="s">
+        <v>256</v>
+      </c>
+      <c r="AM5" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="AN5" s="11" t="s">
+        <v>257</v>
+      </c>
+      <c r="AO5" s="11" t="s">
+        <v>258</v>
+      </c>
+      <c r="AP5" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="AQ5" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="AR5" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="AS5" s="11" t="s">
+        <v>259</v>
+      </c>
+      <c r="AT5" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="AU5" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="AV5" s="11" t="s">
+        <v>260</v>
+      </c>
+      <c r="AW5" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="AX5" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="AY5" s="11" t="s">
+        <v>261</v>
+      </c>
+      <c r="AZ5" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="BA5" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="BB5" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="BC5" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="BD5" s="11" t="s">
         <v>230</v>
       </c>
-      <c r="C5" s="11" t="s">
-        <v>230</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>230</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>248</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>249</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>230</v>
-      </c>
-      <c r="H5" s="11" t="s">
+      <c r="BE5" s="11" t="s">
+        <v>262</v>
+      </c>
+      <c r="BF5" s="11" t="s">
         <v>229</v>
-      </c>
-      <c r="I5" s="11" t="s">
-        <v>250</v>
-      </c>
-      <c r="J5" s="11" t="s">
-        <v>251</v>
-      </c>
-      <c r="K5" s="11" t="s">
-        <v>230</v>
-      </c>
-      <c r="L5" s="11" t="s">
-        <v>230</v>
-      </c>
-      <c r="M5" s="11" t="s">
-        <v>230</v>
-      </c>
-      <c r="N5" s="11" t="s">
-        <v>230</v>
-      </c>
-      <c r="O5" s="11" t="s">
-        <v>252</v>
-      </c>
-      <c r="P5" s="11" t="s">
-        <v>229</v>
-      </c>
-      <c r="Q5" s="11" t="s">
-        <v>230</v>
-      </c>
-      <c r="R5" s="11" t="s">
-        <v>229</v>
-      </c>
-      <c r="S5" s="11" t="s">
-        <v>253</v>
-      </c>
-      <c r="T5" s="11" t="s">
-        <v>254</v>
-      </c>
-      <c r="U5" s="11" t="s">
-        <v>230</v>
-      </c>
-      <c r="V5" s="11" t="s">
-        <v>230</v>
-      </c>
-      <c r="W5" s="11" t="s">
-        <v>230</v>
-      </c>
-      <c r="X5" s="11" t="s">
-        <v>230</v>
-      </c>
-      <c r="Y5" s="11" t="s">
-        <v>255</v>
-      </c>
-      <c r="Z5" s="11" t="s">
-        <v>230</v>
-      </c>
-      <c r="AA5" s="11" t="s">
-        <v>229</v>
-      </c>
-      <c r="AB5" s="11" t="s">
-        <v>230</v>
-      </c>
-      <c r="AC5" s="11" t="s">
-        <v>230</v>
-      </c>
-      <c r="AD5" s="11" t="s">
-        <v>230</v>
-      </c>
-      <c r="AE5" s="11" t="s">
-        <v>230</v>
-      </c>
-      <c r="AF5" s="11" t="s">
-        <v>229</v>
-      </c>
-      <c r="AG5" s="11" t="s">
-        <v>230</v>
-      </c>
-      <c r="AH5" s="11" t="s">
-        <v>229</v>
-      </c>
-      <c r="AI5" s="11" t="s">
-        <v>230</v>
-      </c>
-      <c r="AJ5" s="11" t="s">
-        <v>230</v>
-      </c>
-      <c r="AK5" s="11" t="s">
-        <v>256</v>
-      </c>
-      <c r="AL5" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="AM5" s="11" t="s">
-        <v>229</v>
-      </c>
-      <c r="AN5" s="11" t="s">
-        <v>258</v>
-      </c>
-      <c r="AO5" s="11" t="s">
-        <v>259</v>
-      </c>
-      <c r="AP5" s="11" t="s">
-        <v>230</v>
-      </c>
-      <c r="AQ5" s="11" t="s">
-        <v>230</v>
-      </c>
-      <c r="AR5" s="11" t="s">
-        <v>230</v>
-      </c>
-      <c r="AS5" s="11" t="s">
-        <v>260</v>
-      </c>
-      <c r="AT5" s="11" t="s">
-        <v>230</v>
-      </c>
-      <c r="AU5" s="11" t="s">
-        <v>230</v>
-      </c>
-      <c r="AV5" s="11" t="s">
-        <v>261</v>
-      </c>
-      <c r="AW5" s="11" t="s">
-        <v>230</v>
-      </c>
-      <c r="AX5" s="11" t="s">
-        <v>229</v>
-      </c>
-      <c r="AY5" s="11" t="s">
-        <v>262</v>
-      </c>
-      <c r="AZ5" s="11" t="s">
-        <v>229</v>
-      </c>
-      <c r="BA5" s="11" t="s">
-        <v>229</v>
-      </c>
-      <c r="BB5" s="11" t="s">
-        <v>230</v>
-      </c>
-      <c r="BC5" s="11" t="s">
-        <v>229</v>
-      </c>
-      <c r="BD5" s="11" t="s">
-        <v>231</v>
-      </c>
-      <c r="BE5" s="11" t="s">
-        <v>263</v>
-      </c>
-      <c r="BF5" s="11" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="6" spans="1:58" ht="68.45" customHeight="1">
@@ -8680,11 +8769,11 @@
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
       <c r="H6" s="8" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="I6" s="8"/>
       <c r="J6" s="8" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="K6" s="9"/>
       <c r="L6" s="9"/>
@@ -8692,11 +8781,11 @@
       <c r="N6" s="9"/>
       <c r="O6" s="9"/>
       <c r="P6" s="8" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="Q6" s="9"/>
       <c r="R6" s="8" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="S6" s="9"/>
       <c r="T6" s="9"/>
@@ -8707,25 +8796,25 @@
       <c r="Y6" s="9"/>
       <c r="Z6" s="9"/>
       <c r="AA6" s="8" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="AB6" s="12"/>
       <c r="AC6" s="9"/>
       <c r="AD6" s="9"/>
       <c r="AE6" s="9"/>
       <c r="AF6" s="8" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="AG6" s="8"/>
       <c r="AH6" s="8" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="AI6" s="9"/>
       <c r="AJ6" s="8"/>
       <c r="AK6" s="9"/>
       <c r="AL6" s="8"/>
       <c r="AM6" s="8" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="AN6" s="9"/>
       <c r="AO6" s="9"/>
@@ -8738,21 +8827,21 @@
       <c r="AV6" s="12"/>
       <c r="AW6" s="9"/>
       <c r="AX6" s="8" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="AY6" s="9"/>
       <c r="AZ6" s="8" t="s">
+        <v>271</v>
+      </c>
+      <c r="BA6" s="8" t="s">
         <v>272</v>
-      </c>
-      <c r="BA6" s="8" t="s">
-        <v>273</v>
       </c>
       <c r="BB6" s="9"/>
       <c r="BC6" s="8" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="BD6" s="8" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="BE6" s="9"/>
       <c r="BF6" s="9"/>

</xml_diff>

<commit_message>
FIX: issue #2339 (make object! from map always gives error, although allowed in the table)
</commit_message>
<xml_diff>
--- a/docs/conversion-matrix.xlsx
+++ b/docs/conversion-matrix.xlsx
@@ -15,7 +15,7 @@
   </sheets>
   <calcPr calcId="144525"/>
   <customWorkbookViews>
-    <customWorkbookView name="dk - Personal View" guid="{6590DA0F-755E-492A-8B86-272A49DB945C}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="1063" activeSheetId="4"/>
+    <customWorkbookView name="dk - Personal View" guid="{6590DA0F-755E-492A-8B86-272A49DB945C}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1920" windowHeight="1063" activeSheetId="4"/>
   </customWorkbookViews>
 </workbook>
 </file>
@@ -1434,7 +1434,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="955" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="954" uniqueCount="277">
   <si>
     <t>From \ To</t>
   </si>
@@ -2711,7 +2711,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{D2638271-76ED-4E5F-AB9C-525B8411A55F}" diskRevisions="1" revisionId="33" version="11">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{45542740-3333-483C-A7A1-17DC71BAE69C}" diskRevisions="1" revisionId="34" version="12">
   <header guid="{EB7A1191-CBBA-4B45-A8AB-97C58606F627}" dateTime="2016-11-18T10:22:06" maxSheetId="6" userName="qtxie" r:id="rId8" minRId="22" maxRId="24">
     <sheetIdMap count="5">
       <sheetId val="1"/>
@@ -2740,6 +2740,15 @@
     </sheetIdMap>
   </header>
   <header guid="{D2638271-76ED-4E5F-AB9C-525B8411A55F}" dateTime="2017-02-20T18:58:13" maxSheetId="6" userName="dk" r:id="rId11" minRId="28" maxRId="33">
+    <sheetIdMap count="5">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{45542740-3333-483C-A7A1-17DC71BAE69C}" dateTime="2017-02-21T16:52:32" maxSheetId="6" userName="dk" r:id="rId12" minRId="34">
     <sheetIdMap count="5">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -2846,6 +2855,35 @@
     </oc>
     <nc r="R15"/>
   </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog2.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="34" sId="4" odxf="1" dxf="1">
+    <oc r="T22" t="inlineStr">
+      <is>
+        <t>New object from map</t>
+      </is>
+    </oc>
+    <nc r="T22"/>
+    <odxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79992065187536243"/>
+        </patternFill>
+      </fill>
+    </odxf>
+    <ndxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </ndxf>
+  </rcc>
+  <rcv guid="{6590DA0F-755E-492A-8B86-272A49DB945C}" action="delete"/>
+  <rcv guid="{6590DA0F-755E-492A-8B86-272A49DB945C}" action="add"/>
 </revisions>
 </file>
 
@@ -4013,7 +4051,7 @@
   <dimension ref="B3:Y23"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P18" sqref="P18"/>
+      <selection activeCell="Q15" sqref="Q15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -4932,7 +4970,7 @@
   <dimension ref="B3:Y23"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P18" sqref="P18"/>
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -5810,7 +5848,7 @@
   </sheetData>
   <customSheetViews>
     <customSheetView guid="{6590DA0F-755E-492A-8B86-272A49DB945C}" scale="85">
-      <selection activeCell="Q22" sqref="Q22:Q23"/>
+      <selection activeCell="K25" sqref="K25"/>
       <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
     </customSheetView>
@@ -5826,7 +5864,7 @@
   <dimension ref="B3:AB26"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P20" sqref="P20"/>
+      <selection activeCell="U18" sqref="U18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -5840,6 +5878,7 @@
     <col min="16" max="16" width="13.7109375" style="18" customWidth="1"/>
     <col min="17" max="18" width="11.85546875" style="18" customWidth="1"/>
     <col min="19" max="25" width="13.28515625" style="18" customWidth="1"/>
+    <col min="28" max="28" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:28" ht="41.25" customHeight="1">
@@ -6937,7 +6976,7 @@
   </sheetData>
   <customSheetViews>
     <customSheetView guid="{6590DA0F-755E-492A-8B86-272A49DB945C}" scale="70">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="U18" sqref="U18"/>
       <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
     </customSheetView>
@@ -6953,7 +6992,7 @@
   <dimension ref="B3:AB26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q16" sqref="Q16"/>
+      <selection activeCell="T20" sqref="T20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -6969,6 +7008,7 @@
     <col min="21" max="21" width="14.7109375" style="18" customWidth="1"/>
     <col min="22" max="22" width="14.28515625" style="18" customWidth="1"/>
     <col min="23" max="25" width="13.28515625" style="18" customWidth="1"/>
+    <col min="28" max="28" width="12" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:28" ht="41.25" customHeight="1">
@@ -7867,9 +7907,7 @@
       </c>
       <c r="R22" s="25"/>
       <c r="S22" s="24"/>
-      <c r="T22" s="25" t="s">
-        <v>137</v>
-      </c>
+      <c r="T22" s="24"/>
       <c r="U22" s="22" t="s">
         <v>80</v>
       </c>
@@ -8042,7 +8080,7 @@
   </sheetData>
   <customSheetViews>
     <customSheetView guid="{6590DA0F-755E-492A-8B86-272A49DB945C}" scale="70">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="T20" sqref="T20"/>
       <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
     </customSheetView>
@@ -8061,7 +8099,7 @@
   <dimension ref="A1:IV23"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
@@ -9869,7 +9907,7 @@
   </sheetData>
   <customSheetViews>
     <customSheetView guid="{6590DA0F-755E-492A-8B86-272A49DB945C}" showGridLines="0" fitToPage="1">
-      <pane xSplit="1" ySplit="2" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
       <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.27777777777777801" footer="0.27777777777777801"/>
       <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
DOCS: updates conversion matrix for `MAKE/TO url! block!` cases.
</commit_message>
<xml_diff>
--- a/docs/conversion-matrix.xlsx
+++ b/docs/conversion-matrix.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr date1904="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28365" windowHeight="13845" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27602" windowHeight="13844" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="R3 TO matrix" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
   </sheets>
   <calcPr calcId="144525"/>
   <customWorkbookViews>
-    <customWorkbookView name="dk - Personal View" guid="{6590DA0F-755E-492A-8B86-272A49DB945C}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1920" windowHeight="1063" activeSheetId="4"/>
+    <customWorkbookView name="dk - Personal View" guid="{6590DA0F-755E-492A-8B86-272A49DB945C}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="1043" activeSheetId="3"/>
   </customWorkbookViews>
 </workbook>
 </file>
@@ -908,6 +908,31 @@
         </r>
       </text>
     </comment>
+    <comment ref="P18" authorId="0" guid="{41B9FE91-F73F-41C9-8911-DBAD2D445727}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>dk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+block! TO url! will concatenate FORMed values and insert adequate separators
+</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="R21" authorId="0">
       <text>
         <r>
@@ -1233,6 +1258,31 @@
         </r>
       </text>
     </comment>
+    <comment ref="P18" authorId="0" guid="{D85D79F8-53BD-4B4A-913C-8BDC4CBFF443}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>dk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+MAKE url! from block! will concatenate FORMed values and insert adequate separators
+</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="R21" authorId="0">
       <text>
         <r>
@@ -2277,7 +2327,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -2324,6 +2374,19 @@
       <sz val="8"/>
       <name val="Tahoma"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="10">
@@ -2711,7 +2774,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{45542740-3333-483C-A7A1-17DC71BAE69C}" diskRevisions="1" revisionId="34" version="12">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{F835C028-ACC9-4CBA-930F-396F34863EC5}" diskRevisions="1" revisionId="34" version="13">
   <header guid="{EB7A1191-CBBA-4B45-A8AB-97C58606F627}" dateTime="2016-11-18T10:22:06" maxSheetId="6" userName="qtxie" r:id="rId8" minRId="22" maxRId="24">
     <sheetIdMap count="5">
       <sheetId val="1"/>
@@ -2749,6 +2812,15 @@
     </sheetIdMap>
   </header>
   <header guid="{45542740-3333-483C-A7A1-17DC71BAE69C}" dateTime="2017-02-21T16:52:32" maxSheetId="6" userName="dk" r:id="rId12" minRId="34">
+    <sheetIdMap count="5">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{F835C028-ACC9-4CBA-930F-396F34863EC5}" dateTime="2017-04-07T23:48:04" maxSheetId="6" userName="dk" r:id="rId13">
     <sheetIdMap count="5">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -2882,6 +2954,15 @@
       </fill>
     </ndxf>
   </rcc>
+  <rcv guid="{6590DA0F-755E-492A-8B86-272A49DB945C}" action="delete"/>
+  <rcv guid="{6590DA0F-755E-492A-8B86-272A49DB945C}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog3.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcmt sheetId="3" cell="P18" guid="{41B9FE91-F73F-41C9-8911-DBAD2D445727}" author="dk" newLength="81"/>
+  <rcmt sheetId="4" cell="P18" guid="{D85D79F8-53BD-4B4A-913C-8BDC4CBFF443}" author="dk" newLength="88"/>
   <rcv guid="{6590DA0F-755E-492A-8B86-272A49DB945C}" action="delete"/>
   <rcv guid="{6590DA0F-755E-492A-8B86-272A49DB945C}" action="add"/>
 </revisions>
@@ -4054,19 +4135,19 @@
       <selection activeCell="Q15" sqref="Q15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.85"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" customWidth="1"/>
-    <col min="3" max="13" width="11.85546875" style="18" customWidth="1"/>
-    <col min="14" max="14" width="13.85546875" style="18" customWidth="1"/>
+    <col min="1" max="1" width="9.375" customWidth="1"/>
+    <col min="2" max="2" width="13.375" customWidth="1"/>
+    <col min="3" max="13" width="11.875" style="18" customWidth="1"/>
+    <col min="14" max="14" width="13.875" style="18" customWidth="1"/>
     <col min="15" max="15" width="14" style="18" customWidth="1"/>
-    <col min="16" max="16" width="13.7109375" style="18" customWidth="1"/>
-    <col min="17" max="18" width="11.85546875" style="18" customWidth="1"/>
-    <col min="19" max="22" width="13.28515625" style="18" customWidth="1"/>
+    <col min="16" max="16" width="13.75" style="18" customWidth="1"/>
+    <col min="17" max="18" width="11.875" style="18" customWidth="1"/>
+    <col min="19" max="22" width="13.25" style="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:25" ht="41.25" customHeight="1">
+    <row r="3" spans="2:25" ht="41.2" customHeight="1">
       <c r="B3" s="19" t="s">
         <v>0</v>
       </c>
@@ -4973,19 +5054,19 @@
       <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.85"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" customWidth="1"/>
-    <col min="3" max="13" width="11.85546875" style="18" customWidth="1"/>
+    <col min="1" max="1" width="9.375" customWidth="1"/>
+    <col min="2" max="2" width="13.375" customWidth="1"/>
+    <col min="3" max="13" width="11.875" style="18" customWidth="1"/>
     <col min="14" max="15" width="14" style="18" customWidth="1"/>
-    <col min="16" max="16" width="13.7109375" style="18" customWidth="1"/>
-    <col min="17" max="17" width="13.28515625" style="18" customWidth="1"/>
-    <col min="18" max="18" width="13.7109375" style="18" customWidth="1"/>
-    <col min="19" max="22" width="13.28515625" style="18" customWidth="1"/>
+    <col min="16" max="16" width="13.75" style="18" customWidth="1"/>
+    <col min="17" max="17" width="13.25" style="18" customWidth="1"/>
+    <col min="18" max="18" width="13.75" style="18" customWidth="1"/>
+    <col min="19" max="22" width="13.25" style="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:25" ht="41.25" customHeight="1">
+    <row r="3" spans="2:25" ht="41.2" customHeight="1">
       <c r="B3" s="19" t="s">
         <v>0</v>
       </c>
@@ -5863,25 +5944,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:AB26"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="U18" sqref="U18"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="S17" sqref="S17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.85"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" customWidth="1"/>
-    <col min="3" max="12" width="11.85546875" style="18" customWidth="1"/>
-    <col min="13" max="13" width="12.140625" style="18" customWidth="1"/>
-    <col min="14" max="14" width="13.85546875" style="18" customWidth="1"/>
+    <col min="1" max="1" width="9.375" customWidth="1"/>
+    <col min="2" max="2" width="13.375" customWidth="1"/>
+    <col min="3" max="12" width="11.875" style="18" customWidth="1"/>
+    <col min="13" max="13" width="12.125" style="18" customWidth="1"/>
+    <col min="14" max="14" width="13.875" style="18" customWidth="1"/>
     <col min="15" max="15" width="14" style="18" customWidth="1"/>
-    <col min="16" max="16" width="13.7109375" style="18" customWidth="1"/>
-    <col min="17" max="18" width="11.85546875" style="18" customWidth="1"/>
-    <col min="19" max="25" width="13.28515625" style="18" customWidth="1"/>
-    <col min="28" max="28" width="11.7109375" customWidth="1"/>
+    <col min="16" max="16" width="13.75" style="18" customWidth="1"/>
+    <col min="17" max="18" width="11.875" style="18" customWidth="1"/>
+    <col min="19" max="25" width="13.25" style="18" customWidth="1"/>
+    <col min="28" max="28" width="11.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:28" ht="41.25" customHeight="1">
+    <row r="3" spans="2:28" ht="41.2" customHeight="1">
       <c r="B3" s="19" t="s">
         <v>0</v>
       </c>
@@ -6976,7 +7057,7 @@
   </sheetData>
   <customSheetViews>
     <customSheetView guid="{6590DA0F-755E-492A-8B86-272A49DB945C}" scale="70">
-      <selection activeCell="U18" sqref="U18"/>
+      <selection activeCell="S17" sqref="S17"/>
       <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
     </customSheetView>
@@ -6991,27 +7072,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:AB26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="T20" sqref="T20"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="R15" sqref="R15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.85"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" customWidth="1"/>
-    <col min="3" max="13" width="11.85546875" style="18" customWidth="1"/>
+    <col min="1" max="1" width="9.375" customWidth="1"/>
+    <col min="2" max="2" width="13.375" customWidth="1"/>
+    <col min="3" max="13" width="11.875" style="18" customWidth="1"/>
     <col min="14" max="15" width="14" style="18" customWidth="1"/>
-    <col min="16" max="16" width="13.7109375" style="18" customWidth="1"/>
-    <col min="17" max="17" width="13.85546875" style="18" customWidth="1"/>
-    <col min="18" max="18" width="13.7109375" style="18" customWidth="1"/>
-    <col min="19" max="20" width="13.28515625" style="18" customWidth="1"/>
-    <col min="21" max="21" width="14.7109375" style="18" customWidth="1"/>
-    <col min="22" max="22" width="14.28515625" style="18" customWidth="1"/>
-    <col min="23" max="25" width="13.28515625" style="18" customWidth="1"/>
+    <col min="16" max="16" width="13.75" style="18" customWidth="1"/>
+    <col min="17" max="17" width="13.875" style="18" customWidth="1"/>
+    <col min="18" max="18" width="13.75" style="18" customWidth="1"/>
+    <col min="19" max="20" width="13.25" style="18" customWidth="1"/>
+    <col min="21" max="21" width="14.75" style="18" customWidth="1"/>
+    <col min="22" max="22" width="14.25" style="18" customWidth="1"/>
+    <col min="23" max="25" width="13.25" style="18" customWidth="1"/>
     <col min="28" max="28" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:28" ht="41.25" customHeight="1">
+    <row r="3" spans="2:28" ht="41.2" customHeight="1">
       <c r="B3" s="19" t="s">
         <v>0</v>
       </c>
@@ -8080,7 +8161,7 @@
   </sheetData>
   <customSheetViews>
     <customSheetView guid="{6590DA0F-755E-492A-8B86-272A49DB945C}" scale="70">
-      <selection activeCell="T20" sqref="T20"/>
+      <selection activeCell="R15" sqref="R15"/>
       <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
     </customSheetView>
@@ -8105,12 +8186,12 @@
       <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="18" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="16.25" defaultRowHeight="18" customHeight="1"/>
   <cols>
-    <col min="1" max="256" width="16.28515625" style="1" customWidth="1"/>
+    <col min="1" max="256" width="16.25" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:58" ht="27.95" customHeight="1">
+    <row r="1" spans="1:58" ht="28" customHeight="1">
       <c r="A1" s="33" t="s">
         <v>188</v>
       </c>
@@ -8172,7 +8253,7 @@
       <c r="BE1" s="33"/>
       <c r="BF1" s="33"/>
     </row>
-    <row r="2" spans="1:58" ht="20.65" customHeight="1">
+    <row r="2" spans="1:58" ht="20.7" customHeight="1">
       <c r="A2" s="2"/>
       <c r="B2" s="3" t="s">
         <v>189</v>
@@ -8522,7 +8603,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="4" spans="1:58" ht="44.45" customHeight="1">
+    <row r="4" spans="1:58" ht="44.4" customHeight="1">
       <c r="A4" s="35"/>
       <c r="B4" s="7"/>
       <c r="C4" s="8" t="s">
@@ -8884,7 +8965,7 @@
       <c r="BE6" s="9"/>
       <c r="BF6" s="9"/>
     </row>
-    <row r="7" spans="1:58" ht="20.45" customHeight="1">
+    <row r="7" spans="1:58" ht="20.5" customHeight="1">
       <c r="A7" s="6"/>
       <c r="B7" s="13"/>
       <c r="C7" s="14"/>
@@ -8944,7 +9025,7 @@
       <c r="BE7" s="14"/>
       <c r="BF7" s="14"/>
     </row>
-    <row r="8" spans="1:58" ht="20.45" customHeight="1">
+    <row r="8" spans="1:58" ht="20.5" customHeight="1">
       <c r="A8" s="6"/>
       <c r="B8" s="15"/>
       <c r="C8" s="16"/>
@@ -9004,7 +9085,7 @@
       <c r="BE8" s="16"/>
       <c r="BF8" s="16"/>
     </row>
-    <row r="9" spans="1:58" ht="20.45" customHeight="1">
+    <row r="9" spans="1:58" ht="20.5" customHeight="1">
       <c r="A9" s="6"/>
       <c r="B9" s="13"/>
       <c r="C9" s="14"/>
@@ -9064,7 +9145,7 @@
       <c r="BE9" s="14"/>
       <c r="BF9" s="14"/>
     </row>
-    <row r="10" spans="1:58" ht="20.45" customHeight="1">
+    <row r="10" spans="1:58" ht="20.5" customHeight="1">
       <c r="A10" s="6"/>
       <c r="B10" s="15"/>
       <c r="C10" s="16"/>
@@ -9124,7 +9205,7 @@
       <c r="BE10" s="16"/>
       <c r="BF10" s="16"/>
     </row>
-    <row r="11" spans="1:58" ht="20.45" customHeight="1">
+    <row r="11" spans="1:58" ht="20.5" customHeight="1">
       <c r="A11" s="6"/>
       <c r="B11" s="13"/>
       <c r="C11" s="14"/>
@@ -9184,7 +9265,7 @@
       <c r="BE11" s="14"/>
       <c r="BF11" s="14"/>
     </row>
-    <row r="12" spans="1:58" ht="20.45" customHeight="1">
+    <row r="12" spans="1:58" ht="20.5" customHeight="1">
       <c r="A12" s="6"/>
       <c r="B12" s="15"/>
       <c r="C12" s="16"/>
@@ -9244,7 +9325,7 @@
       <c r="BE12" s="16"/>
       <c r="BF12" s="16"/>
     </row>
-    <row r="13" spans="1:58" ht="20.45" customHeight="1">
+    <row r="13" spans="1:58" ht="20.5" customHeight="1">
       <c r="A13" s="6"/>
       <c r="B13" s="13"/>
       <c r="C13" s="14"/>
@@ -9304,7 +9385,7 @@
       <c r="BE13" s="14"/>
       <c r="BF13" s="14"/>
     </row>
-    <row r="14" spans="1:58" ht="20.45" customHeight="1">
+    <row r="14" spans="1:58" ht="20.5" customHeight="1">
       <c r="A14" s="6"/>
       <c r="B14" s="15"/>
       <c r="C14" s="16"/>
@@ -9364,7 +9445,7 @@
       <c r="BE14" s="16"/>
       <c r="BF14" s="16"/>
     </row>
-    <row r="15" spans="1:58" ht="20.45" customHeight="1">
+    <row r="15" spans="1:58" ht="20.5" customHeight="1">
       <c r="A15" s="6"/>
       <c r="B15" s="13"/>
       <c r="C15" s="14"/>
@@ -9424,7 +9505,7 @@
       <c r="BE15" s="14"/>
       <c r="BF15" s="14"/>
     </row>
-    <row r="16" spans="1:58" ht="20.45" customHeight="1">
+    <row r="16" spans="1:58" ht="20.5" customHeight="1">
       <c r="A16" s="6"/>
       <c r="B16" s="15"/>
       <c r="C16" s="16"/>
@@ -9484,7 +9565,7 @@
       <c r="BE16" s="16"/>
       <c r="BF16" s="16"/>
     </row>
-    <row r="17" spans="1:58" ht="20.45" customHeight="1">
+    <row r="17" spans="1:58" ht="20.5" customHeight="1">
       <c r="A17" s="6"/>
       <c r="B17" s="13"/>
       <c r="C17" s="14"/>
@@ -9544,7 +9625,7 @@
       <c r="BE17" s="14"/>
       <c r="BF17" s="14"/>
     </row>
-    <row r="18" spans="1:58" ht="20.45" customHeight="1">
+    <row r="18" spans="1:58" ht="20.5" customHeight="1">
       <c r="A18" s="6"/>
       <c r="B18" s="15"/>
       <c r="C18" s="16"/>
@@ -9604,7 +9685,7 @@
       <c r="BE18" s="16"/>
       <c r="BF18" s="16"/>
     </row>
-    <row r="19" spans="1:58" ht="20.45" customHeight="1">
+    <row r="19" spans="1:58" ht="20.5" customHeight="1">
       <c r="A19" s="6"/>
       <c r="B19" s="13"/>
       <c r="C19" s="14"/>
@@ -9664,7 +9745,7 @@
       <c r="BE19" s="14"/>
       <c r="BF19" s="14"/>
     </row>
-    <row r="20" spans="1:58" ht="20.45" customHeight="1">
+    <row r="20" spans="1:58" ht="20.5" customHeight="1">
       <c r="A20" s="6"/>
       <c r="B20" s="15"/>
       <c r="C20" s="16"/>
@@ -9724,7 +9805,7 @@
       <c r="BE20" s="16"/>
       <c r="BF20" s="16"/>
     </row>
-    <row r="21" spans="1:58" ht="20.45" customHeight="1">
+    <row r="21" spans="1:58" ht="20.5" customHeight="1">
       <c r="A21" s="6"/>
       <c r="B21" s="13"/>
       <c r="C21" s="14"/>
@@ -9784,7 +9865,7 @@
       <c r="BE21" s="14"/>
       <c r="BF21" s="14"/>
     </row>
-    <row r="22" spans="1:58" ht="20.45" customHeight="1">
+    <row r="22" spans="1:58" ht="20.5" customHeight="1">
       <c r="A22" s="6"/>
       <c r="B22" s="15"/>
       <c r="C22" s="16"/>
@@ -9844,7 +9925,7 @@
       <c r="BE22" s="16"/>
       <c r="BF22" s="16"/>
     </row>
-    <row r="23" spans="1:58" ht="20.45" customHeight="1">
+    <row r="23" spans="1:58" ht="20.5" customHeight="1">
       <c r="A23" s="17"/>
       <c r="B23" s="13"/>
       <c r="C23" s="14"/>

</xml_diff>

<commit_message>
FIX: issue #2551 (DOC: conversion table omits MAKE object! from any-list! value)
</commit_message>
<xml_diff>
--- a/docs/conversion-matrix.xlsx
+++ b/docs/conversion-matrix.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr date1904="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27602" windowHeight="13844" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27602" windowHeight="13844" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="R3 TO matrix" sheetId="1" r:id="rId1"/>
@@ -1484,7 +1484,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="954" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="955" uniqueCount="278">
   <si>
     <t>From \ To</t>
   </si>
@@ -2321,6 +2321,9 @@
   </si>
   <si>
     <t>Concatenate each FORMed value</t>
+  </si>
+  <si>
+    <t>New object from body block</t>
   </si>
 </sst>
 </file>
@@ -2774,7 +2777,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{F835C028-ACC9-4CBA-930F-396F34863EC5}" diskRevisions="1" revisionId="34" version="13">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{0F1265E3-10D0-4872-A06A-A526B9F48E14}" diskRevisions="1" revisionId="35" version="14">
   <header guid="{EB7A1191-CBBA-4B45-A8AB-97C58606F627}" dateTime="2016-11-18T10:22:06" maxSheetId="6" userName="qtxie" r:id="rId8" minRId="22" maxRId="24">
     <sheetIdMap count="5">
       <sheetId val="1"/>
@@ -2821,6 +2824,15 @@
     </sheetIdMap>
   </header>
   <header guid="{F835C028-ACC9-4CBA-930F-396F34863EC5}" dateTime="2017-04-07T23:48:04" maxSheetId="6" userName="dk" r:id="rId13">
+    <sheetIdMap count="5">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{0F1265E3-10D0-4872-A06A-A526B9F48E14}" dateTime="2017-04-08T23:26:57" maxSheetId="6" userName="dk" r:id="rId14" minRId="35">
     <sheetIdMap count="5">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -2965,6 +2977,27 @@
   <rcmt sheetId="4" cell="P18" guid="{D85D79F8-53BD-4B4A-913C-8BDC4CBFF443}" author="dk" newLength="88"/>
   <rcv guid="{6590DA0F-755E-492A-8B86-272A49DB945C}" action="delete"/>
   <rcv guid="{6590DA0F-755E-492A-8B86-272A49DB945C}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog4.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rfmt sheetId="4" sqref="T18" start="0" length="0">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79992065187536243"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </rfmt>
+  <rcc rId="35" sId="4">
+    <nc r="T18" t="inlineStr">
+      <is>
+        <t>New object from body block</t>
+      </is>
+    </nc>
+  </rcc>
 </revisions>
 </file>
 
@@ -5944,7 +5977,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:AB26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="S17" sqref="S17"/>
     </sheetView>
   </sheetViews>
@@ -7072,8 +7105,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:AB26"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="R15" sqref="R15"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="T19" sqref="T19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.85"/>
@@ -7821,7 +7854,9 @@
       <c r="S18" s="25" t="s">
         <v>183</v>
       </c>
-      <c r="T18" s="24"/>
+      <c r="T18" s="25" t="s">
+        <v>277</v>
+      </c>
       <c r="U18" s="25" t="s">
         <v>135</v>
       </c>

</xml_diff>

<commit_message>
FIX: issue #2566 (Conversion matrices allow make series! any-float!, but compiler disallows percent!)
</commit_message>
<xml_diff>
--- a/docs/conversion-matrix.xlsx
+++ b/docs/conversion-matrix.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr date1904="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27602" windowHeight="13844" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27600" windowHeight="13845" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="R3 TO matrix" sheetId="1" r:id="rId1"/>
@@ -1082,6 +1082,131 @@
         </r>
       </text>
     </comment>
+    <comment ref="P5" authorId="0" guid="{E32332DF-70B0-4158-B7AF-05D28786F79D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>dk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+percent! is not allowed
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Q5" authorId="0" guid="{66C873E2-4441-4BDF-8D81-24C36DB880D1}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>dk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+percent! is not allowed
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="R5" authorId="0" guid="{CE279250-3BDA-4F12-BA21-2E74ED2A8AAA}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>dk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+percent! is not allowed
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="U5" authorId="0" guid="{0B5B29FD-145F-448D-928E-751E40B07634}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>dk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+percent! is not allowed
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="V5" authorId="0" guid="{D0A42E6C-860A-4939-AD1F-BB779E3AEB9B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>dk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+percent! is not allowed
+</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="C6" authorId="0">
       <text>
         <r>
@@ -2022,21 +2147,6 @@
     <t>New binary with truncated any-float slots preallocated</t>
   </si>
   <si>
-    <t>New string with truncated any-float slots preallocated</t>
-  </si>
-  <si>
-    <t>New list with truncated any-float slots preallocated</t>
-  </si>
-  <si>
-    <t>New path with truncated any-float slots preallocated</t>
-  </si>
-  <si>
-    <t>New map with truncated any-float slots preallocated</t>
-  </si>
-  <si>
-    <t>New vector with truncated any-float slots preallocated</t>
-  </si>
-  <si>
     <t>New error! from string (User error)</t>
   </si>
   <si>
@@ -2324,13 +2434,28 @@
   </si>
   <si>
     <t>New object from body block</t>
+  </si>
+  <si>
+    <t>New string with truncated float! slots preallocated</t>
+  </si>
+  <si>
+    <t>New list with truncated float! slots preallocated</t>
+  </si>
+  <si>
+    <t>New path with truncated float! slots preallocated</t>
+  </si>
+  <si>
+    <t>New map with truncated float! slots preallocated</t>
+  </si>
+  <si>
+    <t>New vector with truncated float! slots preallocated</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -2387,6 +2512,19 @@
     <font>
       <b/>
       <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
       <charset val="1"/>
@@ -2777,7 +2915,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{0F1265E3-10D0-4872-A06A-A526B9F48E14}" diskRevisions="1" revisionId="35" version="14">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{98C9F52A-D0F7-4802-8C11-A1F7EF194880}" diskRevisions="1" revisionId="40" version="15">
   <header guid="{EB7A1191-CBBA-4B45-A8AB-97C58606F627}" dateTime="2016-11-18T10:22:06" maxSheetId="6" userName="qtxie" r:id="rId8" minRId="22" maxRId="24">
     <sheetIdMap count="5">
       <sheetId val="1"/>
@@ -2833,6 +2971,15 @@
     </sheetIdMap>
   </header>
   <header guid="{0F1265E3-10D0-4872-A06A-A526B9F48E14}" dateTime="2017-04-08T23:26:57" maxSheetId="6" userName="dk" r:id="rId14" minRId="35">
+    <sheetIdMap count="5">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{98C9F52A-D0F7-4802-8C11-A1F7EF194880}" dateTime="2017-07-29T00:43:12" maxSheetId="6" userName="dk" r:id="rId15" minRId="36" maxRId="40">
     <sheetIdMap count="5">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -2998,6 +3145,76 @@
       </is>
     </nc>
   </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog5.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="36" sId="4">
+    <oc r="P5" t="inlineStr">
+      <is>
+        <t>New string with truncated any-float slots preallocated</t>
+      </is>
+    </oc>
+    <nc r="P5" t="inlineStr">
+      <is>
+        <t>New string with truncated float! slots preallocated</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="37" sId="4">
+    <oc r="Q5" t="inlineStr">
+      <is>
+        <t>New list with truncated any-float slots preallocated</t>
+      </is>
+    </oc>
+    <nc r="Q5" t="inlineStr">
+      <is>
+        <t>New list with truncated float! slots preallocated</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="38" sId="4">
+    <oc r="R5" t="inlineStr">
+      <is>
+        <t>New path with truncated any-float slots preallocated</t>
+      </is>
+    </oc>
+    <nc r="R5" t="inlineStr">
+      <is>
+        <t>New path with truncated float! slots preallocated</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="39" sId="4">
+    <oc r="U5" t="inlineStr">
+      <is>
+        <t>New map with truncated any-float slots preallocated</t>
+      </is>
+    </oc>
+    <nc r="U5" t="inlineStr">
+      <is>
+        <t>New map with truncated float! slots preallocated</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="40" sId="4">
+    <oc r="V5" t="inlineStr">
+      <is>
+        <t>New vector with truncated any-float slots preallocated</t>
+      </is>
+    </oc>
+    <nc r="V5" t="inlineStr">
+      <is>
+        <t>New vector with truncated float! slots preallocated</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcmt sheetId="4" cell="P5" guid="{E32332DF-70B0-4158-B7AF-05D28786F79D}" author="dk" newLength="28"/>
+  <rcmt sheetId="4" cell="Q5" guid="{66C873E2-4441-4BDF-8D81-24C36DB880D1}" author="dk" newLength="28"/>
+  <rcmt sheetId="4" cell="R5" guid="{CE279250-3BDA-4F12-BA21-2E74ED2A8AAA}" author="dk" newLength="28"/>
+  <rcmt sheetId="4" cell="U5" guid="{0B5B29FD-145F-448D-928E-751E40B07634}" author="dk" newLength="28"/>
+  <rcmt sheetId="4" cell="V5" guid="{D0A42E6C-860A-4939-AD1F-BB779E3AEB9B}" author="dk" newLength="28"/>
 </revisions>
 </file>
 
@@ -4168,19 +4385,19 @@
       <selection activeCell="Q15" sqref="Q15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.85"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="9.375" customWidth="1"/>
-    <col min="2" max="2" width="13.375" customWidth="1"/>
-    <col min="3" max="13" width="11.875" style="18" customWidth="1"/>
-    <col min="14" max="14" width="13.875" style="18" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" customWidth="1"/>
+    <col min="3" max="13" width="11.85546875" style="18" customWidth="1"/>
+    <col min="14" max="14" width="13.85546875" style="18" customWidth="1"/>
     <col min="15" max="15" width="14" style="18" customWidth="1"/>
-    <col min="16" max="16" width="13.75" style="18" customWidth="1"/>
-    <col min="17" max="18" width="11.875" style="18" customWidth="1"/>
-    <col min="19" max="22" width="13.25" style="18" customWidth="1"/>
+    <col min="16" max="16" width="13.7109375" style="18" customWidth="1"/>
+    <col min="17" max="18" width="11.85546875" style="18" customWidth="1"/>
+    <col min="19" max="22" width="13.28515625" style="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:25" ht="41.2" customHeight="1">
+    <row r="3" spans="2:25" ht="41.25" customHeight="1">
       <c r="B3" s="19" t="s">
         <v>0</v>
       </c>
@@ -4863,7 +5080,7 @@
       </c>
       <c r="O18" s="24"/>
       <c r="P18" s="23" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="Q18" s="22" t="s">
         <v>80</v>
@@ -5087,19 +5304,19 @@
       <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.85"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="9.375" customWidth="1"/>
-    <col min="2" max="2" width="13.375" customWidth="1"/>
-    <col min="3" max="13" width="11.875" style="18" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" customWidth="1"/>
+    <col min="3" max="13" width="11.85546875" style="18" customWidth="1"/>
     <col min="14" max="15" width="14" style="18" customWidth="1"/>
-    <col min="16" max="16" width="13.75" style="18" customWidth="1"/>
-    <col min="17" max="17" width="13.25" style="18" customWidth="1"/>
-    <col min="18" max="18" width="13.75" style="18" customWidth="1"/>
-    <col min="19" max="22" width="13.25" style="18" customWidth="1"/>
+    <col min="16" max="16" width="13.7109375" style="18" customWidth="1"/>
+    <col min="17" max="17" width="13.28515625" style="18" customWidth="1"/>
+    <col min="18" max="18" width="13.7109375" style="18" customWidth="1"/>
+    <col min="19" max="22" width="13.28515625" style="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:25" ht="41.2" customHeight="1">
+    <row r="3" spans="2:25" ht="41.25" customHeight="1">
       <c r="B3" s="19" t="s">
         <v>0</v>
       </c>
@@ -5752,7 +5969,7 @@
       </c>
       <c r="O18" s="24"/>
       <c r="P18" s="23" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="Q18" s="22"/>
       <c r="R18" s="23" t="s">
@@ -5981,21 +6198,21 @@
       <selection activeCell="S17" sqref="S17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.85"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="9.375" customWidth="1"/>
-    <col min="2" max="2" width="13.375" customWidth="1"/>
-    <col min="3" max="12" width="11.875" style="18" customWidth="1"/>
-    <col min="13" max="13" width="12.125" style="18" customWidth="1"/>
-    <col min="14" max="14" width="13.875" style="18" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" customWidth="1"/>
+    <col min="3" max="12" width="11.85546875" style="18" customWidth="1"/>
+    <col min="13" max="13" width="12.140625" style="18" customWidth="1"/>
+    <col min="14" max="14" width="13.85546875" style="18" customWidth="1"/>
     <col min="15" max="15" width="14" style="18" customWidth="1"/>
-    <col min="16" max="16" width="13.75" style="18" customWidth="1"/>
-    <col min="17" max="18" width="11.875" style="18" customWidth="1"/>
-    <col min="19" max="25" width="13.25" style="18" customWidth="1"/>
-    <col min="28" max="28" width="11.75" customWidth="1"/>
+    <col min="16" max="16" width="13.7109375" style="18" customWidth="1"/>
+    <col min="17" max="18" width="11.85546875" style="18" customWidth="1"/>
+    <col min="19" max="25" width="13.28515625" style="18" customWidth="1"/>
+    <col min="28" max="28" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:28" ht="41.2" customHeight="1">
+    <row r="3" spans="2:28" ht="41.25" customHeight="1">
       <c r="B3" s="19" t="s">
         <v>0</v>
       </c>
@@ -6739,13 +6956,13 @@
       </c>
       <c r="O18" s="24"/>
       <c r="P18" s="23" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="Q18" s="22" t="s">
         <v>80</v>
       </c>
       <c r="R18" s="23" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="S18" s="24"/>
       <c r="T18" s="24"/>
@@ -7106,26 +7323,26 @@
   <dimension ref="B3:AB26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="T19" sqref="T19"/>
+      <selection activeCell="V6" sqref="V6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.85"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="9.375" customWidth="1"/>
-    <col min="2" max="2" width="13.375" customWidth="1"/>
-    <col min="3" max="13" width="11.875" style="18" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" customWidth="1"/>
+    <col min="3" max="13" width="11.85546875" style="18" customWidth="1"/>
     <col min="14" max="15" width="14" style="18" customWidth="1"/>
-    <col min="16" max="16" width="13.75" style="18" customWidth="1"/>
-    <col min="17" max="17" width="13.875" style="18" customWidth="1"/>
-    <col min="18" max="18" width="13.75" style="18" customWidth="1"/>
-    <col min="19" max="20" width="13.25" style="18" customWidth="1"/>
-    <col min="21" max="21" width="14.75" style="18" customWidth="1"/>
-    <col min="22" max="22" width="14.25" style="18" customWidth="1"/>
-    <col min="23" max="25" width="13.25" style="18" customWidth="1"/>
+    <col min="16" max="16" width="13.7109375" style="18" customWidth="1"/>
+    <col min="17" max="17" width="13.85546875" style="18" customWidth="1"/>
+    <col min="18" max="18" width="13.7109375" style="18" customWidth="1"/>
+    <col min="19" max="20" width="13.28515625" style="18" customWidth="1"/>
+    <col min="21" max="21" width="14.7109375" style="18" customWidth="1"/>
+    <col min="22" max="22" width="14.28515625" style="18" customWidth="1"/>
+    <col min="23" max="25" width="13.28515625" style="18" customWidth="1"/>
     <col min="28" max="28" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:28" ht="41.2" customHeight="1">
+    <row r="3" spans="2:28" ht="41.25" customHeight="1">
       <c r="B3" s="19" t="s">
         <v>0</v>
       </c>
@@ -7293,21 +7510,21 @@
       </c>
       <c r="O5" s="24"/>
       <c r="P5" s="25" t="s">
-        <v>177</v>
+        <v>273</v>
       </c>
       <c r="Q5" s="25" t="s">
-        <v>178</v>
+        <v>274</v>
       </c>
       <c r="R5" s="25" t="s">
-        <v>179</v>
+        <v>275</v>
       </c>
       <c r="S5" s="24"/>
       <c r="T5" s="24"/>
       <c r="U5" s="25" t="s">
-        <v>180</v>
+        <v>276</v>
       </c>
       <c r="V5" s="25" t="s">
-        <v>181</v>
+        <v>277</v>
       </c>
       <c r="W5" s="24"/>
       <c r="X5" s="26" t="s">
@@ -7804,7 +8021,7 @@
       <c r="W17" s="24"/>
       <c r="X17" s="24"/>
       <c r="Y17" s="26" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
     </row>
     <row r="18" spans="2:28" ht="43.5" customHeight="1">
@@ -7816,7 +8033,7 @@
         <v>160</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="F18" s="24"/>
       <c r="G18" s="23" t="s">
@@ -7843,19 +8060,19 @@
       </c>
       <c r="O18" s="24"/>
       <c r="P18" s="23" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="Q18" s="22" t="s">
         <v>80</v>
       </c>
       <c r="R18" s="23" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="S18" s="25" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="T18" s="25" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="U18" s="25" t="s">
         <v>135</v>
@@ -7864,13 +8081,13 @@
         <v>136</v>
       </c>
       <c r="W18" s="25" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="X18" s="26" t="s">
         <v>161</v>
       </c>
       <c r="Y18" s="30" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="19" spans="2:28" ht="43.5" customHeight="1">
@@ -8150,7 +8367,7 @@
       <c r="U25" s="24"/>
       <c r="V25" s="24"/>
       <c r="W25" s="25" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="X25" s="22"/>
       <c r="Y25" s="24"/>
@@ -8179,7 +8396,7 @@
       <c r="N26" s="24"/>
       <c r="O26" s="24"/>
       <c r="P26" s="23" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="Q26" s="25"/>
       <c r="R26" s="25"/>
@@ -8221,14 +8438,14 @@
       <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.25" defaultRowHeight="18" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="18" customHeight="1"/>
   <cols>
-    <col min="1" max="256" width="16.25" style="1" customWidth="1"/>
+    <col min="1" max="256" width="16.28515625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:58" ht="28" customHeight="1">
+    <row r="1" spans="1:58" ht="27.95" customHeight="1">
       <c r="A1" s="33" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="B1" s="33"/>
       <c r="C1" s="33"/>
@@ -8288,22 +8505,22 @@
       <c r="BE1" s="33"/>
       <c r="BF1" s="33"/>
     </row>
-    <row r="2" spans="1:58" ht="20.7" customHeight="1">
+    <row r="2" spans="1:58" ht="20.65" customHeight="1">
       <c r="A2" s="2"/>
       <c r="B2" s="3" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>11</v>
@@ -8312,49 +8529,49 @@
         <v>12</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="M2" s="3" t="s">
         <v>9</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="O2" s="3" t="s">
         <v>2</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="Q2" s="3" t="s">
         <v>141</v>
       </c>
       <c r="R2" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="W2" s="3" t="s">
         <v>199</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="T2" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="U2" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="V2" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="W2" s="3" t="s">
-        <v>204</v>
       </c>
       <c r="X2" s="3" t="s">
         <v>139</v>
@@ -8363,28 +8580,28 @@
         <v>1</v>
       </c>
       <c r="Z2" s="3" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="AA2" s="3" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="AB2" s="3" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="AC2" s="3" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="AD2" s="3" t="s">
         <v>19</v>
       </c>
       <c r="AE2" s="3" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="AF2" s="3" t="s">
         <v>7</v>
       </c>
       <c r="AG2" s="3" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="AH2" s="3" t="s">
         <v>6</v>
@@ -8393,49 +8610,49 @@
         <v>18</v>
       </c>
       <c r="AJ2" s="3" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="AK2" s="3" t="s">
         <v>140</v>
       </c>
       <c r="AL2" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="AM2" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="AN2" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="AO2" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="AP2" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="AQ2" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="AM2" s="3" t="s">
+      <c r="AR2" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="AN2" s="3" t="s">
+      <c r="AS2" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="AO2" s="3" t="s">
+      <c r="AT2" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="AP2" s="3" t="s">
+      <c r="AU2" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="AQ2" s="3" t="s">
+      <c r="AV2" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="AR2" s="3" t="s">
+      <c r="AW2" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="AS2" s="3" t="s">
+      <c r="AX2" s="3" t="s">
         <v>219</v>
-      </c>
-      <c r="AT2" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="AU2" s="3" t="s">
-        <v>221</v>
-      </c>
-      <c r="AV2" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="AW2" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="AX2" s="3" t="s">
-        <v>224</v>
       </c>
       <c r="AY2" s="3" t="s">
         <v>3</v>
@@ -8450,209 +8667,209 @@
         <v>8</v>
       </c>
       <c r="BC2" s="3" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="BD2" s="3" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="BE2" s="3" t="s">
         <v>20</v>
       </c>
       <c r="BF2" s="3" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
     </row>
     <row r="3" spans="1:58" ht="32.65" customHeight="1">
       <c r="A3" s="34" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="P3" s="5" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="Q3" s="5" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="R3" s="5" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="S3" s="5" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="T3" s="5" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="U3" s="5" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="V3" s="5" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="W3" s="5" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="X3" s="5" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="Y3" s="5" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="Z3" s="5" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="AA3" s="5" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="AB3" s="5" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="AC3" s="5" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="AD3" s="5" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="AE3" s="5" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="AF3" s="5" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="AG3" s="5" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="AH3" s="5" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="AI3" s="5" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="AJ3" s="5" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="AK3" s="5" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="AL3" s="5" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="AM3" s="5" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="AN3" s="5" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="AO3" s="5" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="AP3" s="5" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="AQ3" s="5" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="AR3" s="5" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="AS3" s="5" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="AT3" s="5" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="AU3" s="5" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="AV3" s="5" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="AW3" s="5" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="AX3" s="5" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="AY3" s="5" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="AZ3" s="5" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="BA3" s="5" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="BB3" s="5" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="BC3" s="5" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="BD3" s="5" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="BE3" s="5" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="BF3" s="5" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="4" spans="1:58" ht="44.4" customHeight="1">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="4" spans="1:58" ht="44.45" customHeight="1">
       <c r="A4" s="35"/>
       <c r="B4" s="7"/>
       <c r="C4" s="8" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
       <c r="G4" s="9"/>
       <c r="H4" s="8" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="J4" s="9"/>
       <c r="K4" s="9"/>
@@ -8661,52 +8878,52 @@
       <c r="N4" s="9"/>
       <c r="O4" s="9"/>
       <c r="P4" s="8" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="Q4" s="9"/>
       <c r="R4" s="8" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="S4" s="9"/>
       <c r="T4" s="9"/>
       <c r="U4" s="8" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="V4" s="8" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="W4" s="9"/>
       <c r="X4" s="9"/>
       <c r="Y4" s="9"/>
       <c r="Z4" s="9"/>
       <c r="AA4" s="8" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="AB4" s="8" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="AC4" s="9"/>
       <c r="AD4" s="9"/>
       <c r="AE4" s="9"/>
       <c r="AF4" s="8" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="AG4" s="8" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="AH4" s="8" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="AI4" s="9"/>
       <c r="AJ4" s="8" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="AK4" s="9"/>
       <c r="AL4" s="8" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="AM4" s="8" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="AN4" s="9"/>
       <c r="AO4" s="9"/>
@@ -8715,24 +8932,24 @@
       <c r="AR4" s="9"/>
       <c r="AS4" s="9"/>
       <c r="AT4" s="8" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="AU4" s="9"/>
       <c r="AV4" s="8" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="AW4" s="9"/>
       <c r="AX4" s="8" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="AY4" s="9"/>
       <c r="AZ4" s="9"/>
       <c r="BA4" s="8" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="BB4" s="9"/>
       <c r="BC4" s="8" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="BD4" s="9"/>
       <c r="BE4" s="9"/>
@@ -8743,175 +8960,175 @@
         <v>1</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="E5" s="11" t="s">
+        <v>242</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>243</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>244</v>
+      </c>
+      <c r="J5" s="11" t="s">
+        <v>245</v>
+      </c>
+      <c r="K5" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="L5" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="M5" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="N5" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="O5" s="11" t="s">
+        <v>246</v>
+      </c>
+      <c r="P5" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="Q5" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="R5" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="S5" s="11" t="s">
         <v>247</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="T5" s="11" t="s">
         <v>248</v>
       </c>
-      <c r="G5" s="11" t="s">
-        <v>229</v>
-      </c>
-      <c r="H5" s="11" t="s">
-        <v>228</v>
-      </c>
-      <c r="I5" s="11" t="s">
+      <c r="U5" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="V5" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="W5" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="X5" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="Y5" s="11" t="s">
         <v>249</v>
       </c>
-      <c r="J5" s="11" t="s">
+      <c r="Z5" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="AA5" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="AB5" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="AC5" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="AD5" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="AE5" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="AF5" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="AG5" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="AH5" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="AI5" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="AJ5" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="AK5" s="11" t="s">
         <v>250</v>
       </c>
-      <c r="K5" s="11" t="s">
-        <v>229</v>
-      </c>
-      <c r="L5" s="11" t="s">
-        <v>229</v>
-      </c>
-      <c r="M5" s="11" t="s">
-        <v>229</v>
-      </c>
-      <c r="N5" s="11" t="s">
-        <v>229</v>
-      </c>
-      <c r="O5" s="11" t="s">
+      <c r="AL5" s="11" t="s">
         <v>251</v>
       </c>
-      <c r="P5" s="11" t="s">
-        <v>228</v>
-      </c>
-      <c r="Q5" s="11" t="s">
-        <v>229</v>
-      </c>
-      <c r="R5" s="11" t="s">
-        <v>228</v>
-      </c>
-      <c r="S5" s="11" t="s">
+      <c r="AM5" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="AN5" s="11" t="s">
         <v>252</v>
       </c>
-      <c r="T5" s="11" t="s">
+      <c r="AO5" s="11" t="s">
         <v>253</v>
       </c>
-      <c r="U5" s="11" t="s">
-        <v>229</v>
-      </c>
-      <c r="V5" s="11" t="s">
-        <v>229</v>
-      </c>
-      <c r="W5" s="11" t="s">
-        <v>229</v>
-      </c>
-      <c r="X5" s="11" t="s">
-        <v>229</v>
-      </c>
-      <c r="Y5" s="11" t="s">
+      <c r="AP5" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="AQ5" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="AR5" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="AS5" s="11" t="s">
         <v>254</v>
       </c>
-      <c r="Z5" s="11" t="s">
-        <v>229</v>
-      </c>
-      <c r="AA5" s="11" t="s">
-        <v>228</v>
-      </c>
-      <c r="AB5" s="11" t="s">
-        <v>229</v>
-      </c>
-      <c r="AC5" s="11" t="s">
-        <v>229</v>
-      </c>
-      <c r="AD5" s="11" t="s">
-        <v>229</v>
-      </c>
-      <c r="AE5" s="11" t="s">
-        <v>229</v>
-      </c>
-      <c r="AF5" s="11" t="s">
-        <v>228</v>
-      </c>
-      <c r="AG5" s="11" t="s">
-        <v>229</v>
-      </c>
-      <c r="AH5" s="11" t="s">
-        <v>228</v>
-      </c>
-      <c r="AI5" s="11" t="s">
-        <v>229</v>
-      </c>
-      <c r="AJ5" s="11" t="s">
-        <v>229</v>
-      </c>
-      <c r="AK5" s="11" t="s">
+      <c r="AT5" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="AU5" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="AV5" s="11" t="s">
         <v>255</v>
       </c>
-      <c r="AL5" s="11" t="s">
+      <c r="AW5" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="AX5" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="AY5" s="11" t="s">
         <v>256</v>
       </c>
-      <c r="AM5" s="11" t="s">
-        <v>228</v>
-      </c>
-      <c r="AN5" s="11" t="s">
+      <c r="AZ5" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="BA5" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="BB5" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="BC5" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="BD5" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="BE5" s="11" t="s">
         <v>257</v>
       </c>
-      <c r="AO5" s="11" t="s">
-        <v>258</v>
-      </c>
-      <c r="AP5" s="11" t="s">
-        <v>229</v>
-      </c>
-      <c r="AQ5" s="11" t="s">
-        <v>229</v>
-      </c>
-      <c r="AR5" s="11" t="s">
-        <v>229</v>
-      </c>
-      <c r="AS5" s="11" t="s">
-        <v>259</v>
-      </c>
-      <c r="AT5" s="11" t="s">
-        <v>229</v>
-      </c>
-      <c r="AU5" s="11" t="s">
-        <v>229</v>
-      </c>
-      <c r="AV5" s="11" t="s">
-        <v>260</v>
-      </c>
-      <c r="AW5" s="11" t="s">
-        <v>229</v>
-      </c>
-      <c r="AX5" s="11" t="s">
-        <v>228</v>
-      </c>
-      <c r="AY5" s="11" t="s">
-        <v>261</v>
-      </c>
-      <c r="AZ5" s="11" t="s">
-        <v>228</v>
-      </c>
-      <c r="BA5" s="11" t="s">
-        <v>228</v>
-      </c>
-      <c r="BB5" s="11" t="s">
-        <v>229</v>
-      </c>
-      <c r="BC5" s="11" t="s">
-        <v>228</v>
-      </c>
-      <c r="BD5" s="11" t="s">
-        <v>230</v>
-      </c>
-      <c r="BE5" s="11" t="s">
-        <v>262</v>
-      </c>
       <c r="BF5" s="11" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
     </row>
     <row r="6" spans="1:58" ht="68.45" customHeight="1">
@@ -8923,11 +9140,11 @@
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
       <c r="H6" s="8" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="I6" s="8"/>
       <c r="J6" s="8" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="K6" s="9"/>
       <c r="L6" s="9"/>
@@ -8935,11 +9152,11 @@
       <c r="N6" s="9"/>
       <c r="O6" s="9"/>
       <c r="P6" s="8" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="Q6" s="9"/>
       <c r="R6" s="8" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="S6" s="9"/>
       <c r="T6" s="9"/>
@@ -8950,25 +9167,25 @@
       <c r="Y6" s="9"/>
       <c r="Z6" s="9"/>
       <c r="AA6" s="8" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="AB6" s="12"/>
       <c r="AC6" s="9"/>
       <c r="AD6" s="9"/>
       <c r="AE6" s="9"/>
       <c r="AF6" s="8" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="AG6" s="8"/>
       <c r="AH6" s="8" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="AI6" s="9"/>
       <c r="AJ6" s="8"/>
       <c r="AK6" s="9"/>
       <c r="AL6" s="8"/>
       <c r="AM6" s="8" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="AN6" s="9"/>
       <c r="AO6" s="9"/>
@@ -8981,26 +9198,26 @@
       <c r="AV6" s="12"/>
       <c r="AW6" s="9"/>
       <c r="AX6" s="8" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="AY6" s="9"/>
       <c r="AZ6" s="8" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="BA6" s="8" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="BB6" s="9"/>
       <c r="BC6" s="8" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="BD6" s="8" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="BE6" s="9"/>
       <c r="BF6" s="9"/>
     </row>
-    <row r="7" spans="1:58" ht="20.5" customHeight="1">
+    <row r="7" spans="1:58" ht="20.45" customHeight="1">
       <c r="A7" s="6"/>
       <c r="B7" s="13"/>
       <c r="C7" s="14"/>
@@ -9060,7 +9277,7 @@
       <c r="BE7" s="14"/>
       <c r="BF7" s="14"/>
     </row>
-    <row r="8" spans="1:58" ht="20.5" customHeight="1">
+    <row r="8" spans="1:58" ht="20.45" customHeight="1">
       <c r="A8" s="6"/>
       <c r="B8" s="15"/>
       <c r="C8" s="16"/>
@@ -9120,7 +9337,7 @@
       <c r="BE8" s="16"/>
       <c r="BF8" s="16"/>
     </row>
-    <row r="9" spans="1:58" ht="20.5" customHeight="1">
+    <row r="9" spans="1:58" ht="20.45" customHeight="1">
       <c r="A9" s="6"/>
       <c r="B9" s="13"/>
       <c r="C9" s="14"/>
@@ -9180,7 +9397,7 @@
       <c r="BE9" s="14"/>
       <c r="BF9" s="14"/>
     </row>
-    <row r="10" spans="1:58" ht="20.5" customHeight="1">
+    <row r="10" spans="1:58" ht="20.45" customHeight="1">
       <c r="A10" s="6"/>
       <c r="B10" s="15"/>
       <c r="C10" s="16"/>
@@ -9240,7 +9457,7 @@
       <c r="BE10" s="16"/>
       <c r="BF10" s="16"/>
     </row>
-    <row r="11" spans="1:58" ht="20.5" customHeight="1">
+    <row r="11" spans="1:58" ht="20.45" customHeight="1">
       <c r="A11" s="6"/>
       <c r="B11" s="13"/>
       <c r="C11" s="14"/>
@@ -9300,7 +9517,7 @@
       <c r="BE11" s="14"/>
       <c r="BF11" s="14"/>
     </row>
-    <row r="12" spans="1:58" ht="20.5" customHeight="1">
+    <row r="12" spans="1:58" ht="20.45" customHeight="1">
       <c r="A12" s="6"/>
       <c r="B12" s="15"/>
       <c r="C12" s="16"/>
@@ -9360,7 +9577,7 @@
       <c r="BE12" s="16"/>
       <c r="BF12" s="16"/>
     </row>
-    <row r="13" spans="1:58" ht="20.5" customHeight="1">
+    <row r="13" spans="1:58" ht="20.45" customHeight="1">
       <c r="A13" s="6"/>
       <c r="B13" s="13"/>
       <c r="C13" s="14"/>
@@ -9420,7 +9637,7 @@
       <c r="BE13" s="14"/>
       <c r="BF13" s="14"/>
     </row>
-    <row r="14" spans="1:58" ht="20.5" customHeight="1">
+    <row r="14" spans="1:58" ht="20.45" customHeight="1">
       <c r="A14" s="6"/>
       <c r="B14" s="15"/>
       <c r="C14" s="16"/>
@@ -9480,7 +9697,7 @@
       <c r="BE14" s="16"/>
       <c r="BF14" s="16"/>
     </row>
-    <row r="15" spans="1:58" ht="20.5" customHeight="1">
+    <row r="15" spans="1:58" ht="20.45" customHeight="1">
       <c r="A15" s="6"/>
       <c r="B15" s="13"/>
       <c r="C15" s="14"/>
@@ -9540,7 +9757,7 @@
       <c r="BE15" s="14"/>
       <c r="BF15" s="14"/>
     </row>
-    <row r="16" spans="1:58" ht="20.5" customHeight="1">
+    <row r="16" spans="1:58" ht="20.45" customHeight="1">
       <c r="A16" s="6"/>
       <c r="B16" s="15"/>
       <c r="C16" s="16"/>
@@ -9600,7 +9817,7 @@
       <c r="BE16" s="16"/>
       <c r="BF16" s="16"/>
     </row>
-    <row r="17" spans="1:58" ht="20.5" customHeight="1">
+    <row r="17" spans="1:58" ht="20.45" customHeight="1">
       <c r="A17" s="6"/>
       <c r="B17" s="13"/>
       <c r="C17" s="14"/>
@@ -9660,7 +9877,7 @@
       <c r="BE17" s="14"/>
       <c r="BF17" s="14"/>
     </row>
-    <row r="18" spans="1:58" ht="20.5" customHeight="1">
+    <row r="18" spans="1:58" ht="20.45" customHeight="1">
       <c r="A18" s="6"/>
       <c r="B18" s="15"/>
       <c r="C18" s="16"/>
@@ -9720,7 +9937,7 @@
       <c r="BE18" s="16"/>
       <c r="BF18" s="16"/>
     </row>
-    <row r="19" spans="1:58" ht="20.5" customHeight="1">
+    <row r="19" spans="1:58" ht="20.45" customHeight="1">
       <c r="A19" s="6"/>
       <c r="B19" s="13"/>
       <c r="C19" s="14"/>
@@ -9780,7 +9997,7 @@
       <c r="BE19" s="14"/>
       <c r="BF19" s="14"/>
     </row>
-    <row r="20" spans="1:58" ht="20.5" customHeight="1">
+    <row r="20" spans="1:58" ht="20.45" customHeight="1">
       <c r="A20" s="6"/>
       <c r="B20" s="15"/>
       <c r="C20" s="16"/>
@@ -9840,7 +10057,7 @@
       <c r="BE20" s="16"/>
       <c r="BF20" s="16"/>
     </row>
-    <row r="21" spans="1:58" ht="20.5" customHeight="1">
+    <row r="21" spans="1:58" ht="20.45" customHeight="1">
       <c r="A21" s="6"/>
       <c r="B21" s="13"/>
       <c r="C21" s="14"/>
@@ -9900,7 +10117,7 @@
       <c r="BE21" s="14"/>
       <c r="BF21" s="14"/>
     </row>
-    <row r="22" spans="1:58" ht="20.5" customHeight="1">
+    <row r="22" spans="1:58" ht="20.45" customHeight="1">
       <c r="A22" s="6"/>
       <c r="B22" s="15"/>
       <c r="C22" s="16"/>
@@ -9960,7 +10177,7 @@
       <c r="BE22" s="16"/>
       <c r="BF22" s="16"/>
     </row>
-    <row r="23" spans="1:58" ht="20.5" customHeight="1">
+    <row r="23" spans="1:58" ht="20.45" customHeight="1">
       <c r="A23" s="17"/>
       <c r="B23" s="13"/>
       <c r="C23" s="14"/>

</xml_diff>

<commit_message>
DOC: improved wording for `make <series> <float>` cases to avoid confusion (issue #2940).
</commit_message>
<xml_diff>
--- a/docs/conversion-matrix.xlsx
+++ b/docs/conversion-matrix.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr date1904="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27600" windowHeight="13845" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27602" windowHeight="13844" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="R3 TO matrix" sheetId="1" r:id="rId1"/>
@@ -1609,7 +1609,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="955" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="955" uniqueCount="285">
   <si>
     <t>From \ To</t>
   </si>
@@ -2144,9 +2144,6 @@
     <t>New error with integer error code</t>
   </si>
   <si>
-    <t>New binary with truncated any-float slots preallocated</t>
-  </si>
-  <si>
     <t>New error! from string (User error)</t>
   </si>
   <si>
@@ -2436,19 +2433,43 @@
     <t>New object from body block</t>
   </si>
   <si>
-    <t>New string with truncated float! slots preallocated</t>
-  </si>
-  <si>
-    <t>New list with truncated float! slots preallocated</t>
-  </si>
-  <si>
-    <t>New path with truncated float! slots preallocated</t>
-  </si>
-  <si>
-    <t>New map with truncated float! slots preallocated</t>
-  </si>
-  <si>
-    <t>New vector with truncated float! slots preallocated</t>
+    <t>New binary with truncated any-float number of slots preallocated</t>
+  </si>
+  <si>
+    <t>New string with truncated float! number of slots preallocated</t>
+  </si>
+  <si>
+    <t>New list with truncated float! number of slots preallocated</t>
+  </si>
+  <si>
+    <t>New path with truncated float! number of slots preallocated</t>
+  </si>
+  <si>
+    <t>New map with truncated float! slots number of preallocated</t>
+  </si>
+  <si>
+    <t>New vector with truncated float! slots number of preallocated</t>
+  </si>
+  <si>
+    <t>New bitset with integer number of slots preallocated</t>
+  </si>
+  <si>
+    <t>New binary with integer number of slots preallocated</t>
+  </si>
+  <si>
+    <t>New string with integer slots number of preallocated</t>
+  </si>
+  <si>
+    <t>New list with integer slots number of preallocated</t>
+  </si>
+  <si>
+    <t>New path with integer slots number of preallocated</t>
+  </si>
+  <si>
+    <t>New map with integer slots number of preallocated</t>
+  </si>
+  <si>
+    <t>New vector with integer number of slots preallocated</t>
   </si>
 </sst>
 </file>
@@ -2915,7 +2936,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{98C9F52A-D0F7-4802-8C11-A1F7EF194880}" diskRevisions="1" revisionId="40" version="15">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{264BB4E1-8C21-465A-8536-3EE0FB803C4B}" diskRevisions="1" revisionId="53" version="16">
   <header guid="{EB7A1191-CBBA-4B45-A8AB-97C58606F627}" dateTime="2016-11-18T10:22:06" maxSheetId="6" userName="qtxie" r:id="rId8" minRId="22" maxRId="24">
     <sheetIdMap count="5">
       <sheetId val="1"/>
@@ -2980,6 +3001,15 @@
     </sheetIdMap>
   </header>
   <header guid="{98C9F52A-D0F7-4802-8C11-A1F7EF194880}" dateTime="2017-07-29T00:43:12" maxSheetId="6" userName="dk" r:id="rId15" minRId="36" maxRId="40">
+    <sheetIdMap count="5">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{264BB4E1-8C21-465A-8536-3EE0FB803C4B}" dateTime="2017-07-30T12:42:35" maxSheetId="6" userName="dk" r:id="rId16" minRId="41" maxRId="53">
     <sheetIdMap count="5">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -3215,6 +3245,167 @@
   <rcmt sheetId="4" cell="R5" guid="{CE279250-3BDA-4F12-BA21-2E74ED2A8AAA}" author="dk" newLength="28"/>
   <rcmt sheetId="4" cell="U5" guid="{0B5B29FD-145F-448D-928E-751E40B07634}" author="dk" newLength="28"/>
   <rcmt sheetId="4" cell="V5" guid="{D0A42E6C-860A-4939-AD1F-BB779E3AEB9B}" author="dk" newLength="28"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog6.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="41" sId="4">
+    <oc r="N5" t="inlineStr">
+      <is>
+        <t>New binary with truncated any-float slots preallocated</t>
+      </is>
+    </oc>
+    <nc r="N5" t="inlineStr">
+      <is>
+        <t>New binary with truncated any-float number of slots preallocated</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="42" sId="4">
+    <oc r="P5" t="inlineStr">
+      <is>
+        <t>New string with truncated float! slots preallocated</t>
+      </is>
+    </oc>
+    <nc r="P5" t="inlineStr">
+      <is>
+        <t>New string with truncated float! number of slots preallocated</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="43" sId="4">
+    <oc r="Q5" t="inlineStr">
+      <is>
+        <t>New list with truncated float! slots preallocated</t>
+      </is>
+    </oc>
+    <nc r="Q5" t="inlineStr">
+      <is>
+        <t>New list with truncated float! number of slots preallocated</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="44" sId="4">
+    <oc r="R5" t="inlineStr">
+      <is>
+        <t>New path with truncated float! slots preallocated</t>
+      </is>
+    </oc>
+    <nc r="R5" t="inlineStr">
+      <is>
+        <t>New path with truncated float! number of slots preallocated</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="45" sId="4">
+    <oc r="U5" t="inlineStr">
+      <is>
+        <t>New map with truncated float! slots preallocated</t>
+      </is>
+    </oc>
+    <nc r="U5" t="inlineStr">
+      <is>
+        <t>New map with truncated float! slots number of preallocated</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="46" sId="4">
+    <oc r="V5" t="inlineStr">
+      <is>
+        <t>New vector with truncated float! slots preallocated</t>
+      </is>
+    </oc>
+    <nc r="V5" t="inlineStr">
+      <is>
+        <t>New vector with truncated float! slots number of preallocated</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="47" sId="4">
+    <oc r="M4" t="inlineStr">
+      <is>
+        <t>New bitset with integer slots preallocated</t>
+      </is>
+    </oc>
+    <nc r="M4" t="inlineStr">
+      <is>
+        <t>New bitset with integer number of slots preallocated</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="48" sId="4">
+    <oc r="N4" t="inlineStr">
+      <is>
+        <t>New binary with integer slots preallocated</t>
+      </is>
+    </oc>
+    <nc r="N4" t="inlineStr">
+      <is>
+        <t>New binary with integer number of slots preallocated</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="49" sId="4">
+    <oc r="P4" t="inlineStr">
+      <is>
+        <t>New string with integer slots preallocated</t>
+      </is>
+    </oc>
+    <nc r="P4" t="inlineStr">
+      <is>
+        <t>New string with integer slots number of preallocated</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="50" sId="4">
+    <oc r="Q4" t="inlineStr">
+      <is>
+        <t>New list with integer slots preallocated</t>
+      </is>
+    </oc>
+    <nc r="Q4" t="inlineStr">
+      <is>
+        <t>New list with integer slots number of preallocated</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="51" sId="4">
+    <oc r="R4" t="inlineStr">
+      <is>
+        <t>New path with integer slots preallocated</t>
+      </is>
+    </oc>
+    <nc r="R4" t="inlineStr">
+      <is>
+        <t>New path with integer slots number of preallocated</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="52" sId="4">
+    <oc r="U4" t="inlineStr">
+      <is>
+        <t>New map with integer slots preallocated</t>
+      </is>
+    </oc>
+    <nc r="U4" t="inlineStr">
+      <is>
+        <t>New map with integer slots number of preallocated</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="53" sId="4">
+    <oc r="V4" t="inlineStr">
+      <is>
+        <t>New vector with integer slots preallocated</t>
+      </is>
+    </oc>
+    <nc r="V4" t="inlineStr">
+      <is>
+        <t>New vector with integer number of slots preallocated</t>
+      </is>
+    </nc>
+  </rcc>
 </revisions>
 </file>
 
@@ -4385,19 +4576,19 @@
       <selection activeCell="Q15" sqref="Q15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.85"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" customWidth="1"/>
-    <col min="3" max="13" width="11.85546875" style="18" customWidth="1"/>
-    <col min="14" max="14" width="13.85546875" style="18" customWidth="1"/>
+    <col min="1" max="1" width="9.375" customWidth="1"/>
+    <col min="2" max="2" width="13.375" customWidth="1"/>
+    <col min="3" max="13" width="11.875" style="18" customWidth="1"/>
+    <col min="14" max="14" width="13.875" style="18" customWidth="1"/>
     <col min="15" max="15" width="14" style="18" customWidth="1"/>
-    <col min="16" max="16" width="13.7109375" style="18" customWidth="1"/>
-    <col min="17" max="18" width="11.85546875" style="18" customWidth="1"/>
-    <col min="19" max="22" width="13.28515625" style="18" customWidth="1"/>
+    <col min="16" max="16" width="13.75" style="18" customWidth="1"/>
+    <col min="17" max="18" width="11.875" style="18" customWidth="1"/>
+    <col min="19" max="22" width="13.25" style="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:25" ht="41.25" customHeight="1">
+    <row r="3" spans="2:25" ht="41.2" customHeight="1">
       <c r="B3" s="19" t="s">
         <v>0</v>
       </c>
@@ -5080,7 +5271,7 @@
       </c>
       <c r="O18" s="24"/>
       <c r="P18" s="23" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="Q18" s="22" t="s">
         <v>80</v>
@@ -5304,19 +5495,19 @@
       <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.85"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" customWidth="1"/>
-    <col min="3" max="13" width="11.85546875" style="18" customWidth="1"/>
+    <col min="1" max="1" width="9.375" customWidth="1"/>
+    <col min="2" max="2" width="13.375" customWidth="1"/>
+    <col min="3" max="13" width="11.875" style="18" customWidth="1"/>
     <col min="14" max="15" width="14" style="18" customWidth="1"/>
-    <col min="16" max="16" width="13.7109375" style="18" customWidth="1"/>
-    <col min="17" max="17" width="13.28515625" style="18" customWidth="1"/>
-    <col min="18" max="18" width="13.7109375" style="18" customWidth="1"/>
-    <col min="19" max="22" width="13.28515625" style="18" customWidth="1"/>
+    <col min="16" max="16" width="13.75" style="18" customWidth="1"/>
+    <col min="17" max="17" width="13.25" style="18" customWidth="1"/>
+    <col min="18" max="18" width="13.75" style="18" customWidth="1"/>
+    <col min="19" max="22" width="13.25" style="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:25" ht="41.25" customHeight="1">
+    <row r="3" spans="2:25" ht="41.2" customHeight="1">
       <c r="B3" s="19" t="s">
         <v>0</v>
       </c>
@@ -5969,7 +6160,7 @@
       </c>
       <c r="O18" s="24"/>
       <c r="P18" s="23" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="Q18" s="22"/>
       <c r="R18" s="23" t="s">
@@ -6194,25 +6385,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:AB26"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="S17" sqref="S17"/>
+    <sheetView topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.85"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" customWidth="1"/>
-    <col min="3" max="12" width="11.85546875" style="18" customWidth="1"/>
-    <col min="13" max="13" width="12.140625" style="18" customWidth="1"/>
-    <col min="14" max="14" width="13.85546875" style="18" customWidth="1"/>
+    <col min="1" max="1" width="9.375" customWidth="1"/>
+    <col min="2" max="2" width="13.375" customWidth="1"/>
+    <col min="3" max="12" width="11.875" style="18" customWidth="1"/>
+    <col min="13" max="13" width="12.125" style="18" customWidth="1"/>
+    <col min="14" max="14" width="13.875" style="18" customWidth="1"/>
     <col min="15" max="15" width="14" style="18" customWidth="1"/>
-    <col min="16" max="16" width="13.7109375" style="18" customWidth="1"/>
-    <col min="17" max="18" width="11.85546875" style="18" customWidth="1"/>
-    <col min="19" max="25" width="13.28515625" style="18" customWidth="1"/>
-    <col min="28" max="28" width="11.7109375" customWidth="1"/>
+    <col min="16" max="16" width="13.75" style="18" customWidth="1"/>
+    <col min="17" max="18" width="11.875" style="18" customWidth="1"/>
+    <col min="19" max="25" width="13.25" style="18" customWidth="1"/>
+    <col min="28" max="28" width="11.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:28" ht="41.25" customHeight="1">
+    <row r="3" spans="2:28" ht="41.2" customHeight="1">
       <c r="B3" s="19" t="s">
         <v>0</v>
       </c>
@@ -6956,13 +7147,13 @@
       </c>
       <c r="O18" s="24"/>
       <c r="P18" s="23" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="Q18" s="22" t="s">
         <v>80</v>
       </c>
       <c r="R18" s="23" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="S18" s="24"/>
       <c r="T18" s="24"/>
@@ -7323,26 +7514,26 @@
   <dimension ref="B3:AB26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="V6" sqref="V6"/>
+      <selection activeCell="V5" sqref="V5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.85"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" customWidth="1"/>
-    <col min="3" max="13" width="11.85546875" style="18" customWidth="1"/>
+    <col min="1" max="1" width="9.375" customWidth="1"/>
+    <col min="2" max="2" width="13.375" customWidth="1"/>
+    <col min="3" max="13" width="11.875" style="18" customWidth="1"/>
     <col min="14" max="15" width="14" style="18" customWidth="1"/>
-    <col min="16" max="16" width="13.7109375" style="18" customWidth="1"/>
-    <col min="17" max="17" width="13.85546875" style="18" customWidth="1"/>
-    <col min="18" max="18" width="13.7109375" style="18" customWidth="1"/>
-    <col min="19" max="20" width="13.28515625" style="18" customWidth="1"/>
-    <col min="21" max="21" width="14.7109375" style="18" customWidth="1"/>
-    <col min="22" max="22" width="14.28515625" style="18" customWidth="1"/>
-    <col min="23" max="25" width="13.28515625" style="18" customWidth="1"/>
+    <col min="16" max="16" width="13.75" style="18" customWidth="1"/>
+    <col min="17" max="17" width="13.875" style="18" customWidth="1"/>
+    <col min="18" max="18" width="13.75" style="18" customWidth="1"/>
+    <col min="19" max="20" width="13.25" style="18" customWidth="1"/>
+    <col min="21" max="21" width="14.75" style="18" customWidth="1"/>
+    <col min="22" max="22" width="14.25" style="18" customWidth="1"/>
+    <col min="23" max="25" width="13.25" style="18" customWidth="1"/>
     <col min="28" max="28" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:28" ht="41.25" customHeight="1">
+    <row r="3" spans="2:28" ht="41.2" customHeight="1">
       <c r="B3" s="19" t="s">
         <v>0</v>
       </c>
@@ -7443,28 +7634,28 @@
       <c r="K4" s="24"/>
       <c r="L4" s="24"/>
       <c r="M4" s="23" t="s">
-        <v>26</v>
+        <v>278</v>
       </c>
       <c r="N4" s="25" t="s">
-        <v>117</v>
+        <v>279</v>
       </c>
       <c r="O4" s="24"/>
       <c r="P4" s="25" t="s">
-        <v>118</v>
+        <v>280</v>
       </c>
       <c r="Q4" s="25" t="s">
-        <v>119</v>
+        <v>281</v>
       </c>
       <c r="R4" s="25" t="s">
-        <v>120</v>
+        <v>282</v>
       </c>
       <c r="S4" s="24"/>
       <c r="T4" s="24"/>
       <c r="U4" s="25" t="s">
-        <v>121</v>
+        <v>283</v>
       </c>
       <c r="V4" s="25" t="s">
-        <v>122</v>
+        <v>284</v>
       </c>
       <c r="W4" s="24"/>
       <c r="X4" s="26" t="s">
@@ -7506,7 +7697,7 @@
       <c r="L5" s="24"/>
       <c r="M5" s="24"/>
       <c r="N5" s="25" t="s">
-        <v>176</v>
+        <v>272</v>
       </c>
       <c r="O5" s="24"/>
       <c r="P5" s="25" t="s">
@@ -8021,7 +8212,7 @@
       <c r="W17" s="24"/>
       <c r="X17" s="24"/>
       <c r="Y17" s="26" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="18" spans="2:28" ht="43.5" customHeight="1">
@@ -8033,7 +8224,7 @@
         <v>160</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="F18" s="24"/>
       <c r="G18" s="23" t="s">
@@ -8060,19 +8251,19 @@
       </c>
       <c r="O18" s="24"/>
       <c r="P18" s="23" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="Q18" s="22" t="s">
         <v>80</v>
       </c>
       <c r="R18" s="23" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="S18" s="25" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="T18" s="25" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="U18" s="25" t="s">
         <v>135</v>
@@ -8081,13 +8272,13 @@
         <v>136</v>
       </c>
       <c r="W18" s="25" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="X18" s="26" t="s">
         <v>161</v>
       </c>
       <c r="Y18" s="30" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="19" spans="2:28" ht="43.5" customHeight="1">
@@ -8367,7 +8558,7 @@
       <c r="U25" s="24"/>
       <c r="V25" s="24"/>
       <c r="W25" s="25" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="X25" s="22"/>
       <c r="Y25" s="24"/>
@@ -8396,7 +8587,7 @@
       <c r="N26" s="24"/>
       <c r="O26" s="24"/>
       <c r="P26" s="23" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="Q26" s="25"/>
       <c r="R26" s="25"/>
@@ -8438,14 +8629,14 @@
       <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="18" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="16.25" defaultRowHeight="18" customHeight="1"/>
   <cols>
-    <col min="1" max="256" width="16.28515625" style="1" customWidth="1"/>
+    <col min="1" max="256" width="16.25" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:58" ht="27.95" customHeight="1">
+    <row r="1" spans="1:58" ht="28" customHeight="1">
       <c r="A1" s="33" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B1" s="33"/>
       <c r="C1" s="33"/>
@@ -8505,22 +8696,22 @@
       <c r="BE1" s="33"/>
       <c r="BF1" s="33"/>
     </row>
-    <row r="2" spans="1:58" ht="20.65" customHeight="1">
+    <row r="2" spans="1:58" ht="20.7" customHeight="1">
       <c r="A2" s="2"/>
       <c r="B2" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>187</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>188</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>11</v>
@@ -8529,49 +8720,49 @@
         <v>12</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="K2" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="L2" s="3" t="s">
         <v>190</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>191</v>
       </c>
       <c r="M2" s="3" t="s">
         <v>9</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="O2" s="3" t="s">
         <v>2</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="Q2" s="3" t="s">
         <v>141</v>
       </c>
       <c r="R2" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="S2" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="T2" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="T2" s="3" t="s">
+      <c r="U2" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="U2" s="3" t="s">
+      <c r="V2" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="V2" s="3" t="s">
+      <c r="W2" s="3" t="s">
         <v>198</v>
-      </c>
-      <c r="W2" s="3" t="s">
-        <v>199</v>
       </c>
       <c r="X2" s="3" t="s">
         <v>139</v>
@@ -8580,28 +8771,28 @@
         <v>1</v>
       </c>
       <c r="Z2" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="AA2" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="AA2" s="3" t="s">
+      <c r="AB2" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="AB2" s="3" t="s">
+      <c r="AC2" s="3" t="s">
         <v>202</v>
-      </c>
-      <c r="AC2" s="3" t="s">
-        <v>203</v>
       </c>
       <c r="AD2" s="3" t="s">
         <v>19</v>
       </c>
       <c r="AE2" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="AF2" s="3" t="s">
         <v>7</v>
       </c>
       <c r="AG2" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="AH2" s="3" t="s">
         <v>6</v>
@@ -8610,49 +8801,49 @@
         <v>18</v>
       </c>
       <c r="AJ2" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="AK2" s="3" t="s">
         <v>140</v>
       </c>
       <c r="AL2" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="AM2" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="AM2" s="3" t="s">
+      <c r="AN2" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="AN2" s="3" t="s">
+      <c r="AO2" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="AO2" s="3" t="s">
+      <c r="AP2" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="AP2" s="3" t="s">
+      <c r="AQ2" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="AQ2" s="3" t="s">
+      <c r="AR2" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="AR2" s="3" t="s">
+      <c r="AS2" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="AS2" s="3" t="s">
+      <c r="AT2" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="AT2" s="3" t="s">
+      <c r="AU2" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="AU2" s="3" t="s">
+      <c r="AV2" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="AV2" s="3" t="s">
+      <c r="AW2" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="AW2" s="3" t="s">
+      <c r="AX2" s="3" t="s">
         <v>218</v>
-      </c>
-      <c r="AX2" s="3" t="s">
-        <v>219</v>
       </c>
       <c r="AY2" s="3" t="s">
         <v>3</v>
@@ -8667,209 +8858,209 @@
         <v>8</v>
       </c>
       <c r="BC2" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="BD2" s="3" t="s">
         <v>220</v>
-      </c>
-      <c r="BD2" s="3" t="s">
-        <v>221</v>
       </c>
       <c r="BE2" s="3" t="s">
         <v>20</v>
       </c>
       <c r="BF2" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="3" spans="1:58" ht="32.65" customHeight="1">
       <c r="A3" s="34" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>223</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="F3" s="5" t="s">
         <v>223</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="G3" s="5" t="s">
         <v>223</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="H3" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="O3" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="P3" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="Q3" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="R3" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="S3" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="T3" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="U3" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="V3" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="W3" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="X3" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="Y3" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="Z3" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="AA3" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="AB3" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="AC3" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="AD3" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="AE3" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="AF3" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="AG3" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="AH3" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="AI3" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="AJ3" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="AK3" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="AL3" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="AM3" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="AN3" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="AO3" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="AP3" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="AQ3" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="AR3" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="AS3" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="AT3" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="AU3" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="AV3" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="AW3" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="AX3" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="AY3" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="AZ3" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="BA3" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="BB3" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="BC3" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="BD3" s="5" t="s">
         <v>224</v>
       </c>
-      <c r="F3" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="H3" s="5" t="s">
+      <c r="BE3" s="5" t="s">
         <v>223</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="BF3" s="5" t="s">
         <v>223</v>
       </c>
-      <c r="J3" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="K3" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="M3" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="N3" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="O3" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="P3" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="Q3" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="R3" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="S3" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="T3" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="U3" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="V3" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="W3" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="X3" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="Y3" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="Z3" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="AA3" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="AB3" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="AC3" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="AD3" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="AE3" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="AF3" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="AG3" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="AH3" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="AI3" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="AJ3" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="AK3" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="AL3" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="AM3" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="AN3" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="AO3" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="AP3" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="AQ3" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="AR3" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="AS3" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="AT3" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="AU3" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="AV3" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="AW3" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="AX3" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="AY3" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="AZ3" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="BA3" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="BB3" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="BC3" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="BD3" s="5" t="s">
-        <v>225</v>
-      </c>
-      <c r="BE3" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="BF3" s="5" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="4" spans="1:58" ht="44.45" customHeight="1">
+    </row>
+    <row r="4" spans="1:58" ht="44.4" customHeight="1">
       <c r="A4" s="35"/>
       <c r="B4" s="7"/>
       <c r="C4" s="8" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
       <c r="G4" s="9"/>
       <c r="H4" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="I4" s="8" t="s">
         <v>227</v>
-      </c>
-      <c r="I4" s="8" t="s">
-        <v>228</v>
       </c>
       <c r="J4" s="9"/>
       <c r="K4" s="9"/>
@@ -8878,52 +9069,52 @@
       <c r="N4" s="9"/>
       <c r="O4" s="9"/>
       <c r="P4" s="8" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="Q4" s="9"/>
       <c r="R4" s="8" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="S4" s="9"/>
       <c r="T4" s="9"/>
       <c r="U4" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="V4" s="8" t="s">
         <v>231</v>
-      </c>
-      <c r="V4" s="8" t="s">
-        <v>232</v>
       </c>
       <c r="W4" s="9"/>
       <c r="X4" s="9"/>
       <c r="Y4" s="9"/>
       <c r="Z4" s="9"/>
       <c r="AA4" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="AB4" s="8" t="s">
         <v>233</v>
-      </c>
-      <c r="AB4" s="8" t="s">
-        <v>234</v>
       </c>
       <c r="AC4" s="9"/>
       <c r="AD4" s="9"/>
       <c r="AE4" s="9"/>
       <c r="AF4" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="AG4" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="AH4" s="8" t="s">
         <v>235</v>
-      </c>
-      <c r="AG4" s="8" t="s">
-        <v>235</v>
-      </c>
-      <c r="AH4" s="8" t="s">
-        <v>236</v>
       </c>
       <c r="AI4" s="9"/>
       <c r="AJ4" s="8" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="AK4" s="9"/>
       <c r="AL4" s="8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AM4" s="8" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="AN4" s="9"/>
       <c r="AO4" s="9"/>
@@ -8932,24 +9123,24 @@
       <c r="AR4" s="9"/>
       <c r="AS4" s="9"/>
       <c r="AT4" s="8" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="AU4" s="9"/>
       <c r="AV4" s="8" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="AW4" s="9"/>
       <c r="AX4" s="8" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AY4" s="9"/>
       <c r="AZ4" s="9"/>
       <c r="BA4" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="BB4" s="9"/>
       <c r="BC4" s="8" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="BD4" s="9"/>
       <c r="BE4" s="9"/>
@@ -8960,175 +9151,175 @@
         <v>1</v>
       </c>
       <c r="B5" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>241</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>242</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>243</v>
+      </c>
+      <c r="J5" s="11" t="s">
+        <v>244</v>
+      </c>
+      <c r="K5" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="L5" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="M5" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="N5" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="O5" s="11" t="s">
+        <v>245</v>
+      </c>
+      <c r="P5" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="Q5" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="R5" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="S5" s="11" t="s">
+        <v>246</v>
+      </c>
+      <c r="T5" s="11" t="s">
+        <v>247</v>
+      </c>
+      <c r="U5" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="V5" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="W5" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="X5" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="Y5" s="11" t="s">
+        <v>248</v>
+      </c>
+      <c r="Z5" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="AA5" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="AB5" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="AC5" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="AD5" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="AE5" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="AF5" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="AG5" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="AH5" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="AI5" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="AJ5" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="AK5" s="11" t="s">
+        <v>249</v>
+      </c>
+      <c r="AL5" s="11" t="s">
+        <v>250</v>
+      </c>
+      <c r="AM5" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="AN5" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="AO5" s="11" t="s">
+        <v>252</v>
+      </c>
+      <c r="AP5" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="AQ5" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="AR5" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="AS5" s="11" t="s">
+        <v>253</v>
+      </c>
+      <c r="AT5" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="AU5" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="AV5" s="11" t="s">
+        <v>254</v>
+      </c>
+      <c r="AW5" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="AX5" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="AY5" s="11" t="s">
+        <v>255</v>
+      </c>
+      <c r="AZ5" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="BA5" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="BB5" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="BC5" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="BD5" s="11" t="s">
         <v>224</v>
       </c>
-      <c r="C5" s="11" t="s">
-        <v>224</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>224</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>242</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>243</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>224</v>
-      </c>
-      <c r="H5" s="11" t="s">
+      <c r="BE5" s="11" t="s">
+        <v>256</v>
+      </c>
+      <c r="BF5" s="11" t="s">
         <v>223</v>
-      </c>
-      <c r="I5" s="11" t="s">
-        <v>244</v>
-      </c>
-      <c r="J5" s="11" t="s">
-        <v>245</v>
-      </c>
-      <c r="K5" s="11" t="s">
-        <v>224</v>
-      </c>
-      <c r="L5" s="11" t="s">
-        <v>224</v>
-      </c>
-      <c r="M5" s="11" t="s">
-        <v>224</v>
-      </c>
-      <c r="N5" s="11" t="s">
-        <v>224</v>
-      </c>
-      <c r="O5" s="11" t="s">
-        <v>246</v>
-      </c>
-      <c r="P5" s="11" t="s">
-        <v>223</v>
-      </c>
-      <c r="Q5" s="11" t="s">
-        <v>224</v>
-      </c>
-      <c r="R5" s="11" t="s">
-        <v>223</v>
-      </c>
-      <c r="S5" s="11" t="s">
-        <v>247</v>
-      </c>
-      <c r="T5" s="11" t="s">
-        <v>248</v>
-      </c>
-      <c r="U5" s="11" t="s">
-        <v>224</v>
-      </c>
-      <c r="V5" s="11" t="s">
-        <v>224</v>
-      </c>
-      <c r="W5" s="11" t="s">
-        <v>224</v>
-      </c>
-      <c r="X5" s="11" t="s">
-        <v>224</v>
-      </c>
-      <c r="Y5" s="11" t="s">
-        <v>249</v>
-      </c>
-      <c r="Z5" s="11" t="s">
-        <v>224</v>
-      </c>
-      <c r="AA5" s="11" t="s">
-        <v>223</v>
-      </c>
-      <c r="AB5" s="11" t="s">
-        <v>224</v>
-      </c>
-      <c r="AC5" s="11" t="s">
-        <v>224</v>
-      </c>
-      <c r="AD5" s="11" t="s">
-        <v>224</v>
-      </c>
-      <c r="AE5" s="11" t="s">
-        <v>224</v>
-      </c>
-      <c r="AF5" s="11" t="s">
-        <v>223</v>
-      </c>
-      <c r="AG5" s="11" t="s">
-        <v>224</v>
-      </c>
-      <c r="AH5" s="11" t="s">
-        <v>223</v>
-      </c>
-      <c r="AI5" s="11" t="s">
-        <v>224</v>
-      </c>
-      <c r="AJ5" s="11" t="s">
-        <v>224</v>
-      </c>
-      <c r="AK5" s="11" t="s">
-        <v>250</v>
-      </c>
-      <c r="AL5" s="11" t="s">
-        <v>251</v>
-      </c>
-      <c r="AM5" s="11" t="s">
-        <v>223</v>
-      </c>
-      <c r="AN5" s="11" t="s">
-        <v>252</v>
-      </c>
-      <c r="AO5" s="11" t="s">
-        <v>253</v>
-      </c>
-      <c r="AP5" s="11" t="s">
-        <v>224</v>
-      </c>
-      <c r="AQ5" s="11" t="s">
-        <v>224</v>
-      </c>
-      <c r="AR5" s="11" t="s">
-        <v>224</v>
-      </c>
-      <c r="AS5" s="11" t="s">
-        <v>254</v>
-      </c>
-      <c r="AT5" s="11" t="s">
-        <v>224</v>
-      </c>
-      <c r="AU5" s="11" t="s">
-        <v>224</v>
-      </c>
-      <c r="AV5" s="11" t="s">
-        <v>255</v>
-      </c>
-      <c r="AW5" s="11" t="s">
-        <v>224</v>
-      </c>
-      <c r="AX5" s="11" t="s">
-        <v>223</v>
-      </c>
-      <c r="AY5" s="11" t="s">
-        <v>256</v>
-      </c>
-      <c r="AZ5" s="11" t="s">
-        <v>223</v>
-      </c>
-      <c r="BA5" s="11" t="s">
-        <v>223</v>
-      </c>
-      <c r="BB5" s="11" t="s">
-        <v>224</v>
-      </c>
-      <c r="BC5" s="11" t="s">
-        <v>223</v>
-      </c>
-      <c r="BD5" s="11" t="s">
-        <v>225</v>
-      </c>
-      <c r="BE5" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="BF5" s="11" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="6" spans="1:58" ht="68.45" customHeight="1">
@@ -9140,11 +9331,11 @@
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
       <c r="H6" s="8" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="I6" s="8"/>
       <c r="J6" s="8" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="K6" s="9"/>
       <c r="L6" s="9"/>
@@ -9152,11 +9343,11 @@
       <c r="N6" s="9"/>
       <c r="O6" s="9"/>
       <c r="P6" s="8" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="Q6" s="9"/>
       <c r="R6" s="8" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="S6" s="9"/>
       <c r="T6" s="9"/>
@@ -9167,25 +9358,25 @@
       <c r="Y6" s="9"/>
       <c r="Z6" s="9"/>
       <c r="AA6" s="8" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="AB6" s="12"/>
       <c r="AC6" s="9"/>
       <c r="AD6" s="9"/>
       <c r="AE6" s="9"/>
       <c r="AF6" s="8" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="AG6" s="8"/>
       <c r="AH6" s="8" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="AI6" s="9"/>
       <c r="AJ6" s="8"/>
       <c r="AK6" s="9"/>
       <c r="AL6" s="8"/>
       <c r="AM6" s="8" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="AN6" s="9"/>
       <c r="AO6" s="9"/>
@@ -9198,26 +9389,26 @@
       <c r="AV6" s="12"/>
       <c r="AW6" s="9"/>
       <c r="AX6" s="8" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="AY6" s="9"/>
       <c r="AZ6" s="8" t="s">
+        <v>265</v>
+      </c>
+      <c r="BA6" s="8" t="s">
         <v>266</v>
-      </c>
-      <c r="BA6" s="8" t="s">
-        <v>267</v>
       </c>
       <c r="BB6" s="9"/>
       <c r="BC6" s="8" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="BD6" s="8" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="BE6" s="9"/>
       <c r="BF6" s="9"/>
     </row>
-    <row r="7" spans="1:58" ht="20.45" customHeight="1">
+    <row r="7" spans="1:58" ht="20.5" customHeight="1">
       <c r="A7" s="6"/>
       <c r="B7" s="13"/>
       <c r="C7" s="14"/>
@@ -9277,7 +9468,7 @@
       <c r="BE7" s="14"/>
       <c r="BF7" s="14"/>
     </row>
-    <row r="8" spans="1:58" ht="20.45" customHeight="1">
+    <row r="8" spans="1:58" ht="20.5" customHeight="1">
       <c r="A8" s="6"/>
       <c r="B8" s="15"/>
       <c r="C8" s="16"/>
@@ -9337,7 +9528,7 @@
       <c r="BE8" s="16"/>
       <c r="BF8" s="16"/>
     </row>
-    <row r="9" spans="1:58" ht="20.45" customHeight="1">
+    <row r="9" spans="1:58" ht="20.5" customHeight="1">
       <c r="A9" s="6"/>
       <c r="B9" s="13"/>
       <c r="C9" s="14"/>
@@ -9397,7 +9588,7 @@
       <c r="BE9" s="14"/>
       <c r="BF9" s="14"/>
     </row>
-    <row r="10" spans="1:58" ht="20.45" customHeight="1">
+    <row r="10" spans="1:58" ht="20.5" customHeight="1">
       <c r="A10" s="6"/>
       <c r="B10" s="15"/>
       <c r="C10" s="16"/>
@@ -9457,7 +9648,7 @@
       <c r="BE10" s="16"/>
       <c r="BF10" s="16"/>
     </row>
-    <row r="11" spans="1:58" ht="20.45" customHeight="1">
+    <row r="11" spans="1:58" ht="20.5" customHeight="1">
       <c r="A11" s="6"/>
       <c r="B11" s="13"/>
       <c r="C11" s="14"/>
@@ -9517,7 +9708,7 @@
       <c r="BE11" s="14"/>
       <c r="BF11" s="14"/>
     </row>
-    <row r="12" spans="1:58" ht="20.45" customHeight="1">
+    <row r="12" spans="1:58" ht="20.5" customHeight="1">
       <c r="A12" s="6"/>
       <c r="B12" s="15"/>
       <c r="C12" s="16"/>
@@ -9577,7 +9768,7 @@
       <c r="BE12" s="16"/>
       <c r="BF12" s="16"/>
     </row>
-    <row r="13" spans="1:58" ht="20.45" customHeight="1">
+    <row r="13" spans="1:58" ht="20.5" customHeight="1">
       <c r="A13" s="6"/>
       <c r="B13" s="13"/>
       <c r="C13" s="14"/>
@@ -9637,7 +9828,7 @@
       <c r="BE13" s="14"/>
       <c r="BF13" s="14"/>
     </row>
-    <row r="14" spans="1:58" ht="20.45" customHeight="1">
+    <row r="14" spans="1:58" ht="20.5" customHeight="1">
       <c r="A14" s="6"/>
       <c r="B14" s="15"/>
       <c r="C14" s="16"/>
@@ -9697,7 +9888,7 @@
       <c r="BE14" s="16"/>
       <c r="BF14" s="16"/>
     </row>
-    <row r="15" spans="1:58" ht="20.45" customHeight="1">
+    <row r="15" spans="1:58" ht="20.5" customHeight="1">
       <c r="A15" s="6"/>
       <c r="B15" s="13"/>
       <c r="C15" s="14"/>
@@ -9757,7 +9948,7 @@
       <c r="BE15" s="14"/>
       <c r="BF15" s="14"/>
     </row>
-    <row r="16" spans="1:58" ht="20.45" customHeight="1">
+    <row r="16" spans="1:58" ht="20.5" customHeight="1">
       <c r="A16" s="6"/>
       <c r="B16" s="15"/>
       <c r="C16" s="16"/>
@@ -9817,7 +10008,7 @@
       <c r="BE16" s="16"/>
       <c r="BF16" s="16"/>
     </row>
-    <row r="17" spans="1:58" ht="20.45" customHeight="1">
+    <row r="17" spans="1:58" ht="20.5" customHeight="1">
       <c r="A17" s="6"/>
       <c r="B17" s="13"/>
       <c r="C17" s="14"/>
@@ -9877,7 +10068,7 @@
       <c r="BE17" s="14"/>
       <c r="BF17" s="14"/>
     </row>
-    <row r="18" spans="1:58" ht="20.45" customHeight="1">
+    <row r="18" spans="1:58" ht="20.5" customHeight="1">
       <c r="A18" s="6"/>
       <c r="B18" s="15"/>
       <c r="C18" s="16"/>
@@ -9937,7 +10128,7 @@
       <c r="BE18" s="16"/>
       <c r="BF18" s="16"/>
     </row>
-    <row r="19" spans="1:58" ht="20.45" customHeight="1">
+    <row r="19" spans="1:58" ht="20.5" customHeight="1">
       <c r="A19" s="6"/>
       <c r="B19" s="13"/>
       <c r="C19" s="14"/>
@@ -9997,7 +10188,7 @@
       <c r="BE19" s="14"/>
       <c r="BF19" s="14"/>
     </row>
-    <row r="20" spans="1:58" ht="20.45" customHeight="1">
+    <row r="20" spans="1:58" ht="20.5" customHeight="1">
       <c r="A20" s="6"/>
       <c r="B20" s="15"/>
       <c r="C20" s="16"/>
@@ -10057,7 +10248,7 @@
       <c r="BE20" s="16"/>
       <c r="BF20" s="16"/>
     </row>
-    <row r="21" spans="1:58" ht="20.45" customHeight="1">
+    <row r="21" spans="1:58" ht="20.5" customHeight="1">
       <c r="A21" s="6"/>
       <c r="B21" s="13"/>
       <c r="C21" s="14"/>
@@ -10117,7 +10308,7 @@
       <c r="BE21" s="14"/>
       <c r="BF21" s="14"/>
     </row>
-    <row r="22" spans="1:58" ht="20.45" customHeight="1">
+    <row r="22" spans="1:58" ht="20.5" customHeight="1">
       <c r="A22" s="6"/>
       <c r="B22" s="15"/>
       <c r="C22" s="16"/>
@@ -10177,7 +10368,7 @@
       <c r="BE22" s="16"/>
       <c r="BF22" s="16"/>
     </row>
-    <row r="23" spans="1:58" ht="20.45" customHeight="1">
+    <row r="23" spans="1:58" ht="20.5" customHeight="1">
       <c r="A23" s="17"/>
       <c r="B23" s="13"/>
       <c r="C23" s="14"/>

</xml_diff>

<commit_message>
DOC: reorganizes files in sub-folders.
</commit_message>
<xml_diff>
--- a/docs/conversion-matrix.xlsx
+++ b/docs/conversion-matrix.xlsx
@@ -4,18 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr date1904="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27602" windowHeight="13844" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27600" windowHeight="13840" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="R3 TO matrix" sheetId="1" r:id="rId1"/>
     <sheet name="R3 MAKE matrix" sheetId="2" r:id="rId2"/>
     <sheet name="Red TO matrix" sheetId="3" r:id="rId3"/>
     <sheet name="Red MAKE matrix" sheetId="4" r:id="rId4"/>
-    <sheet name="Sheet 1 - Red Datatype Comparis" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet 1 - Red Datatype Comparis" sheetId="5" state="hidden" r:id="rId5"/>
   </sheets>
   <calcPr calcId="144525"/>
   <customWorkbookViews>
-    <customWorkbookView name="dk - Personal View" guid="{6590DA0F-755E-492A-8B86-272A49DB945C}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="1043" activeSheetId="3"/>
+    <customWorkbookView name="dk - Personal View" guid="{6590DA0F-755E-492A-8B86-272A49DB945C}" mergeInterval="0" personalView="1" maximized="1" windowWidth="3836" windowHeight="1924" activeSheetId="4"/>
   </customWorkbookViews>
 </workbook>
 </file>
@@ -2936,7 +2936,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{264BB4E1-8C21-465A-8536-3EE0FB803C4B}" diskRevisions="1" revisionId="53" version="16">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{BB4C0838-225F-4D9E-9602-155C6C49421D}" diskRevisions="1" revisionId="53" version="17">
   <header guid="{EB7A1191-CBBA-4B45-A8AB-97C58606F627}" dateTime="2016-11-18T10:22:06" maxSheetId="6" userName="qtxie" r:id="rId8" minRId="22" maxRId="24">
     <sheetIdMap count="5">
       <sheetId val="1"/>
@@ -3010,6 +3010,15 @@
     </sheetIdMap>
   </header>
   <header guid="{264BB4E1-8C21-465A-8536-3EE0FB803C4B}" dateTime="2017-07-30T12:42:35" maxSheetId="6" userName="dk" r:id="rId16" minRId="41" maxRId="53">
+    <sheetIdMap count="5">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{BB4C0838-225F-4D9E-9602-155C6C49421D}" dateTime="2019-10-03T21:22:28" maxSheetId="6" userName="dk" r:id="rId17">
     <sheetIdMap count="5">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -3406,6 +3415,13 @@
       </is>
     </nc>
   </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog7.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcv guid="{6590DA0F-755E-492A-8B86-272A49DB945C}" action="delete"/>
+  <rcv guid="{6590DA0F-755E-492A-8B86-272A49DB945C}" action="add"/>
 </revisions>
 </file>
 
@@ -4576,19 +4592,19 @@
       <selection activeCell="Q15" sqref="Q15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.85"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="9.375" customWidth="1"/>
-    <col min="2" max="2" width="13.375" customWidth="1"/>
-    <col min="3" max="13" width="11.875" style="18" customWidth="1"/>
-    <col min="14" max="14" width="13.875" style="18" customWidth="1"/>
+    <col min="1" max="1" width="9.36328125" customWidth="1"/>
+    <col min="2" max="2" width="13.36328125" customWidth="1"/>
+    <col min="3" max="13" width="11.90625" style="18" customWidth="1"/>
+    <col min="14" max="14" width="13.90625" style="18" customWidth="1"/>
     <col min="15" max="15" width="14" style="18" customWidth="1"/>
-    <col min="16" max="16" width="13.75" style="18" customWidth="1"/>
-    <col min="17" max="18" width="11.875" style="18" customWidth="1"/>
-    <col min="19" max="22" width="13.25" style="18" customWidth="1"/>
+    <col min="16" max="16" width="13.7265625" style="18" customWidth="1"/>
+    <col min="17" max="18" width="11.90625" style="18" customWidth="1"/>
+    <col min="19" max="22" width="13.26953125" style="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:25" ht="41.2" customHeight="1">
+    <row r="3" spans="2:25" ht="41.25" customHeight="1">
       <c r="B3" s="19" t="s">
         <v>0</v>
       </c>
@@ -5495,19 +5511,19 @@
       <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.85"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="9.375" customWidth="1"/>
-    <col min="2" max="2" width="13.375" customWidth="1"/>
-    <col min="3" max="13" width="11.875" style="18" customWidth="1"/>
+    <col min="1" max="1" width="9.36328125" customWidth="1"/>
+    <col min="2" max="2" width="13.36328125" customWidth="1"/>
+    <col min="3" max="13" width="11.90625" style="18" customWidth="1"/>
     <col min="14" max="15" width="14" style="18" customWidth="1"/>
-    <col min="16" max="16" width="13.75" style="18" customWidth="1"/>
-    <col min="17" max="17" width="13.25" style="18" customWidth="1"/>
-    <col min="18" max="18" width="13.75" style="18" customWidth="1"/>
-    <col min="19" max="22" width="13.25" style="18" customWidth="1"/>
+    <col min="16" max="16" width="13.7265625" style="18" customWidth="1"/>
+    <col min="17" max="17" width="13.26953125" style="18" customWidth="1"/>
+    <col min="18" max="18" width="13.7265625" style="18" customWidth="1"/>
+    <col min="19" max="22" width="13.26953125" style="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:25" ht="41.2" customHeight="1">
+    <row r="3" spans="2:25" ht="41.25" customHeight="1">
       <c r="B3" s="19" t="s">
         <v>0</v>
       </c>
@@ -6385,25 +6401,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:AB26"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="S17" sqref="S17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.85"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="9.375" customWidth="1"/>
-    <col min="2" max="2" width="13.375" customWidth="1"/>
-    <col min="3" max="12" width="11.875" style="18" customWidth="1"/>
-    <col min="13" max="13" width="12.125" style="18" customWidth="1"/>
-    <col min="14" max="14" width="13.875" style="18" customWidth="1"/>
+    <col min="1" max="1" width="9.36328125" customWidth="1"/>
+    <col min="2" max="2" width="13.36328125" customWidth="1"/>
+    <col min="3" max="12" width="11.90625" style="18" customWidth="1"/>
+    <col min="13" max="13" width="12.08984375" style="18" customWidth="1"/>
+    <col min="14" max="14" width="13.90625" style="18" customWidth="1"/>
     <col min="15" max="15" width="14" style="18" customWidth="1"/>
-    <col min="16" max="16" width="13.75" style="18" customWidth="1"/>
-    <col min="17" max="18" width="11.875" style="18" customWidth="1"/>
-    <col min="19" max="25" width="13.25" style="18" customWidth="1"/>
-    <col min="28" max="28" width="11.75" customWidth="1"/>
+    <col min="16" max="16" width="13.7265625" style="18" customWidth="1"/>
+    <col min="17" max="18" width="11.90625" style="18" customWidth="1"/>
+    <col min="19" max="25" width="13.26953125" style="18" customWidth="1"/>
+    <col min="28" max="28" width="11.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:28" ht="41.2" customHeight="1">
+    <row r="3" spans="2:28" ht="41.25" customHeight="1">
       <c r="B3" s="19" t="s">
         <v>0</v>
       </c>
@@ -7497,7 +7513,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{6590DA0F-755E-492A-8B86-272A49DB945C}" scale="70">
+    <customSheetView guid="{6590DA0F-755E-492A-8B86-272A49DB945C}" scale="85">
       <selection activeCell="S17" sqref="S17"/>
       <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
@@ -7513,27 +7529,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:AB26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="V5" sqref="V5"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R15" sqref="R15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.85"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="9.375" customWidth="1"/>
-    <col min="2" max="2" width="13.375" customWidth="1"/>
-    <col min="3" max="13" width="11.875" style="18" customWidth="1"/>
+    <col min="1" max="1" width="9.36328125" customWidth="1"/>
+    <col min="2" max="2" width="13.36328125" customWidth="1"/>
+    <col min="3" max="13" width="11.90625" style="18" customWidth="1"/>
     <col min="14" max="15" width="14" style="18" customWidth="1"/>
-    <col min="16" max="16" width="13.75" style="18" customWidth="1"/>
-    <col min="17" max="17" width="13.875" style="18" customWidth="1"/>
-    <col min="18" max="18" width="13.75" style="18" customWidth="1"/>
-    <col min="19" max="20" width="13.25" style="18" customWidth="1"/>
-    <col min="21" max="21" width="14.75" style="18" customWidth="1"/>
-    <col min="22" max="22" width="14.25" style="18" customWidth="1"/>
-    <col min="23" max="25" width="13.25" style="18" customWidth="1"/>
+    <col min="16" max="16" width="13.7265625" style="18" customWidth="1"/>
+    <col min="17" max="17" width="13.90625" style="18" customWidth="1"/>
+    <col min="18" max="18" width="13.7265625" style="18" customWidth="1"/>
+    <col min="19" max="20" width="13.26953125" style="18" customWidth="1"/>
+    <col min="21" max="21" width="14.7265625" style="18" customWidth="1"/>
+    <col min="22" max="22" width="14.26953125" style="18" customWidth="1"/>
+    <col min="23" max="25" width="13.26953125" style="18" customWidth="1"/>
     <col min="28" max="28" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:28" ht="41.2" customHeight="1">
+    <row r="3" spans="2:28" ht="41.25" customHeight="1">
       <c r="B3" s="19" t="s">
         <v>0</v>
       </c>
@@ -8603,7 +8619,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{6590DA0F-755E-492A-8B86-272A49DB945C}" scale="70">
+    <customSheetView guid="{6590DA0F-755E-492A-8B86-272A49DB945C}" scale="85">
       <selection activeCell="R15" sqref="R15"/>
       <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
@@ -8629,9 +8645,9 @@
       <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.25" defaultRowHeight="18" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="16.26953125" defaultRowHeight="18" customHeight="1"/>
   <cols>
-    <col min="1" max="256" width="16.25" style="1" customWidth="1"/>
+    <col min="1" max="256" width="16.26953125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:58" ht="28" customHeight="1">
@@ -8696,7 +8712,7 @@
       <c r="BE1" s="33"/>
       <c r="BF1" s="33"/>
     </row>
-    <row r="2" spans="1:58" ht="20.7" customHeight="1">
+    <row r="2" spans="1:58" ht="20.75" customHeight="1">
       <c r="A2" s="2"/>
       <c r="B2" s="3" t="s">
         <v>183</v>
@@ -9146,7 +9162,7 @@
       <c r="BE4" s="9"/>
       <c r="BF4" s="9"/>
     </row>
-    <row r="5" spans="1:58" ht="68.45" customHeight="1">
+    <row r="5" spans="1:58" ht="68.5" customHeight="1">
       <c r="A5" s="36" t="s">
         <v>1</v>
       </c>
@@ -9322,7 +9338,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="6" spans="1:58" ht="68.45" customHeight="1">
+    <row r="6" spans="1:58" ht="68.5" customHeight="1">
       <c r="A6" s="35"/>
       <c r="B6" s="7"/>
       <c r="C6" s="12"/>
@@ -10430,7 +10446,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{6590DA0F-755E-492A-8B86-272A49DB945C}" showGridLines="0" fitToPage="1">
+    <customSheetView guid="{6590DA0F-755E-492A-8B86-272A49DB945C}" showGridLines="0" fitToPage="1" state="hidden">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
       <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.27777777777777801" footer="0.27777777777777801"/>

</xml_diff>